<commit_message>
Atualiza Caixa 25 com roupas do Bento
- 7 itens de vestuário infantil
- Prioridade Alta
- Total: 437 itens no catálogo
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F437"/>
+  <dimension ref="A1:F438"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6201,12 +6201,12 @@
       </c>
       <c r="B196" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C196" s="2" t="inlineStr">
         <is>
-          <t>Pijamas</t>
+          <t>Roupas diversas do Bento (lavadas recentemente)</t>
         </is>
       </c>
       <c r="D196" s="2" t="inlineStr">
@@ -6219,11 +6219,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F196" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F196" s="2" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" s="2" t="inlineStr">
@@ -6233,12 +6229,12 @@
       </c>
       <c r="B197" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C197" s="2" t="inlineStr">
         <is>
-          <t>Cuecas</t>
+          <t>Moletons</t>
         </is>
       </c>
       <c r="D197" s="2" t="inlineStr">
@@ -6251,11 +6247,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F197" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F197" s="2" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" s="2" t="inlineStr">
@@ -6265,12 +6257,12 @@
       </c>
       <c r="B198" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C198" s="2" t="inlineStr">
         <is>
-          <t>Meias</t>
+          <t>Roupas de piscina</t>
         </is>
       </c>
       <c r="D198" s="2" t="inlineStr">
@@ -6283,11 +6275,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F198" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F198" s="2" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" s="2" t="inlineStr">
@@ -6297,12 +6285,12 @@
       </c>
       <c r="B199" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C199" s="2" t="inlineStr">
         <is>
-          <t>Bermudas</t>
+          <t>Bonés</t>
         </is>
       </c>
       <c r="D199" s="2" t="inlineStr">
@@ -6315,11 +6303,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F199" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F199" s="2" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" s="2" t="inlineStr">
@@ -6329,12 +6313,12 @@
       </c>
       <c r="B200" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C200" s="2" t="inlineStr">
         <is>
-          <t>Camisetas</t>
+          <t>Pijamas</t>
         </is>
       </c>
       <c r="D200" s="2" t="inlineStr">
@@ -6347,11 +6331,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F200" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F200" s="2" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" s="2" t="inlineStr">
@@ -6361,12 +6341,12 @@
       </c>
       <c r="B201" s="2" t="inlineStr">
         <is>
-          <t>Roupas - Uso diário</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C201" s="2" t="inlineStr">
         <is>
-          <t>Moletom</t>
+          <t>Camisetas</t>
         </is>
       </c>
       <c r="D201" s="2" t="inlineStr">
@@ -6379,26 +6359,22 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F201" s="2" t="inlineStr">
-        <is>
-          <t>Prioridade alta de abertura; separar para acesso imediato nos primeiros dias</t>
-        </is>
-      </c>
+      <c r="F201" s="2" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>Caixa 27</t>
+          <t>Caixa 25</t>
         </is>
       </c>
       <c r="B202" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Atividades</t>
+          <t>Vestuário infantil</t>
         </is>
       </c>
       <c r="C202" s="2" t="inlineStr">
         <is>
-          <t>Jogo Puxa-Batatinha</t>
+          <t>Roupas esportivas</t>
         </is>
       </c>
       <c r="D202" s="2" t="inlineStr">
@@ -6406,16 +6382,12 @@
           <t>Quarto do Bento</t>
         </is>
       </c>
-      <c r="E202" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F202" s="2" t="inlineStr">
-        <is>
-          <t>Caixa em andamento; jogos de tabuleiro e atividades</t>
-        </is>
-      </c>
+      <c r="E202" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F202" s="2" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" s="2" t="inlineStr">
@@ -6430,7 +6402,7 @@
       </c>
       <c r="C203" s="2" t="inlineStr">
         <is>
-          <t>Jogo de mímicas</t>
+          <t>Jogo Puxa-Batatinha</t>
         </is>
       </c>
       <c r="D203" s="2" t="inlineStr">
@@ -6462,7 +6434,7 @@
       </c>
       <c r="C204" s="2" t="inlineStr">
         <is>
-          <t>Pula-Macaco</t>
+          <t>Jogo de mímicas</t>
         </is>
       </c>
       <c r="D204" s="2" t="inlineStr">
@@ -6494,7 +6466,7 @@
       </c>
       <c r="C205" s="2" t="inlineStr">
         <is>
-          <t>Cilada</t>
+          <t>Pula-Macaco</t>
         </is>
       </c>
       <c r="D205" s="2" t="inlineStr">
@@ -6526,7 +6498,7 @@
       </c>
       <c r="C206" s="2" t="inlineStr">
         <is>
-          <t>É Lógico</t>
+          <t>Cilada</t>
         </is>
       </c>
       <c r="D206" s="2" t="inlineStr">
@@ -6558,7 +6530,7 @@
       </c>
       <c r="C207" s="2" t="inlineStr">
         <is>
-          <t>Super Banco Imobiliário</t>
+          <t>É Lógico</t>
         </is>
       </c>
       <c r="D207" s="2" t="inlineStr">
@@ -6580,7 +6552,7 @@
     <row r="208">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>Caixa 28</t>
+          <t>Caixa 27</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -6590,7 +6562,7 @@
       </c>
       <c r="C208" s="2" t="inlineStr">
         <is>
-          <t>Jogo da Duca</t>
+          <t>Super Banco Imobiliário</t>
         </is>
       </c>
       <c r="D208" s="2" t="inlineStr">
@@ -6605,7 +6577,7 @@
       </c>
       <c r="F208" s="2" t="inlineStr">
         <is>
-          <t>Caixa em andamento; jogos, atividades e acessório de banho</t>
+          <t>Caixa em andamento; jogos de tabuleiro e atividades</t>
         </is>
       </c>
     </row>
@@ -6622,7 +6594,7 @@
       </c>
       <c r="C209" s="2" t="inlineStr">
         <is>
-          <t>Cara a Cara</t>
+          <t>Jogo da Duca</t>
         </is>
       </c>
       <c r="D209" s="2" t="inlineStr">
@@ -6654,7 +6626,7 @@
       </c>
       <c r="C210" s="2" t="inlineStr">
         <is>
-          <t>Verdade ou Desafio</t>
+          <t>Cara a Cara</t>
         </is>
       </c>
       <c r="D210" s="2" t="inlineStr">
@@ -6686,7 +6658,7 @@
       </c>
       <c r="C211" s="2" t="inlineStr">
         <is>
-          <t>Kit de mágica</t>
+          <t>Verdade ou Desafio</t>
         </is>
       </c>
       <c r="D211" s="2" t="inlineStr">
@@ -6718,7 +6690,7 @@
       </c>
       <c r="C212" s="2" t="inlineStr">
         <is>
-          <t>Imagem &amp; Ação Júnior</t>
+          <t>Kit de mágica</t>
         </is>
       </c>
       <c r="D212" s="2" t="inlineStr">
@@ -6750,7 +6722,7 @@
       </c>
       <c r="C213" s="2" t="inlineStr">
         <is>
-          <t>Kit de bordado do sistema solar</t>
+          <t>Imagem &amp; Ação Júnior</t>
         </is>
       </c>
       <c r="D213" s="2" t="inlineStr">
@@ -6777,12 +6749,12 @@
       </c>
       <c r="B214" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de banho</t>
+          <t>Jogos e Atividades</t>
         </is>
       </c>
       <c r="C214" s="2" t="inlineStr">
         <is>
-          <t>Mangueira da banheira</t>
+          <t>Kit de bordado do sistema solar</t>
         </is>
       </c>
       <c r="D214" s="2" t="inlineStr">
@@ -6804,17 +6776,17 @@
     <row r="215">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29</t>
+          <t>Caixa 28</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
         <is>
-          <t>Calçados</t>
+          <t>Acessórios de banho</t>
         </is>
       </c>
       <c r="C215" s="2" t="inlineStr">
         <is>
-          <t>Tênis do Bento</t>
+          <t>Mangueira da banheira</t>
         </is>
       </c>
       <c r="D215" s="2" t="inlineStr">
@@ -6822,31 +6794,31 @@
           <t>Quarto do Bento</t>
         </is>
       </c>
-      <c r="E215" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+      <c r="E215" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F215" s="2" t="inlineStr">
         <is>
-          <t>Prioridade alta de abertura; organizar próximo ao guarda-roupa</t>
+          <t>Caixa em andamento; jogos, atividades e acessório de banho</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>Caixa 30</t>
+          <t>Caixa 29</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
         <is>
-          <t>Jogos de Cartas</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>Jogos de cartas variados</t>
+          <t>Tênis do Bento</t>
         </is>
       </c>
       <c r="D216" s="2" t="inlineStr">
@@ -6854,31 +6826,31 @@
           <t>Quarto do Bento</t>
         </is>
       </c>
-      <c r="E216" s="6" t="inlineStr">
-        <is>
-          <t>Baixa</t>
+      <c r="E216" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F216" s="2" t="inlineStr">
         <is>
-          <t>Pode abrir após organização inicial; manter agrupados</t>
+          <t>Prioridade alta de abertura; organizar próximo ao guarda-roupa</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>Caixa 31</t>
+          <t>Caixa 30</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Jogos de Cartas</t>
         </is>
       </c>
       <c r="C217" s="2" t="inlineStr">
         <is>
-          <t>Organizadores acrílicos e itens de organização diversos</t>
+          <t>Jogos de cartas variados</t>
         </is>
       </c>
       <c r="D217" s="2" t="inlineStr">
@@ -6886,36 +6858,36 @@
           <t>Quarto do Bento</t>
         </is>
       </c>
-      <c r="E217" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+      <c r="E217" s="6" t="inlineStr">
+        <is>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="F217" s="2" t="inlineStr">
         <is>
-          <t>Abrir durante a organização dos armários e prateleiras</t>
+          <t>Pode abrir após organização inicial; manter agrupados</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>Caixa 32</t>
+          <t>Caixa 31</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C218" s="2" t="inlineStr">
         <is>
-          <t>Big Nate Arrasou</t>
+          <t>Organizadores acrílicos e itens de organização diversos</t>
         </is>
       </c>
       <c r="D218" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E218" s="7" t="inlineStr">
@@ -6925,7 +6897,7 @@
       </c>
       <c r="F218" s="2" t="inlineStr">
         <is>
-          <t>Livros e itens de memória</t>
+          <t>Abrir durante a organização dos armários e prateleiras</t>
         </is>
       </c>
     </row>
@@ -6942,7 +6914,7 @@
       </c>
       <c r="C219" s="2" t="inlineStr">
         <is>
-          <t>Cozinha Só para Um (Rita Lobo)</t>
+          <t>Big Nate Arrasou</t>
         </is>
       </c>
       <c r="D219" s="2" t="inlineStr">
@@ -6974,7 +6946,7 @@
       </c>
       <c r="C220" s="2" t="inlineStr">
         <is>
-          <t>Todas as Cestas (Paola Carosella)</t>
+          <t>Cozinha Só para Um (Rita Lobo)</t>
         </is>
       </c>
       <c r="D220" s="2" t="inlineStr">
@@ -7006,7 +6978,7 @@
       </c>
       <c r="C221" s="2" t="inlineStr">
         <is>
-          <t>Mocotó: O Pai e o Filho Restaurante</t>
+          <t>Todas as Cestas (Paola Carosella)</t>
         </is>
       </c>
       <c r="D221" s="2" t="inlineStr">
@@ -7038,7 +7010,7 @@
       </c>
       <c r="C222" s="2" t="inlineStr">
         <is>
-          <t>Cozinha Prática (Rita Lobo)</t>
+          <t>Mocotó: O Pai e o Filho Restaurante</t>
         </is>
       </c>
       <c r="D222" s="2" t="inlineStr">
@@ -7070,7 +7042,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>Cozinha Quatro Mãos (Rita Lobo)</t>
+          <t>Cozinha Prática (Rita Lobo)</t>
         </is>
       </c>
       <c r="D223" s="2" t="inlineStr">
@@ -7102,7 +7074,7 @@
       </c>
       <c r="C224" s="2" t="inlineStr">
         <is>
-          <t>Panelinha: Receitas que Funcionam (Rita Lobo)</t>
+          <t>Cozinha Quatro Mãos (Rita Lobo)</t>
         </is>
       </c>
       <c r="D224" s="2" t="inlineStr">
@@ -7134,7 +7106,7 @@
       </c>
       <c r="C225" s="2" t="inlineStr">
         <is>
-          <t>Jujutsu Kaisen – Vol. 2</t>
+          <t>Panelinha: Receitas que Funcionam (Rita Lobo)</t>
         </is>
       </c>
       <c r="D225" s="2" t="inlineStr">
@@ -7166,7 +7138,7 @@
       </c>
       <c r="C226" s="2" t="inlineStr">
         <is>
-          <t>Um Garoto Chamado Roberto (Gabriel Pensador)</t>
+          <t>Jujutsu Kaisen – Vol. 2</t>
         </is>
       </c>
       <c r="D226" s="2" t="inlineStr">
@@ -7193,12 +7165,12 @@
       </c>
       <c r="B227" s="2" t="inlineStr">
         <is>
-          <t>Memória esportiva</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C227" s="2" t="inlineStr">
         <is>
-          <t>Porta-retrato com medalha meia maratona New Balance</t>
+          <t>Um Garoto Chamado Roberto (Gabriel Pensador)</t>
         </is>
       </c>
       <c r="D227" s="2" t="inlineStr">
@@ -7230,7 +7202,7 @@
       </c>
       <c r="C228" s="2" t="inlineStr">
         <is>
-          <t>Medalha meia maratona de Porto Alegre</t>
+          <t>Porta-retrato com medalha meia maratona New Balance</t>
         </is>
       </c>
       <c r="D228" s="2" t="inlineStr">
@@ -7257,12 +7229,12 @@
       </c>
       <c r="B229" s="2" t="inlineStr">
         <is>
-          <t>Fotografia</t>
+          <t>Memória esportiva</t>
         </is>
       </c>
       <c r="C229" s="2" t="inlineStr">
         <is>
-          <t>Álbum de fotos Instax</t>
+          <t>Medalha meia maratona de Porto Alegre</t>
         </is>
       </c>
       <c r="D229" s="2" t="inlineStr">
@@ -7294,7 +7266,7 @@
       </c>
       <c r="C230" s="2" t="inlineStr">
         <is>
-          <t>Álbum de fotografias recentes</t>
+          <t>Álbum de fotos Instax</t>
         </is>
       </c>
       <c r="D230" s="2" t="inlineStr">
@@ -7321,12 +7293,12 @@
       </c>
       <c r="B231" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Fotografia</t>
         </is>
       </c>
       <c r="C231" s="2" t="inlineStr">
         <is>
-          <t>MacBook Pro do Bento</t>
+          <t>Álbum de fotografias recentes</t>
         </is>
       </c>
       <c r="D231" s="2" t="inlineStr">
@@ -7334,14 +7306,14 @@
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E231" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+      <c r="E231" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F231" s="2" t="inlineStr">
         <is>
-          <t>Livros e itens de memória; CUIDADO - eletrônico valioso</t>
+          <t>Livros e itens de memória</t>
         </is>
       </c>
     </row>
@@ -7358,7 +7330,7 @@
       </c>
       <c r="C232" s="2" t="inlineStr">
         <is>
-          <t>MacBook Air do Bento (quebrado)</t>
+          <t>MacBook Pro do Bento</t>
         </is>
       </c>
       <c r="D232" s="2" t="inlineStr">
@@ -7366,14 +7338,14 @@
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E232" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+      <c r="E232" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F232" s="2" t="inlineStr">
         <is>
-          <t>Livros e itens de memória</t>
+          <t>Livros e itens de memória; CUIDADO - eletrônico valioso</t>
         </is>
       </c>
     </row>
@@ -7385,12 +7357,12 @@
       </c>
       <c r="B233" s="2" t="inlineStr">
         <is>
-          <t>Decoração / Memória afetiva</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C233" s="2" t="inlineStr">
         <is>
-          <t>Quadro de pintura da família (presente para o Rodrigo)</t>
+          <t>MacBook Air do Bento (quebrado)</t>
         </is>
       </c>
       <c r="D233" s="2" t="inlineStr">
@@ -7422,7 +7394,7 @@
       </c>
       <c r="C234" s="2" t="inlineStr">
         <is>
-          <t>Suporte de madeira com fotos (presente de aniversário do Rodrigo)</t>
+          <t>Quadro de pintura da família (presente para o Rodrigo)</t>
         </is>
       </c>
       <c r="D234" s="2" t="inlineStr">
@@ -7449,12 +7421,12 @@
       </c>
       <c r="B235" s="2" t="inlineStr">
         <is>
-          <t>Decoração / Viagem</t>
+          <t>Decoração / Memória afetiva</t>
         </is>
       </c>
       <c r="C235" s="2" t="inlineStr">
         <is>
-          <t>Azulejos de Japaratinga</t>
+          <t>Suporte de madeira com fotos (presente de aniversário do Rodrigo)</t>
         </is>
       </c>
       <c r="D235" s="2" t="inlineStr">
@@ -7481,12 +7453,12 @@
       </c>
       <c r="B236" s="2" t="inlineStr">
         <is>
-          <t>Brinquedo / Lúdico</t>
+          <t>Decoração / Viagem</t>
         </is>
       </c>
       <c r="C236" s="2" t="inlineStr">
         <is>
-          <t>Legão</t>
+          <t>Azulejos de Japaratinga</t>
         </is>
       </c>
       <c r="D236" s="2" t="inlineStr">
@@ -7513,12 +7485,12 @@
       </c>
       <c r="B237" s="2" t="inlineStr">
         <is>
-          <t>Memória / Viagem</t>
+          <t>Brinquedo / Lúdico</t>
         </is>
       </c>
       <c r="C237" s="2" t="inlineStr">
         <is>
-          <t>Fita de Nosso Senhor do Bonfim</t>
+          <t>Legão</t>
         </is>
       </c>
       <c r="D237" s="2" t="inlineStr">
@@ -7545,12 +7517,12 @@
       </c>
       <c r="B238" s="2" t="inlineStr">
         <is>
-          <t>Brinquedo / Montagem</t>
+          <t>Memória / Viagem</t>
         </is>
       </c>
       <c r="C238" s="2" t="inlineStr">
         <is>
-          <t>Lego câmera fotográfica (meio desmontado)</t>
+          <t>Fita de Nosso Senhor do Bonfim</t>
         </is>
       </c>
       <c r="D238" s="2" t="inlineStr">
@@ -7577,12 +7549,12 @@
       </c>
       <c r="B239" s="2" t="inlineStr">
         <is>
-          <t>Memória / Viagem</t>
+          <t>Brinquedo / Montagem</t>
         </is>
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>Bandeira com fita do Atacama</t>
+          <t>Lego câmera fotográfica (meio desmontado)</t>
         </is>
       </c>
       <c r="D239" s="2" t="inlineStr">
@@ -7609,12 +7581,12 @@
       </c>
       <c r="B240" s="2" t="inlineStr">
         <is>
-          <t>Memória afetiva</t>
+          <t>Memória / Viagem</t>
         </is>
       </c>
       <c r="C240" s="2" t="inlineStr">
         <is>
-          <t>Envelope com cartinha de Natal para o Papai Noel</t>
+          <t>Bandeira com fita do Atacama</t>
         </is>
       </c>
       <c r="D240" s="2" t="inlineStr">
@@ -7641,12 +7613,12 @@
       </c>
       <c r="B241" s="2" t="inlineStr">
         <is>
-          <t>Jogo / Lúdico</t>
+          <t>Memória afetiva</t>
         </is>
       </c>
       <c r="C241" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeça de Salvador (em montagem)</t>
+          <t>Envelope com cartinha de Natal para o Papai Noel</t>
         </is>
       </c>
       <c r="D241" s="2" t="inlineStr">
@@ -7668,17 +7640,17 @@
     <row r="242">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>Caixa 33</t>
+          <t>Caixa 32</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
         <is>
-          <t>Pintura em tecido</t>
+          <t>Jogo / Lúdico</t>
         </is>
       </c>
       <c r="C242" s="2" t="inlineStr">
         <is>
-          <t>Tintas para pintura em tecido</t>
+          <t>Quebra-cabeça de Salvador (em montagem)</t>
         </is>
       </c>
       <c r="D242" s="2" t="inlineStr">
@@ -7693,7 +7665,7 @@
       </c>
       <c r="F242" s="2" t="inlineStr">
         <is>
-          <t>Artesanato e aromaterapia</t>
+          <t>Livros e itens de memória</t>
         </is>
       </c>
     </row>
@@ -7710,7 +7682,7 @@
       </c>
       <c r="C243" s="2" t="inlineStr">
         <is>
-          <t>Projeto de pintura em tecido em andamento</t>
+          <t>Tintas para pintura em tecido</t>
         </is>
       </c>
       <c r="D243" s="2" t="inlineStr">
@@ -7742,7 +7714,7 @@
       </c>
       <c r="C244" s="2" t="inlineStr">
         <is>
-          <t>Pincéis para pintura</t>
+          <t>Projeto de pintura em tecido em andamento</t>
         </is>
       </c>
       <c r="D244" s="2" t="inlineStr">
@@ -7769,12 +7741,12 @@
       </c>
       <c r="B245" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Pintura em tecido</t>
         </is>
       </c>
       <c r="C245" s="2" t="inlineStr">
         <is>
-          <t>Toalhinha para pintura</t>
+          <t>Pincéis para pintura</t>
         </is>
       </c>
       <c r="D245" s="2" t="inlineStr">
@@ -7801,12 +7773,12 @@
       </c>
       <c r="B246" s="2" t="inlineStr">
         <is>
-          <t>Aromas</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C246" s="2" t="inlineStr">
         <is>
-          <t>Velas</t>
+          <t>Toalhinha para pintura</t>
         </is>
       </c>
       <c r="D246" s="2" t="inlineStr">
@@ -7833,12 +7805,12 @@
       </c>
       <c r="B247" s="2" t="inlineStr">
         <is>
-          <t>Aromaterapia</t>
+          <t>Aromas</t>
         </is>
       </c>
       <c r="C247" s="2" t="inlineStr">
         <is>
-          <t>Óleos essenciais</t>
+          <t>Velas</t>
         </is>
       </c>
       <c r="D247" s="2" t="inlineStr">
@@ -7865,12 +7837,12 @@
       </c>
       <c r="B248" s="2" t="inlineStr">
         <is>
-          <t>Aromas</t>
+          <t>Aromaterapia</t>
         </is>
       </c>
       <c r="C248" s="2" t="inlineStr">
         <is>
-          <t>Incensos</t>
+          <t>Óleos essenciais</t>
         </is>
       </c>
       <c r="D248" s="2" t="inlineStr">
@@ -7897,12 +7869,12 @@
       </c>
       <c r="B249" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Aromas</t>
         </is>
       </c>
       <c r="C249" s="2" t="inlineStr">
         <is>
-          <t>Fita métrica</t>
+          <t>Incensos</t>
         </is>
       </c>
       <c r="D249" s="2" t="inlineStr">
@@ -7934,7 +7906,7 @@
       </c>
       <c r="C250" s="2" t="inlineStr">
         <is>
-          <t>Estilete</t>
+          <t>Fita métrica</t>
         </is>
       </c>
       <c r="D250" s="2" t="inlineStr">
@@ -7966,7 +7938,7 @@
       </c>
       <c r="C251" s="2" t="inlineStr">
         <is>
-          <t>Refil de estilete</t>
+          <t>Estilete</t>
         </is>
       </c>
       <c r="D251" s="2" t="inlineStr">
@@ -7988,22 +7960,22 @@
     <row r="252">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>Caixa 34</t>
+          <t>Caixa 33</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
         <is>
-          <t>Banho</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C252" s="2" t="inlineStr">
         <is>
-          <t>Espumas de banho</t>
+          <t>Refil de estilete</t>
         </is>
       </c>
       <c r="D252" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E252" s="7" t="inlineStr">
@@ -8013,7 +7985,7 @@
       </c>
       <c r="F252" s="2" t="inlineStr">
         <is>
-          <t>Produtos de banho e beleza</t>
+          <t>Artesanato e aromaterapia</t>
         </is>
       </c>
     </row>
@@ -8030,7 +8002,7 @@
       </c>
       <c r="C253" s="2" t="inlineStr">
         <is>
-          <t>Sais de banho</t>
+          <t>Espumas de banho</t>
         </is>
       </c>
       <c r="D253" s="2" t="inlineStr">
@@ -8057,12 +8029,12 @@
       </c>
       <c r="B254" s="2" t="inlineStr">
         <is>
-          <t>Beleza</t>
+          <t>Banho</t>
         </is>
       </c>
       <c r="C254" s="2" t="inlineStr">
         <is>
-          <t>Produtos de beleza em geral</t>
+          <t>Sais de banho</t>
         </is>
       </c>
       <c r="D254" s="2" t="inlineStr">
@@ -8094,7 +8066,7 @@
       </c>
       <c r="C255" s="2" t="inlineStr">
         <is>
-          <t>Body splash</t>
+          <t>Produtos de beleza em geral</t>
         </is>
       </c>
       <c r="D255" s="2" t="inlineStr">
@@ -8121,12 +8093,12 @@
       </c>
       <c r="B256" s="2" t="inlineStr">
         <is>
-          <t>Cabelos</t>
+          <t>Beleza</t>
         </is>
       </c>
       <c r="C256" s="2" t="inlineStr">
         <is>
-          <t>Creme para pentear</t>
+          <t>Body splash</t>
         </is>
       </c>
       <c r="D256" s="2" t="inlineStr">
@@ -8153,12 +8125,12 @@
       </c>
       <c r="B257" s="2" t="inlineStr">
         <is>
-          <t>Skincare</t>
+          <t>Cabelos</t>
         </is>
       </c>
       <c r="C257" s="2" t="inlineStr">
         <is>
-          <t>Creme facial</t>
+          <t>Creme para pentear</t>
         </is>
       </c>
       <c r="D257" s="2" t="inlineStr">
@@ -8180,22 +8152,22 @@
     <row r="258">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>Caixa 35</t>
+          <t>Caixa 34</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
         <is>
-          <t>Fitness</t>
+          <t>Skincare</t>
         </is>
       </c>
       <c r="C258" s="2" t="inlineStr">
         <is>
-          <t>Estação de equilíbrio Domyos</t>
+          <t>Creme facial</t>
         </is>
       </c>
       <c r="D258" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E258" s="7" t="inlineStr">
@@ -8205,7 +8177,7 @@
       </c>
       <c r="F258" s="2" t="inlineStr">
         <is>
-          <t>Equipamentos de fitness e iluminação</t>
+          <t>Produtos de banho e beleza</t>
         </is>
       </c>
     </row>
@@ -8222,7 +8194,7 @@
       </c>
       <c r="C259" s="2" t="inlineStr">
         <is>
-          <t>Bomba de encher bola</t>
+          <t>Estação de equilíbrio Domyos</t>
         </is>
       </c>
       <c r="D259" s="2" t="inlineStr">
@@ -8249,12 +8221,12 @@
       </c>
       <c r="B260" s="2" t="inlineStr">
         <is>
-          <t>Iluminação</t>
+          <t>Fitness</t>
         </is>
       </c>
       <c r="C260" s="2" t="inlineStr">
         <is>
-          <t>Luminária de mesa</t>
+          <t>Bomba de encher bola</t>
         </is>
       </c>
       <c r="D260" s="2" t="inlineStr">
@@ -8281,12 +8253,12 @@
       </c>
       <c r="B261" s="2" t="inlineStr">
         <is>
-          <t>Fitness</t>
+          <t>Iluminação</t>
         </is>
       </c>
       <c r="C261" s="2" t="inlineStr">
         <is>
-          <t>Rolinho para abdominal</t>
+          <t>Luminária de mesa</t>
         </is>
       </c>
       <c r="D261" s="2" t="inlineStr">
@@ -8308,32 +8280,32 @@
     <row r="262">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>Caixa 36</t>
+          <t>Caixa 35</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
         <is>
-          <t>Vestuário</t>
+          <t>Fitness</t>
         </is>
       </c>
       <c r="C262" s="2" t="inlineStr">
         <is>
-          <t>Vestido H&amp;M comprado no Uruguai</t>
+          <t>Rolinho para abdominal</t>
         </is>
       </c>
       <c r="D262" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
-        </is>
-      </c>
-      <c r="E262" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+          <t>Quarto do Bento</t>
+        </is>
+      </c>
+      <c r="E262" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F262" s="2" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Equipamentos de fitness e iluminação</t>
         </is>
       </c>
     </row>
@@ -8350,7 +8322,7 @@
       </c>
       <c r="C263" s="2" t="inlineStr">
         <is>
-          <t>Vestido pretinho básico da Yukon</t>
+          <t>Vestido H&amp;M comprado no Uruguai</t>
         </is>
       </c>
       <c r="D263" s="2" t="inlineStr">
@@ -8382,7 +8354,7 @@
       </c>
       <c r="C264" s="2" t="inlineStr">
         <is>
-          <t>Macacão jeans da Yukon</t>
+          <t>Vestido pretinho básico da Yukon</t>
         </is>
       </c>
       <c r="D264" s="2" t="inlineStr">
@@ -8414,7 +8386,7 @@
       </c>
       <c r="C265" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça lilás</t>
+          <t>Macacão jeans da Yukon</t>
         </is>
       </c>
       <c r="D265" s="2" t="inlineStr">
@@ -8446,7 +8418,7 @@
       </c>
       <c r="C266" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo verde</t>
+          <t>Vestido longo de alça lilás</t>
         </is>
       </c>
       <c r="D266" s="2" t="inlineStr">
@@ -8478,7 +8450,7 @@
       </c>
       <c r="C267" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de oncinha</t>
+          <t>Vestido longo verde</t>
         </is>
       </c>
       <c r="D267" s="2" t="inlineStr">
@@ -8510,7 +8482,7 @@
       </c>
       <c r="C268" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de coração colorido</t>
+          <t>Vestido longo de oncinha</t>
         </is>
       </c>
       <c r="D268" s="2" t="inlineStr">
@@ -8542,7 +8514,7 @@
       </c>
       <c r="C269" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça azul turquesa</t>
+          <t>Vestido longo de coração colorido</t>
         </is>
       </c>
       <c r="D269" s="2" t="inlineStr">
@@ -8574,7 +8546,7 @@
       </c>
       <c r="C270" s="2" t="inlineStr">
         <is>
-          <t>Vestido azul listrado</t>
+          <t>Vestido longo de alça azul turquesa</t>
         </is>
       </c>
       <c r="D270" s="2" t="inlineStr">
@@ -8606,7 +8578,7 @@
       </c>
       <c r="C271" s="2" t="inlineStr">
         <is>
-          <t>Vestido midi preto de bolinhas</t>
+          <t>Vestido azul listrado</t>
         </is>
       </c>
       <c r="D271" s="2" t="inlineStr">
@@ -8638,7 +8610,7 @@
       </c>
       <c r="C272" s="2" t="inlineStr">
         <is>
-          <t>Vestido xadrez vermelho e preto da Yukon</t>
+          <t>Vestido midi preto de bolinhas</t>
         </is>
       </c>
       <c r="D272" s="2" t="inlineStr">
@@ -8670,7 +8642,7 @@
       </c>
       <c r="C273" s="2" t="inlineStr">
         <is>
-          <t>Vestido lilás vichy</t>
+          <t>Vestido xadrez vermelho e preto da Yukon</t>
         </is>
       </c>
       <c r="D273" s="2" t="inlineStr">
@@ -8702,7 +8674,7 @@
       </c>
       <c r="C274" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça rosa</t>
+          <t>Vestido lilás vichy</t>
         </is>
       </c>
       <c r="D274" s="2" t="inlineStr">
@@ -8734,7 +8706,7 @@
       </c>
       <c r="C275" s="2" t="inlineStr">
         <is>
-          <t>Vestido de alça florido colorido da Yukon</t>
+          <t>Vestido longo de alça rosa</t>
         </is>
       </c>
       <c r="D275" s="2" t="inlineStr">
@@ -8766,7 +8738,7 @@
       </c>
       <c r="C276" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça preto</t>
+          <t>Vestido de alça florido colorido da Yukon</t>
         </is>
       </c>
       <c r="D276" s="2" t="inlineStr">
@@ -8798,7 +8770,7 @@
       </c>
       <c r="C277" s="2" t="inlineStr">
         <is>
-          <t>Vestido midi de alça verde</t>
+          <t>Vestido longo de alça preto</t>
         </is>
       </c>
       <c r="D277" s="2" t="inlineStr">
@@ -8830,7 +8802,7 @@
       </c>
       <c r="C278" s="2" t="inlineStr">
         <is>
-          <t>Macacão cinza da Yukon</t>
+          <t>Vestido midi de alça verde</t>
         </is>
       </c>
       <c r="D278" s="2" t="inlineStr">
@@ -8862,7 +8834,7 @@
       </c>
       <c r="C279" s="2" t="inlineStr">
         <is>
-          <t>Short azul de oncinha</t>
+          <t>Macacão cinza da Yukon</t>
         </is>
       </c>
       <c r="D279" s="2" t="inlineStr">
@@ -8894,7 +8866,7 @@
       </c>
       <c r="C280" s="2" t="inlineStr">
         <is>
-          <t>Short jeans de oncinha</t>
+          <t>Short azul de oncinha</t>
         </is>
       </c>
       <c r="D280" s="2" t="inlineStr">
@@ -8926,7 +8898,7 @@
       </c>
       <c r="C281" s="2" t="inlineStr">
         <is>
-          <t>Short jeans com cinto</t>
+          <t>Short jeans de oncinha</t>
         </is>
       </c>
       <c r="D281" s="2" t="inlineStr">
@@ -8958,7 +8930,7 @@
       </c>
       <c r="C282" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans preta</t>
+          <t>Short jeans com cinto</t>
         </is>
       </c>
       <c r="D282" s="2" t="inlineStr">
@@ -8990,7 +8962,7 @@
       </c>
       <c r="C283" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans azul</t>
+          <t>Calça jeans preta</t>
         </is>
       </c>
       <c r="D283" s="2" t="inlineStr">
@@ -9022,7 +8994,7 @@
       </c>
       <c r="C284" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans azul escura</t>
+          <t>Calça jeans azul</t>
         </is>
       </c>
       <c r="D284" s="2" t="inlineStr">
@@ -9054,7 +9026,7 @@
       </c>
       <c r="C285" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans rasgadinha azul</t>
+          <t>Calça jeans azul escura</t>
         </is>
       </c>
       <c r="D285" s="2" t="inlineStr">
@@ -9076,7 +9048,7 @@
     <row r="286">
       <c r="A286" s="2" t="inlineStr">
         <is>
-          <t>Caixa 37</t>
+          <t>Caixa 36</t>
         </is>
       </c>
       <c r="B286" s="2" t="inlineStr">
@@ -9086,7 +9058,7 @@
       </c>
       <c r="C286" s="2" t="inlineStr">
         <is>
-          <t>Roupas de inverno (a catalogar)</t>
+          <t>Calça jeans rasgadinha azul</t>
         </is>
       </c>
       <c r="D286" s="2" t="inlineStr">
@@ -9094,21 +9066,21 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E286" s="6" t="inlineStr">
-        <is>
-          <t>Baixa</t>
+      <c r="E286" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F286" s="2" t="inlineStr">
         <is>
-          <t>Roupas de inverno</t>
+          <t>Roupas</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="2" t="inlineStr">
         <is>
-          <t>Caixa 38</t>
+          <t>Caixa 37</t>
         </is>
       </c>
       <c r="B287" s="2" t="inlineStr">
@@ -9118,7 +9090,7 @@
       </c>
       <c r="C287" s="2" t="inlineStr">
         <is>
-          <t>Macacões de ciclismo</t>
+          <t>Roupas de inverno (a catalogar)</t>
         </is>
       </c>
       <c r="D287" s="2" t="inlineStr">
@@ -9126,14 +9098,14 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E287" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+      <c r="E287" s="6" t="inlineStr">
+        <is>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="F287" s="2" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Roupas de inverno</t>
         </is>
       </c>
     </row>
@@ -9150,7 +9122,7 @@
       </c>
       <c r="C288" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo cinza de manga curta da Youcom</t>
+          <t>Macacões de ciclismo</t>
         </is>
       </c>
       <c r="D288" s="2" t="inlineStr">
@@ -9182,7 +9154,7 @@
       </c>
       <c r="C289" s="2" t="inlineStr">
         <is>
-          <t>Vestido da Ilha de Paquetá da FARM</t>
+          <t>Vestido longo cinza de manga curta da Youcom</t>
         </is>
       </c>
       <c r="D289" s="2" t="inlineStr">
@@ -9214,7 +9186,7 @@
       </c>
       <c r="C290" s="2" t="inlineStr">
         <is>
-          <t>Camiseta do Rolling Stones</t>
+          <t>Vestido da Ilha de Paquetá da FARM</t>
         </is>
       </c>
       <c r="D290" s="2" t="inlineStr">
@@ -9246,7 +9218,7 @@
       </c>
       <c r="C291" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de Japaratinga</t>
+          <t>Camiseta do Rolling Stones</t>
         </is>
       </c>
       <c r="D291" s="2" t="inlineStr">
@@ -9278,7 +9250,7 @@
       </c>
       <c r="C292" s="2" t="inlineStr">
         <is>
-          <t>Camiseta do Van Gogh</t>
+          <t>Camiseta de Japaratinga</t>
         </is>
       </c>
       <c r="D292" s="2" t="inlineStr">
@@ -9310,7 +9282,7 @@
       </c>
       <c r="C293" s="2" t="inlineStr">
         <is>
-          <t>Camiseta cinza do Corgi da Renner</t>
+          <t>Camiseta do Van Gogh</t>
         </is>
       </c>
       <c r="D293" s="2" t="inlineStr">
@@ -9342,7 +9314,7 @@
       </c>
       <c r="C294" s="2" t="inlineStr">
         <is>
-          <t>Calça preta da Decathlon</t>
+          <t>Camiseta cinza do Corgi da Renner</t>
         </is>
       </c>
       <c r="D294" s="2" t="inlineStr">
@@ -9374,7 +9346,7 @@
       </c>
       <c r="C295" s="2" t="inlineStr">
         <is>
-          <t>Camiseta preta da Yukon com estampa de Fusca</t>
+          <t>Calça preta da Decathlon</t>
         </is>
       </c>
       <c r="D295" s="2" t="inlineStr">
@@ -9406,7 +9378,7 @@
       </c>
       <c r="C296" s="2" t="inlineStr">
         <is>
-          <t>Short curtinho da Yukon</t>
+          <t>Camiseta preta da Yukon com estampa de Fusca</t>
         </is>
       </c>
       <c r="D296" s="2" t="inlineStr">
@@ -9438,7 +9410,7 @@
       </c>
       <c r="C297" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da Meia Maratona de Porto Alegre</t>
+          <t>Short curtinho da Yukon</t>
         </is>
       </c>
       <c r="D297" s="2" t="inlineStr">
@@ -9470,7 +9442,7 @@
       </c>
       <c r="C298" s="2" t="inlineStr">
         <is>
-          <t>Camiseta azul da Maratona de Porto Alegre</t>
+          <t>Camiseta da Meia Maratona de Porto Alegre</t>
         </is>
       </c>
       <c r="D298" s="2" t="inlineStr">
@@ -9502,7 +9474,7 @@
       </c>
       <c r="C299" s="2" t="inlineStr">
         <is>
-          <t>Short preto da Nike</t>
+          <t>Camiseta azul da Maratona de Porto Alegre</t>
         </is>
       </c>
       <c r="D299" s="2" t="inlineStr">
@@ -9534,7 +9506,7 @@
       </c>
       <c r="C300" s="2" t="inlineStr">
         <is>
-          <t>Short florido da Nike</t>
+          <t>Short preto da Nike</t>
         </is>
       </c>
       <c r="D300" s="2" t="inlineStr">
@@ -9566,7 +9538,7 @@
       </c>
       <c r="C301" s="2" t="inlineStr">
         <is>
-          <t>Short Nike Trail</t>
+          <t>Short florido da Nike</t>
         </is>
       </c>
       <c r="D301" s="2" t="inlineStr">
@@ -9598,7 +9570,7 @@
       </c>
       <c r="C302" s="2" t="inlineStr">
         <is>
-          <t>Short preto com florido da Alten</t>
+          <t>Short Nike Trail</t>
         </is>
       </c>
       <c r="D302" s="2" t="inlineStr">
@@ -9630,7 +9602,7 @@
       </c>
       <c r="C303" s="2" t="inlineStr">
         <is>
-          <t>Cropped preto</t>
+          <t>Short preto com florido da Alten</t>
         </is>
       </c>
       <c r="D303" s="2" t="inlineStr">
@@ -9662,7 +9634,7 @@
       </c>
       <c r="C304" s="2" t="inlineStr">
         <is>
-          <t>Cropped regata nude</t>
+          <t>Cropped preto</t>
         </is>
       </c>
       <c r="D304" s="2" t="inlineStr">
@@ -9694,7 +9666,7 @@
       </c>
       <c r="C305" s="2" t="inlineStr">
         <is>
-          <t>Top florido da Coffee</t>
+          <t>Cropped regata nude</t>
         </is>
       </c>
       <c r="D305" s="2" t="inlineStr">
@@ -9726,7 +9698,7 @@
       </c>
       <c r="C306" s="2" t="inlineStr">
         <is>
-          <t>Top florido da Nike</t>
+          <t>Top florido da Coffee</t>
         </is>
       </c>
       <c r="D306" s="2" t="inlineStr">
@@ -9758,7 +9730,7 @@
       </c>
       <c r="C307" s="2" t="inlineStr">
         <is>
-          <t>Top azul com preto da Nike</t>
+          <t>Top florido da Nike</t>
         </is>
       </c>
       <c r="D307" s="2" t="inlineStr">
@@ -9790,7 +9762,7 @@
       </c>
       <c r="C308" s="2" t="inlineStr">
         <is>
-          <t>Dois tops pretos da Nike</t>
+          <t>Top azul com preto da Nike</t>
         </is>
       </c>
       <c r="D308" s="2" t="inlineStr">
@@ -9822,7 +9794,7 @@
       </c>
       <c r="C309" s="2" t="inlineStr">
         <is>
-          <t>Top azul e laranja da Reebok</t>
+          <t>Dois tops pretos da Nike</t>
         </is>
       </c>
       <c r="D309" s="2" t="inlineStr">
@@ -9854,7 +9826,7 @@
       </c>
       <c r="C310" s="2" t="inlineStr">
         <is>
-          <t>Top roxo da Reebok</t>
+          <t>Top azul e laranja da Reebok</t>
         </is>
       </c>
       <c r="D310" s="2" t="inlineStr">
@@ -9886,7 +9858,7 @@
       </c>
       <c r="C311" s="2" t="inlineStr">
         <is>
-          <t>Top roxo da Olympikus</t>
+          <t>Top roxo da Reebok</t>
         </is>
       </c>
       <c r="D311" s="2" t="inlineStr">
@@ -9918,7 +9890,7 @@
       </c>
       <c r="C312" s="2" t="inlineStr">
         <is>
-          <t>Top roxo casual da Yukon</t>
+          <t>Top roxo da Olympikus</t>
         </is>
       </c>
       <c r="D312" s="2" t="inlineStr">
@@ -9950,7 +9922,7 @@
       </c>
       <c r="C313" s="2" t="inlineStr">
         <is>
-          <t>Regata rosa da Nike</t>
+          <t>Top roxo casual da Yukon</t>
         </is>
       </c>
       <c r="D313" s="2" t="inlineStr">
@@ -9982,7 +9954,7 @@
       </c>
       <c r="C314" s="2" t="inlineStr">
         <is>
-          <t>Body branco</t>
+          <t>Regata rosa da Nike</t>
         </is>
       </c>
       <c r="D314" s="2" t="inlineStr">
@@ -10014,7 +9986,7 @@
       </c>
       <c r="C315" s="2" t="inlineStr">
         <is>
-          <t>Blusinha cropped florida da Nike</t>
+          <t>Body branco</t>
         </is>
       </c>
       <c r="D315" s="2" t="inlineStr">
@@ -10046,7 +10018,7 @@
       </c>
       <c r="C316" s="2" t="inlineStr">
         <is>
-          <t>Bermuda Nike Pro</t>
+          <t>Blusinha cropped florida da Nike</t>
         </is>
       </c>
       <c r="D316" s="2" t="inlineStr">
@@ -10078,7 +10050,7 @@
       </c>
       <c r="C317" s="2" t="inlineStr">
         <is>
-          <t>Shorts roxo com rosa da Nike Trail</t>
+          <t>Bermuda Nike Pro</t>
         </is>
       </c>
       <c r="D317" s="2" t="inlineStr">
@@ -10110,7 +10082,7 @@
       </c>
       <c r="C318" s="2" t="inlineStr">
         <is>
-          <t>Shorts estampado da Nike</t>
+          <t>Shorts roxo com rosa da Nike Trail</t>
         </is>
       </c>
       <c r="D318" s="2" t="inlineStr">
@@ -10142,7 +10114,7 @@
       </c>
       <c r="C319" s="2" t="inlineStr">
         <is>
-          <t>Shorts laranja e roxo da Olympikus</t>
+          <t>Shorts estampado da Nike</t>
         </is>
       </c>
       <c r="D319" s="2" t="inlineStr">
@@ -10174,7 +10146,7 @@
       </c>
       <c r="C320" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de manga curta da Sogipa</t>
+          <t>Shorts laranja e roxo da Olympikus</t>
         </is>
       </c>
       <c r="D320" s="2" t="inlineStr">
@@ -10206,7 +10178,7 @@
       </c>
       <c r="C321" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da corrida do Grêmio</t>
+          <t>Camiseta de manga curta da Sogipa</t>
         </is>
       </c>
       <c r="D321" s="2" t="inlineStr">
@@ -10238,7 +10210,7 @@
       </c>
       <c r="C322" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da maratona de Floripa</t>
+          <t>Camiseta da corrida do Grêmio</t>
         </is>
       </c>
       <c r="D322" s="2" t="inlineStr">
@@ -10270,7 +10242,7 @@
       </c>
       <c r="C323" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da corrida do Bob Esponja</t>
+          <t>Camiseta da maratona de Floripa</t>
         </is>
       </c>
       <c r="D323" s="2" t="inlineStr">
@@ -10302,7 +10274,7 @@
       </c>
       <c r="C324" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de manga curta da Olympikus</t>
+          <t>Camiseta da corrida do Bob Esponja</t>
         </is>
       </c>
       <c r="D324" s="2" t="inlineStr">
@@ -10334,7 +10306,7 @@
       </c>
       <c r="C325" s="2" t="inlineStr">
         <is>
-          <t>Blusa de alcinha da Insider</t>
+          <t>Camiseta de manga curta da Olympikus</t>
         </is>
       </c>
       <c r="D325" s="2" t="inlineStr">
@@ -10366,7 +10338,7 @@
       </c>
       <c r="C326" s="2" t="inlineStr">
         <is>
-          <t>Camisetas de algodão (todas)</t>
+          <t>Blusa de alcinha da Insider</t>
         </is>
       </c>
       <c r="D326" s="2" t="inlineStr">
@@ -10398,7 +10370,7 @@
       </c>
       <c r="C327" s="2" t="inlineStr">
         <is>
-          <t>Roupão de piscina vinho</t>
+          <t>Camisetas de algodão (todas)</t>
         </is>
       </c>
       <c r="D327" s="2" t="inlineStr">
@@ -10430,7 +10402,7 @@
       </c>
       <c r="C328" s="2" t="inlineStr">
         <is>
-          <t>Dois pijamas da Hope</t>
+          <t>Roupão de piscina vinho</t>
         </is>
       </c>
       <c r="D328" s="2" t="inlineStr">
@@ -10457,12 +10429,12 @@
       </c>
       <c r="B329" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Vestuário</t>
         </is>
       </c>
       <c r="C329" s="2" t="inlineStr">
         <is>
-          <t>Boné Jordan</t>
+          <t>Dois pijamas da Hope</t>
         </is>
       </c>
       <c r="D329" s="2" t="inlineStr">
@@ -10477,7 +10449,7 @@
       </c>
       <c r="F329" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Roupas</t>
         </is>
       </c>
     </row>
@@ -10494,7 +10466,7 @@
       </c>
       <c r="C330" s="2" t="inlineStr">
         <is>
-          <t>Boné preto da Decathlon</t>
+          <t>Boné Jordan</t>
         </is>
       </c>
       <c r="D330" s="2" t="inlineStr">
@@ -10516,17 +10488,17 @@
     <row r="331">
       <c r="A331" s="2" t="inlineStr">
         <is>
-          <t>Caixa 39</t>
+          <t>Caixa 38</t>
         </is>
       </c>
       <c r="B331" s="2" t="inlineStr">
         <is>
-          <t>Fitness</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C331" s="2" t="inlineStr">
         <is>
-          <t>Bands elásticas para exercício (CrossFit)</t>
+          <t>Boné preto da Decathlon</t>
         </is>
       </c>
       <c r="D331" s="2" t="inlineStr">
@@ -10534,12 +10506,16 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E331" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F331" s="2" t="n"/>
+      <c r="E331" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F331" s="2" t="inlineStr">
+        <is>
+          <t>Acessórios</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="2" t="inlineStr">
@@ -10554,7 +10530,7 @@
       </c>
       <c r="C332" s="2" t="inlineStr">
         <is>
-          <t>Elásticos para treino</t>
+          <t>Bands elásticas para exercício (CrossFit)</t>
         </is>
       </c>
       <c r="D332" s="2" t="inlineStr">
@@ -10577,12 +10553,12 @@
       </c>
       <c r="B333" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Fitness</t>
         </is>
       </c>
       <c r="C333" s="2" t="inlineStr">
         <is>
-          <t>Medalhas do ano passado</t>
+          <t>Elásticos para treino</t>
         </is>
       </c>
       <c r="D333" s="2" t="inlineStr">
@@ -10595,11 +10571,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F333" s="2" t="inlineStr">
-        <is>
-          <t>Recordações</t>
-        </is>
-      </c>
+      <c r="F333" s="2" t="n"/>
     </row>
     <row r="334">
       <c r="A334" s="2" t="inlineStr">
@@ -10614,7 +10586,7 @@
       </c>
       <c r="C334" s="2" t="inlineStr">
         <is>
-          <t>Outras medalhas (Amanda e Rodrigo)</t>
+          <t>Medalhas do ano passado</t>
         </is>
       </c>
       <c r="D334" s="2" t="inlineStr">
@@ -10641,12 +10613,12 @@
       </c>
       <c r="B335" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="C335" s="2" t="inlineStr">
         <is>
-          <t>Armação de óculos verde da Guder</t>
+          <t>Outras medalhas (Amanda e Rodrigo)</t>
         </is>
       </c>
       <c r="D335" s="2" t="inlineStr">
@@ -10659,22 +10631,26 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F335" s="2" t="n"/>
+      <c r="F335" s="2" t="inlineStr">
+        <is>
+          <t>Recordações</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="2" t="inlineStr">
         <is>
-          <t>Caixa 40</t>
+          <t>Caixa 39</t>
         </is>
       </c>
       <c r="B336" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C336" s="2" t="inlineStr">
         <is>
-          <t>Organizadores de acrílico</t>
+          <t>Armação de óculos verde da Guder</t>
         </is>
       </c>
       <c r="D336" s="2" t="inlineStr">
@@ -10702,7 +10678,7 @@
       </c>
       <c r="C337" s="2" t="inlineStr">
         <is>
-          <t>Outros organizadores (diversos)</t>
+          <t>Organizadores de acrílico</t>
         </is>
       </c>
       <c r="D337" s="2" t="inlineStr">
@@ -10720,22 +10696,22 @@
     <row r="338">
       <c r="A338" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 40</t>
         </is>
       </c>
       <c r="B338" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C338" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Outros organizadores (diversos)</t>
         </is>
       </c>
       <c r="D338" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E338" s="7" t="inlineStr">
@@ -10758,7 +10734,7 @@
       </c>
       <c r="C339" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D339" s="2" t="inlineStr">
@@ -10781,12 +10757,12 @@
       </c>
       <c r="B340" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C340" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D340" s="2" t="inlineStr">
@@ -10814,7 +10790,7 @@
       </c>
       <c r="C341" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D341" s="2" t="inlineStr">
@@ -10837,12 +10813,12 @@
       </c>
       <c r="B342" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C342" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D342" s="2" t="inlineStr">
@@ -10865,12 +10841,12 @@
       </c>
       <c r="B343" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C343" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr">
@@ -10898,7 +10874,7 @@
       </c>
       <c r="C344" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D344" s="2" t="inlineStr">
@@ -10921,12 +10897,12 @@
       </c>
       <c r="B345" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C345" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D345" s="2" t="inlineStr">
@@ -10944,22 +10920,22 @@
     <row r="346">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C346" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D346" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E346" s="7" t="inlineStr">
@@ -10982,7 +10958,7 @@
       </c>
       <c r="C347" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D347" s="2" t="inlineStr">
@@ -11010,7 +10986,7 @@
       </c>
       <c r="C348" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D348" s="2" t="inlineStr">
@@ -11038,7 +11014,7 @@
       </c>
       <c r="C349" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D349" s="2" t="inlineStr">
@@ -11066,7 +11042,7 @@
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
@@ -11084,22 +11060,22 @@
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E351" s="7" t="inlineStr">
@@ -11122,7 +11098,7 @@
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
@@ -11145,12 +11121,12 @@
       </c>
       <c r="B353" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
@@ -11163,11 +11139,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F353" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F353" s="2" t="n"/>
     </row>
     <row r="354">
       <c r="A354" s="2" t="inlineStr">
@@ -11182,7 +11154,7 @@
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
@@ -11214,7 +11186,7 @@
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11241,12 +11213,12 @@
       </c>
       <c r="B356" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11259,7 +11231,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F356" s="2" t="n"/>
+      <c r="F356" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="2" t="inlineStr">
@@ -11269,12 +11245,12 @@
       </c>
       <c r="B357" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11287,11 +11263,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F357" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F357" s="2" t="n"/>
     </row>
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
@@ -11301,12 +11273,12 @@
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
@@ -11319,7 +11291,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F358" s="2" t="n"/>
+      <c r="F358" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
@@ -11334,7 +11310,7 @@
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
@@ -11357,12 +11333,12 @@
       </c>
       <c r="B360" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
@@ -11390,7 +11366,7 @@
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
@@ -11418,7 +11394,7 @@
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
@@ -11446,7 +11422,7 @@
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
@@ -11474,7 +11450,7 @@
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
@@ -11502,7 +11478,7 @@
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11530,7 +11506,7 @@
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11548,22 +11524,22 @@
     <row r="367">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E367" s="7" t="inlineStr">
@@ -11571,7 +11547,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F367" s="2" t="inlineStr"/>
+      <c r="F367" s="2" t="n"/>
     </row>
     <row r="368">
       <c r="A368" s="2" t="inlineStr">
@@ -11586,7 +11562,7 @@
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
@@ -11599,7 +11575,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F368" s="2" t="inlineStr"/>
+      <c r="F368" s="2" t="n"/>
     </row>
     <row r="369">
       <c r="A369" s="2" t="inlineStr">
@@ -11609,12 +11585,12 @@
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
@@ -11627,7 +11603,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F369" s="2" t="inlineStr"/>
+      <c r="F369" s="2" t="n"/>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
@@ -11637,12 +11613,12 @@
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11655,7 +11631,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F370" s="2" t="inlineStr"/>
+      <c r="F370" s="2" t="n"/>
     </row>
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
@@ -11665,12 +11641,12 @@
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11683,27 +11659,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F371" s="2" t="inlineStr"/>
+      <c r="F371" s="2" t="n"/>
     </row>
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E372" s="7" t="inlineStr">
@@ -11726,7 +11702,7 @@
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
@@ -11754,7 +11730,7 @@
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
@@ -11782,7 +11758,7 @@
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
@@ -11805,12 +11781,12 @@
       </c>
       <c r="B376" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11838,7 +11814,7 @@
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11861,12 +11837,12 @@
       </c>
       <c r="B378" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
@@ -11894,7 +11870,7 @@
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
@@ -11922,7 +11898,7 @@
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
@@ -11945,12 +11921,12 @@
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
@@ -11978,7 +11954,7 @@
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
@@ -12001,12 +11977,12 @@
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -12034,7 +12010,7 @@
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12062,7 +12038,7 @@
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12080,22 +12056,22 @@
     <row r="386">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E386" s="7" t="inlineStr">
@@ -12118,7 +12094,7 @@
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12136,7 +12112,7 @@
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
@@ -12146,7 +12122,7 @@
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Roupa de cama</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
@@ -12164,62 +12140,62 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Roupa de cama</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E389" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F389" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E389" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F389" s="2" t="n"/>
     </row>
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E390" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F390" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E390" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F390" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
@@ -12229,12 +12205,12 @@
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
@@ -12262,7 +12238,7 @@
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12285,12 +12261,12 @@
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12318,7 +12294,7 @@
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12341,12 +12317,12 @@
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12369,12 +12345,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12397,12 +12373,12 @@
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12425,12 +12401,12 @@
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12453,12 +12429,12 @@
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12481,12 +12457,12 @@
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12509,12 +12485,12 @@
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12532,17 +12508,17 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12570,7 +12546,7 @@
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12598,7 +12574,7 @@
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12621,12 +12597,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12644,22 +12620,22 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E406" s="7" t="inlineStr">
@@ -12682,7 +12658,7 @@
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12705,12 +12681,12 @@
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12738,7 +12714,7 @@
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12761,12 +12737,12 @@
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12794,7 +12770,7 @@
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12822,7 +12798,7 @@
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12850,7 +12826,7 @@
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12878,7 +12854,7 @@
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12906,7 +12882,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12934,7 +12910,7 @@
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12962,7 +12938,7 @@
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12990,7 +12966,7 @@
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -13018,7 +12994,7 @@
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13046,7 +13022,7 @@
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13074,7 +13050,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13092,22 +13068,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13130,7 +13106,7 @@
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13158,7 +13134,7 @@
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13186,7 +13162,7 @@
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13204,22 +13180,22 @@
     <row r="426">
       <c r="A426" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E426" s="7" t="inlineStr">
@@ -13242,7 +13218,7 @@
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13270,7 +13246,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13298,7 +13274,7 @@
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13326,7 +13302,7 @@
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13344,22 +13320,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13382,7 +13358,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13410,7 +13386,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13438,7 +13414,7 @@
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Funko Pop Slash</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13466,7 +13442,7 @@
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Funko Pop Axl Rose</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13494,7 +13470,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Hot Wheels – Naves Star Wars</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13522,20 +13498,48 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D437" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E437" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F437" s="2" t="n"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B438" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C438" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D437" s="2" t="inlineStr">
-        <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E437" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F437" s="2" t="n"/>
+      <c r="D438" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E438" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F438" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13574,7 +13578,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4">
@@ -13594,7 +13598,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona luminárias USB na Caixa 35
- Total: 438 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F438"/>
+  <dimension ref="A1:F439"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6219,7 +6219,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F196" s="2" t="inlineStr"/>
+      <c r="F196" s="2" t="n"/>
     </row>
     <row r="197">
       <c r="A197" s="2" t="inlineStr">
@@ -6247,7 +6247,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F197" s="2" t="inlineStr"/>
+      <c r="F197" s="2" t="n"/>
     </row>
     <row r="198">
       <c r="A198" s="2" t="inlineStr">
@@ -6275,7 +6275,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F198" s="2" t="inlineStr"/>
+      <c r="F198" s="2" t="n"/>
     </row>
     <row r="199">
       <c r="A199" s="2" t="inlineStr">
@@ -6303,7 +6303,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F199" s="2" t="inlineStr"/>
+      <c r="F199" s="2" t="n"/>
     </row>
     <row r="200">
       <c r="A200" s="2" t="inlineStr">
@@ -6331,7 +6331,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F200" s="2" t="inlineStr"/>
+      <c r="F200" s="2" t="n"/>
     </row>
     <row r="201">
       <c r="A201" s="2" t="inlineStr">
@@ -6359,7 +6359,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F201" s="2" t="inlineStr"/>
+      <c r="F201" s="2" t="n"/>
     </row>
     <row r="202">
       <c r="A202" s="2" t="inlineStr">
@@ -6387,7 +6387,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F202" s="2" t="inlineStr"/>
+      <c r="F202" s="2" t="n"/>
     </row>
     <row r="203">
       <c r="A203" s="2" t="inlineStr">
@@ -8312,34 +8312,30 @@
     <row r="263">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>Caixa 36</t>
+          <t>Caixa 35</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
         <is>
-          <t>Vestuário</t>
+          <t>Iluminação</t>
         </is>
       </c>
       <c r="C263" s="2" t="inlineStr">
         <is>
-          <t>Vestido H&amp;M comprado no Uruguai</t>
+          <t>Luminárias de móvel USB</t>
         </is>
       </c>
       <c r="D263" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
-        </is>
-      </c>
-      <c r="E263" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F263" s="2" t="inlineStr">
-        <is>
-          <t>Roupas</t>
-        </is>
-      </c>
+          <t>Quarto do Bento</t>
+        </is>
+      </c>
+      <c r="E263" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F263" s="2" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="2" t="inlineStr">
@@ -8354,7 +8350,7 @@
       </c>
       <c r="C264" s="2" t="inlineStr">
         <is>
-          <t>Vestido pretinho básico da Yukon</t>
+          <t>Vestido H&amp;M comprado no Uruguai</t>
         </is>
       </c>
       <c r="D264" s="2" t="inlineStr">
@@ -8386,7 +8382,7 @@
       </c>
       <c r="C265" s="2" t="inlineStr">
         <is>
-          <t>Macacão jeans da Yukon</t>
+          <t>Vestido pretinho básico da Yukon</t>
         </is>
       </c>
       <c r="D265" s="2" t="inlineStr">
@@ -8418,7 +8414,7 @@
       </c>
       <c r="C266" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça lilás</t>
+          <t>Macacão jeans da Yukon</t>
         </is>
       </c>
       <c r="D266" s="2" t="inlineStr">
@@ -8450,7 +8446,7 @@
       </c>
       <c r="C267" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo verde</t>
+          <t>Vestido longo de alça lilás</t>
         </is>
       </c>
       <c r="D267" s="2" t="inlineStr">
@@ -8482,7 +8478,7 @@
       </c>
       <c r="C268" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de oncinha</t>
+          <t>Vestido longo verde</t>
         </is>
       </c>
       <c r="D268" s="2" t="inlineStr">
@@ -8514,7 +8510,7 @@
       </c>
       <c r="C269" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de coração colorido</t>
+          <t>Vestido longo de oncinha</t>
         </is>
       </c>
       <c r="D269" s="2" t="inlineStr">
@@ -8546,7 +8542,7 @@
       </c>
       <c r="C270" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça azul turquesa</t>
+          <t>Vestido longo de coração colorido</t>
         </is>
       </c>
       <c r="D270" s="2" t="inlineStr">
@@ -8578,7 +8574,7 @@
       </c>
       <c r="C271" s="2" t="inlineStr">
         <is>
-          <t>Vestido azul listrado</t>
+          <t>Vestido longo de alça azul turquesa</t>
         </is>
       </c>
       <c r="D271" s="2" t="inlineStr">
@@ -8610,7 +8606,7 @@
       </c>
       <c r="C272" s="2" t="inlineStr">
         <is>
-          <t>Vestido midi preto de bolinhas</t>
+          <t>Vestido azul listrado</t>
         </is>
       </c>
       <c r="D272" s="2" t="inlineStr">
@@ -8642,7 +8638,7 @@
       </c>
       <c r="C273" s="2" t="inlineStr">
         <is>
-          <t>Vestido xadrez vermelho e preto da Yukon</t>
+          <t>Vestido midi preto de bolinhas</t>
         </is>
       </c>
       <c r="D273" s="2" t="inlineStr">
@@ -8674,7 +8670,7 @@
       </c>
       <c r="C274" s="2" t="inlineStr">
         <is>
-          <t>Vestido lilás vichy</t>
+          <t>Vestido xadrez vermelho e preto da Yukon</t>
         </is>
       </c>
       <c r="D274" s="2" t="inlineStr">
@@ -8706,7 +8702,7 @@
       </c>
       <c r="C275" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça rosa</t>
+          <t>Vestido lilás vichy</t>
         </is>
       </c>
       <c r="D275" s="2" t="inlineStr">
@@ -8738,7 +8734,7 @@
       </c>
       <c r="C276" s="2" t="inlineStr">
         <is>
-          <t>Vestido de alça florido colorido da Yukon</t>
+          <t>Vestido longo de alça rosa</t>
         </is>
       </c>
       <c r="D276" s="2" t="inlineStr">
@@ -8770,7 +8766,7 @@
       </c>
       <c r="C277" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo de alça preto</t>
+          <t>Vestido de alça florido colorido da Yukon</t>
         </is>
       </c>
       <c r="D277" s="2" t="inlineStr">
@@ -8802,7 +8798,7 @@
       </c>
       <c r="C278" s="2" t="inlineStr">
         <is>
-          <t>Vestido midi de alça verde</t>
+          <t>Vestido longo de alça preto</t>
         </is>
       </c>
       <c r="D278" s="2" t="inlineStr">
@@ -8834,7 +8830,7 @@
       </c>
       <c r="C279" s="2" t="inlineStr">
         <is>
-          <t>Macacão cinza da Yukon</t>
+          <t>Vestido midi de alça verde</t>
         </is>
       </c>
       <c r="D279" s="2" t="inlineStr">
@@ -8866,7 +8862,7 @@
       </c>
       <c r="C280" s="2" t="inlineStr">
         <is>
-          <t>Short azul de oncinha</t>
+          <t>Macacão cinza da Yukon</t>
         </is>
       </c>
       <c r="D280" s="2" t="inlineStr">
@@ -8898,7 +8894,7 @@
       </c>
       <c r="C281" s="2" t="inlineStr">
         <is>
-          <t>Short jeans de oncinha</t>
+          <t>Short azul de oncinha</t>
         </is>
       </c>
       <c r="D281" s="2" t="inlineStr">
@@ -8930,7 +8926,7 @@
       </c>
       <c r="C282" s="2" t="inlineStr">
         <is>
-          <t>Short jeans com cinto</t>
+          <t>Short jeans de oncinha</t>
         </is>
       </c>
       <c r="D282" s="2" t="inlineStr">
@@ -8962,7 +8958,7 @@
       </c>
       <c r="C283" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans preta</t>
+          <t>Short jeans com cinto</t>
         </is>
       </c>
       <c r="D283" s="2" t="inlineStr">
@@ -8994,7 +8990,7 @@
       </c>
       <c r="C284" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans azul</t>
+          <t>Calça jeans preta</t>
         </is>
       </c>
       <c r="D284" s="2" t="inlineStr">
@@ -9026,7 +9022,7 @@
       </c>
       <c r="C285" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans azul escura</t>
+          <t>Calça jeans azul</t>
         </is>
       </c>
       <c r="D285" s="2" t="inlineStr">
@@ -9058,7 +9054,7 @@
       </c>
       <c r="C286" s="2" t="inlineStr">
         <is>
-          <t>Calça jeans rasgadinha azul</t>
+          <t>Calça jeans azul escura</t>
         </is>
       </c>
       <c r="D286" s="2" t="inlineStr">
@@ -9080,7 +9076,7 @@
     <row r="287">
       <c r="A287" s="2" t="inlineStr">
         <is>
-          <t>Caixa 37</t>
+          <t>Caixa 36</t>
         </is>
       </c>
       <c r="B287" s="2" t="inlineStr">
@@ -9090,7 +9086,7 @@
       </c>
       <c r="C287" s="2" t="inlineStr">
         <is>
-          <t>Roupas de inverno (a catalogar)</t>
+          <t>Calça jeans rasgadinha azul</t>
         </is>
       </c>
       <c r="D287" s="2" t="inlineStr">
@@ -9098,21 +9094,21 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E287" s="6" t="inlineStr">
-        <is>
-          <t>Baixa</t>
+      <c r="E287" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F287" s="2" t="inlineStr">
         <is>
-          <t>Roupas de inverno</t>
+          <t>Roupas</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="2" t="inlineStr">
         <is>
-          <t>Caixa 38</t>
+          <t>Caixa 37</t>
         </is>
       </c>
       <c r="B288" s="2" t="inlineStr">
@@ -9122,7 +9118,7 @@
       </c>
       <c r="C288" s="2" t="inlineStr">
         <is>
-          <t>Macacões de ciclismo</t>
+          <t>Roupas de inverno (a catalogar)</t>
         </is>
       </c>
       <c r="D288" s="2" t="inlineStr">
@@ -9130,14 +9126,14 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E288" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+      <c r="E288" s="6" t="inlineStr">
+        <is>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="F288" s="2" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Roupas de inverno</t>
         </is>
       </c>
     </row>
@@ -9154,7 +9150,7 @@
       </c>
       <c r="C289" s="2" t="inlineStr">
         <is>
-          <t>Vestido longo cinza de manga curta da Youcom</t>
+          <t>Macacões de ciclismo</t>
         </is>
       </c>
       <c r="D289" s="2" t="inlineStr">
@@ -9186,7 +9182,7 @@
       </c>
       <c r="C290" s="2" t="inlineStr">
         <is>
-          <t>Vestido da Ilha de Paquetá da FARM</t>
+          <t>Vestido longo cinza de manga curta da Youcom</t>
         </is>
       </c>
       <c r="D290" s="2" t="inlineStr">
@@ -9218,7 +9214,7 @@
       </c>
       <c r="C291" s="2" t="inlineStr">
         <is>
-          <t>Camiseta do Rolling Stones</t>
+          <t>Vestido da Ilha de Paquetá da FARM</t>
         </is>
       </c>
       <c r="D291" s="2" t="inlineStr">
@@ -9250,7 +9246,7 @@
       </c>
       <c r="C292" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de Japaratinga</t>
+          <t>Camiseta do Rolling Stones</t>
         </is>
       </c>
       <c r="D292" s="2" t="inlineStr">
@@ -9282,7 +9278,7 @@
       </c>
       <c r="C293" s="2" t="inlineStr">
         <is>
-          <t>Camiseta do Van Gogh</t>
+          <t>Camiseta de Japaratinga</t>
         </is>
       </c>
       <c r="D293" s="2" t="inlineStr">
@@ -9314,7 +9310,7 @@
       </c>
       <c r="C294" s="2" t="inlineStr">
         <is>
-          <t>Camiseta cinza do Corgi da Renner</t>
+          <t>Camiseta do Van Gogh</t>
         </is>
       </c>
       <c r="D294" s="2" t="inlineStr">
@@ -9346,7 +9342,7 @@
       </c>
       <c r="C295" s="2" t="inlineStr">
         <is>
-          <t>Calça preta da Decathlon</t>
+          <t>Camiseta cinza do Corgi da Renner</t>
         </is>
       </c>
       <c r="D295" s="2" t="inlineStr">
@@ -9378,7 +9374,7 @@
       </c>
       <c r="C296" s="2" t="inlineStr">
         <is>
-          <t>Camiseta preta da Yukon com estampa de Fusca</t>
+          <t>Calça preta da Decathlon</t>
         </is>
       </c>
       <c r="D296" s="2" t="inlineStr">
@@ -9410,7 +9406,7 @@
       </c>
       <c r="C297" s="2" t="inlineStr">
         <is>
-          <t>Short curtinho da Yukon</t>
+          <t>Camiseta preta da Yukon com estampa de Fusca</t>
         </is>
       </c>
       <c r="D297" s="2" t="inlineStr">
@@ -9442,7 +9438,7 @@
       </c>
       <c r="C298" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da Meia Maratona de Porto Alegre</t>
+          <t>Short curtinho da Yukon</t>
         </is>
       </c>
       <c r="D298" s="2" t="inlineStr">
@@ -9474,7 +9470,7 @@
       </c>
       <c r="C299" s="2" t="inlineStr">
         <is>
-          <t>Camiseta azul da Maratona de Porto Alegre</t>
+          <t>Camiseta da Meia Maratona de Porto Alegre</t>
         </is>
       </c>
       <c r="D299" s="2" t="inlineStr">
@@ -9506,7 +9502,7 @@
       </c>
       <c r="C300" s="2" t="inlineStr">
         <is>
-          <t>Short preto da Nike</t>
+          <t>Camiseta azul da Maratona de Porto Alegre</t>
         </is>
       </c>
       <c r="D300" s="2" t="inlineStr">
@@ -9538,7 +9534,7 @@
       </c>
       <c r="C301" s="2" t="inlineStr">
         <is>
-          <t>Short florido da Nike</t>
+          <t>Short preto da Nike</t>
         </is>
       </c>
       <c r="D301" s="2" t="inlineStr">
@@ -9570,7 +9566,7 @@
       </c>
       <c r="C302" s="2" t="inlineStr">
         <is>
-          <t>Short Nike Trail</t>
+          <t>Short florido da Nike</t>
         </is>
       </c>
       <c r="D302" s="2" t="inlineStr">
@@ -9602,7 +9598,7 @@
       </c>
       <c r="C303" s="2" t="inlineStr">
         <is>
-          <t>Short preto com florido da Alten</t>
+          <t>Short Nike Trail</t>
         </is>
       </c>
       <c r="D303" s="2" t="inlineStr">
@@ -9634,7 +9630,7 @@
       </c>
       <c r="C304" s="2" t="inlineStr">
         <is>
-          <t>Cropped preto</t>
+          <t>Short preto com florido da Alten</t>
         </is>
       </c>
       <c r="D304" s="2" t="inlineStr">
@@ -9666,7 +9662,7 @@
       </c>
       <c r="C305" s="2" t="inlineStr">
         <is>
-          <t>Cropped regata nude</t>
+          <t>Cropped preto</t>
         </is>
       </c>
       <c r="D305" s="2" t="inlineStr">
@@ -9698,7 +9694,7 @@
       </c>
       <c r="C306" s="2" t="inlineStr">
         <is>
-          <t>Top florido da Coffee</t>
+          <t>Cropped regata nude</t>
         </is>
       </c>
       <c r="D306" s="2" t="inlineStr">
@@ -9730,7 +9726,7 @@
       </c>
       <c r="C307" s="2" t="inlineStr">
         <is>
-          <t>Top florido da Nike</t>
+          <t>Top florido da Coffee</t>
         </is>
       </c>
       <c r="D307" s="2" t="inlineStr">
@@ -9762,7 +9758,7 @@
       </c>
       <c r="C308" s="2" t="inlineStr">
         <is>
-          <t>Top azul com preto da Nike</t>
+          <t>Top florido da Nike</t>
         </is>
       </c>
       <c r="D308" s="2" t="inlineStr">
@@ -9794,7 +9790,7 @@
       </c>
       <c r="C309" s="2" t="inlineStr">
         <is>
-          <t>Dois tops pretos da Nike</t>
+          <t>Top azul com preto da Nike</t>
         </is>
       </c>
       <c r="D309" s="2" t="inlineStr">
@@ -9826,7 +9822,7 @@
       </c>
       <c r="C310" s="2" t="inlineStr">
         <is>
-          <t>Top azul e laranja da Reebok</t>
+          <t>Dois tops pretos da Nike</t>
         </is>
       </c>
       <c r="D310" s="2" t="inlineStr">
@@ -9858,7 +9854,7 @@
       </c>
       <c r="C311" s="2" t="inlineStr">
         <is>
-          <t>Top roxo da Reebok</t>
+          <t>Top azul e laranja da Reebok</t>
         </is>
       </c>
       <c r="D311" s="2" t="inlineStr">
@@ -9890,7 +9886,7 @@
       </c>
       <c r="C312" s="2" t="inlineStr">
         <is>
-          <t>Top roxo da Olympikus</t>
+          <t>Top roxo da Reebok</t>
         </is>
       </c>
       <c r="D312" s="2" t="inlineStr">
@@ -9922,7 +9918,7 @@
       </c>
       <c r="C313" s="2" t="inlineStr">
         <is>
-          <t>Top roxo casual da Yukon</t>
+          <t>Top roxo da Olympikus</t>
         </is>
       </c>
       <c r="D313" s="2" t="inlineStr">
@@ -9954,7 +9950,7 @@
       </c>
       <c r="C314" s="2" t="inlineStr">
         <is>
-          <t>Regata rosa da Nike</t>
+          <t>Top roxo casual da Yukon</t>
         </is>
       </c>
       <c r="D314" s="2" t="inlineStr">
@@ -9986,7 +9982,7 @@
       </c>
       <c r="C315" s="2" t="inlineStr">
         <is>
-          <t>Body branco</t>
+          <t>Regata rosa da Nike</t>
         </is>
       </c>
       <c r="D315" s="2" t="inlineStr">
@@ -10018,7 +10014,7 @@
       </c>
       <c r="C316" s="2" t="inlineStr">
         <is>
-          <t>Blusinha cropped florida da Nike</t>
+          <t>Body branco</t>
         </is>
       </c>
       <c r="D316" s="2" t="inlineStr">
@@ -10050,7 +10046,7 @@
       </c>
       <c r="C317" s="2" t="inlineStr">
         <is>
-          <t>Bermuda Nike Pro</t>
+          <t>Blusinha cropped florida da Nike</t>
         </is>
       </c>
       <c r="D317" s="2" t="inlineStr">
@@ -10082,7 +10078,7 @@
       </c>
       <c r="C318" s="2" t="inlineStr">
         <is>
-          <t>Shorts roxo com rosa da Nike Trail</t>
+          <t>Bermuda Nike Pro</t>
         </is>
       </c>
       <c r="D318" s="2" t="inlineStr">
@@ -10114,7 +10110,7 @@
       </c>
       <c r="C319" s="2" t="inlineStr">
         <is>
-          <t>Shorts estampado da Nike</t>
+          <t>Shorts roxo com rosa da Nike Trail</t>
         </is>
       </c>
       <c r="D319" s="2" t="inlineStr">
@@ -10146,7 +10142,7 @@
       </c>
       <c r="C320" s="2" t="inlineStr">
         <is>
-          <t>Shorts laranja e roxo da Olympikus</t>
+          <t>Shorts estampado da Nike</t>
         </is>
       </c>
       <c r="D320" s="2" t="inlineStr">
@@ -10178,7 +10174,7 @@
       </c>
       <c r="C321" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de manga curta da Sogipa</t>
+          <t>Shorts laranja e roxo da Olympikus</t>
         </is>
       </c>
       <c r="D321" s="2" t="inlineStr">
@@ -10210,7 +10206,7 @@
       </c>
       <c r="C322" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da corrida do Grêmio</t>
+          <t>Camiseta de manga curta da Sogipa</t>
         </is>
       </c>
       <c r="D322" s="2" t="inlineStr">
@@ -10242,7 +10238,7 @@
       </c>
       <c r="C323" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da maratona de Floripa</t>
+          <t>Camiseta da corrida do Grêmio</t>
         </is>
       </c>
       <c r="D323" s="2" t="inlineStr">
@@ -10274,7 +10270,7 @@
       </c>
       <c r="C324" s="2" t="inlineStr">
         <is>
-          <t>Camiseta da corrida do Bob Esponja</t>
+          <t>Camiseta da maratona de Floripa</t>
         </is>
       </c>
       <c r="D324" s="2" t="inlineStr">
@@ -10306,7 +10302,7 @@
       </c>
       <c r="C325" s="2" t="inlineStr">
         <is>
-          <t>Camiseta de manga curta da Olympikus</t>
+          <t>Camiseta da corrida do Bob Esponja</t>
         </is>
       </c>
       <c r="D325" s="2" t="inlineStr">
@@ -10338,7 +10334,7 @@
       </c>
       <c r="C326" s="2" t="inlineStr">
         <is>
-          <t>Blusa de alcinha da Insider</t>
+          <t>Camiseta de manga curta da Olympikus</t>
         </is>
       </c>
       <c r="D326" s="2" t="inlineStr">
@@ -10370,7 +10366,7 @@
       </c>
       <c r="C327" s="2" t="inlineStr">
         <is>
-          <t>Camisetas de algodão (todas)</t>
+          <t>Blusa de alcinha da Insider</t>
         </is>
       </c>
       <c r="D327" s="2" t="inlineStr">
@@ -10402,7 +10398,7 @@
       </c>
       <c r="C328" s="2" t="inlineStr">
         <is>
-          <t>Roupão de piscina vinho</t>
+          <t>Camisetas de algodão (todas)</t>
         </is>
       </c>
       <c r="D328" s="2" t="inlineStr">
@@ -10434,7 +10430,7 @@
       </c>
       <c r="C329" s="2" t="inlineStr">
         <is>
-          <t>Dois pijamas da Hope</t>
+          <t>Roupão de piscina vinho</t>
         </is>
       </c>
       <c r="D329" s="2" t="inlineStr">
@@ -10461,12 +10457,12 @@
       </c>
       <c r="B330" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Vestuário</t>
         </is>
       </c>
       <c r="C330" s="2" t="inlineStr">
         <is>
-          <t>Boné Jordan</t>
+          <t>Dois pijamas da Hope</t>
         </is>
       </c>
       <c r="D330" s="2" t="inlineStr">
@@ -10481,7 +10477,7 @@
       </c>
       <c r="F330" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Roupas</t>
         </is>
       </c>
     </row>
@@ -10498,7 +10494,7 @@
       </c>
       <c r="C331" s="2" t="inlineStr">
         <is>
-          <t>Boné preto da Decathlon</t>
+          <t>Boné Jordan</t>
         </is>
       </c>
       <c r="D331" s="2" t="inlineStr">
@@ -10520,17 +10516,17 @@
     <row r="332">
       <c r="A332" s="2" t="inlineStr">
         <is>
-          <t>Caixa 39</t>
+          <t>Caixa 38</t>
         </is>
       </c>
       <c r="B332" s="2" t="inlineStr">
         <is>
-          <t>Fitness</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C332" s="2" t="inlineStr">
         <is>
-          <t>Bands elásticas para exercício (CrossFit)</t>
+          <t>Boné preto da Decathlon</t>
         </is>
       </c>
       <c r="D332" s="2" t="inlineStr">
@@ -10538,12 +10534,16 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E332" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F332" s="2" t="n"/>
+      <c r="E332" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F332" s="2" t="inlineStr">
+        <is>
+          <t>Acessórios</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="2" t="inlineStr">
@@ -10558,7 +10558,7 @@
       </c>
       <c r="C333" s="2" t="inlineStr">
         <is>
-          <t>Elásticos para treino</t>
+          <t>Bands elásticas para exercício (CrossFit)</t>
         </is>
       </c>
       <c r="D333" s="2" t="inlineStr">
@@ -10581,12 +10581,12 @@
       </c>
       <c r="B334" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Fitness</t>
         </is>
       </c>
       <c r="C334" s="2" t="inlineStr">
         <is>
-          <t>Medalhas do ano passado</t>
+          <t>Elásticos para treino</t>
         </is>
       </c>
       <c r="D334" s="2" t="inlineStr">
@@ -10599,11 +10599,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F334" s="2" t="inlineStr">
-        <is>
-          <t>Recordações</t>
-        </is>
-      </c>
+      <c r="F334" s="2" t="n"/>
     </row>
     <row r="335">
       <c r="A335" s="2" t="inlineStr">
@@ -10618,7 +10614,7 @@
       </c>
       <c r="C335" s="2" t="inlineStr">
         <is>
-          <t>Outras medalhas (Amanda e Rodrigo)</t>
+          <t>Medalhas do ano passado</t>
         </is>
       </c>
       <c r="D335" s="2" t="inlineStr">
@@ -10645,12 +10641,12 @@
       </c>
       <c r="B336" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="C336" s="2" t="inlineStr">
         <is>
-          <t>Armação de óculos verde da Guder</t>
+          <t>Outras medalhas (Amanda e Rodrigo)</t>
         </is>
       </c>
       <c r="D336" s="2" t="inlineStr">
@@ -10663,22 +10659,26 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F336" s="2" t="n"/>
+      <c r="F336" s="2" t="inlineStr">
+        <is>
+          <t>Recordações</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="2" t="inlineStr">
         <is>
-          <t>Caixa 40</t>
+          <t>Caixa 39</t>
         </is>
       </c>
       <c r="B337" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C337" s="2" t="inlineStr">
         <is>
-          <t>Organizadores de acrílico</t>
+          <t>Armação de óculos verde da Guder</t>
         </is>
       </c>
       <c r="D337" s="2" t="inlineStr">
@@ -10706,7 +10706,7 @@
       </c>
       <c r="C338" s="2" t="inlineStr">
         <is>
-          <t>Outros organizadores (diversos)</t>
+          <t>Organizadores de acrílico</t>
         </is>
       </c>
       <c r="D338" s="2" t="inlineStr">
@@ -10724,22 +10724,22 @@
     <row r="339">
       <c r="A339" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 40</t>
         </is>
       </c>
       <c r="B339" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C339" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Outros organizadores (diversos)</t>
         </is>
       </c>
       <c r="D339" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E339" s="7" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="C340" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D340" s="2" t="inlineStr">
@@ -10785,12 +10785,12 @@
       </c>
       <c r="B341" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C341" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D341" s="2" t="inlineStr">
@@ -10818,7 +10818,7 @@
       </c>
       <c r="C342" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D342" s="2" t="inlineStr">
@@ -10841,12 +10841,12 @@
       </c>
       <c r="B343" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C343" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr">
@@ -10869,12 +10869,12 @@
       </c>
       <c r="B344" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C344" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D344" s="2" t="inlineStr">
@@ -10902,7 +10902,7 @@
       </c>
       <c r="C345" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D345" s="2" t="inlineStr">
@@ -10925,12 +10925,12 @@
       </c>
       <c r="B346" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C346" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D346" s="2" t="inlineStr">
@@ -10948,22 +10948,22 @@
     <row r="347">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C347" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D347" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E347" s="7" t="inlineStr">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="C348" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D348" s="2" t="inlineStr">
@@ -11014,7 +11014,7 @@
       </c>
       <c r="C349" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D349" s="2" t="inlineStr">
@@ -11042,7 +11042,7 @@
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
@@ -11088,22 +11088,22 @@
     <row r="352">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E352" s="7" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
@@ -11149,12 +11149,12 @@
       </c>
       <c r="B354" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
@@ -11167,11 +11167,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F354" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F354" s="2" t="n"/>
     </row>
     <row r="355">
       <c r="A355" s="2" t="inlineStr">
@@ -11186,7 +11182,7 @@
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11218,7 +11214,7 @@
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11245,12 +11241,12 @@
       </c>
       <c r="B357" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11263,7 +11259,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F357" s="2" t="n"/>
+      <c r="F357" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
@@ -11273,12 +11273,12 @@
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
@@ -11291,11 +11291,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F358" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F358" s="2" t="n"/>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
@@ -11305,12 +11301,12 @@
       </c>
       <c r="B359" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
@@ -11323,7 +11319,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F359" s="2" t="n"/>
+      <c r="F359" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="2" t="inlineStr">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
@@ -11361,12 +11361,12 @@
       </c>
       <c r="B361" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
@@ -11394,7 +11394,7 @@
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
@@ -11422,7 +11422,7 @@
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
@@ -11450,7 +11450,7 @@
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
@@ -11478,7 +11478,7 @@
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11506,7 +11506,7 @@
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11534,7 +11534,7 @@
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
@@ -11552,22 +11552,22 @@
     <row r="368">
       <c r="A368" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B368" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E368" s="7" t="inlineStr">
@@ -11590,7 +11590,7 @@
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
@@ -11613,12 +11613,12 @@
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11641,12 +11641,12 @@
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11669,12 +11669,12 @@
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
@@ -11692,22 +11692,22 @@
     <row r="373">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E373" s="7" t="inlineStr">
@@ -11730,7 +11730,7 @@
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
@@ -11758,7 +11758,7 @@
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
@@ -11786,7 +11786,7 @@
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11809,12 +11809,12 @@
       </c>
       <c r="B377" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11842,7 +11842,7 @@
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
@@ -11865,12 +11865,12 @@
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
@@ -11926,7 +11926,7 @@
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
@@ -11949,12 +11949,12 @@
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
@@ -11982,7 +11982,7 @@
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -12005,12 +12005,12 @@
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12038,7 +12038,7 @@
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12084,22 +12084,22 @@
     <row r="387">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E387" s="7" t="inlineStr">
@@ -12122,7 +12122,7 @@
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
@@ -12140,7 +12140,7 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -12150,7 +12150,7 @@
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Roupa de cama</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
@@ -12168,62 +12168,62 @@
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Roupa de cama</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E390" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F390" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E390" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F390" s="2" t="n"/>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E391" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F391" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E391" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F391" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
@@ -12233,12 +12233,12 @@
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12266,7 +12266,7 @@
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12289,12 +12289,12 @@
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12322,7 +12322,7 @@
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12345,12 +12345,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12373,12 +12373,12 @@
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12401,12 +12401,12 @@
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12429,12 +12429,12 @@
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12457,12 +12457,12 @@
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12485,12 +12485,12 @@
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12513,12 +12513,12 @@
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12536,17 +12536,17 @@
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12574,7 +12574,7 @@
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12602,7 +12602,7 @@
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12625,12 +12625,12 @@
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12648,22 +12648,22 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E407" s="7" t="inlineStr">
@@ -12686,7 +12686,7 @@
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12709,12 +12709,12 @@
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12742,7 +12742,7 @@
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12765,12 +12765,12 @@
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12854,7 +12854,7 @@
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12882,7 +12882,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12910,7 +12910,7 @@
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12938,7 +12938,7 @@
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12966,7 +12966,7 @@
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12994,7 +12994,7 @@
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13022,7 +13022,7 @@
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13078,7 +13078,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13096,22 +13096,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13134,7 +13134,7 @@
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13162,7 +13162,7 @@
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13190,7 +13190,7 @@
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13208,22 +13208,22 @@
     <row r="427">
       <c r="A427" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E427" s="7" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13274,7 +13274,7 @@
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13348,22 +13348,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13386,7 +13386,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13414,7 +13414,7 @@
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13442,7 +13442,7 @@
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Funko Pop Slash</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13470,7 +13470,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Funko Pop Axl Rose</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Hot Wheels – Naves Star Wars</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
@@ -13526,20 +13526,48 @@
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D438" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E438" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F438" s="2" t="n"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B439" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C439" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D438" s="2" t="inlineStr">
-        <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E438" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F438" s="2" t="n"/>
+      <c r="D439" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E439" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F439" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13578,7 +13606,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4">
@@ -13608,7 +13636,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Atualiza Caixa 302 com itens têxteis detalhados
- Manta para sofá
- Cobertor Damiola Miolo Wine (corrigido)
- Dois jogos americanos
- Manta para sofá vermelha
- Tapetes de banheiro
- Toalha de mesa
- Jogo de cama

Total: 444 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F439"/>
+  <dimension ref="A1:F445"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8335,7 +8335,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F263" s="2" t="inlineStr"/>
+      <c r="F263" s="2" t="n"/>
     </row>
     <row r="264">
       <c r="A264" s="2" t="inlineStr">
@@ -12173,12 +12173,12 @@
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Roupa de cama</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
@@ -12191,59 +12191,55 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F390" s="2" t="n"/>
+      <c r="F390" s="2" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Cobertor Damiola Miolo Wine</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E391" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F391" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E391" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F391" s="2" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E392" s="7" t="inlineStr">
@@ -12251,27 +12247,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F392" s="2" t="n"/>
+      <c r="F392" s="2" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E393" s="7" t="inlineStr">
@@ -12279,27 +12275,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F393" s="2" t="n"/>
+      <c r="F393" s="2" t="inlineStr"/>
     </row>
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E394" s="7" t="inlineStr">
@@ -12307,27 +12303,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F394" s="2" t="n"/>
+      <c r="F394" s="2" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E395" s="7" t="inlineStr">
@@ -12335,27 +12331,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F395" s="2" t="n"/>
+      <c r="F395" s="2" t="inlineStr"/>
     </row>
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E396" s="7" t="inlineStr">
@@ -12363,35 +12359,39 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F396" s="2" t="n"/>
+      <c r="F396" s="2" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E397" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F397" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E397" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F397" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
@@ -12406,7 +12406,7 @@
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12429,12 +12429,12 @@
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12457,12 +12457,12 @@
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12485,12 +12485,12 @@
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12513,12 +12513,12 @@
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12541,12 +12541,12 @@
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12564,17 +12564,17 @@
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12592,17 +12592,17 @@
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12620,17 +12620,17 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12648,7 +12648,7 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
@@ -12658,7 +12658,7 @@
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12676,22 +12676,22 @@
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E408" s="7" t="inlineStr">
@@ -12704,22 +12704,22 @@
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E409" s="7" t="inlineStr">
@@ -12732,22 +12732,22 @@
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E410" s="7" t="inlineStr">
@@ -12760,22 +12760,22 @@
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E411" s="7" t="inlineStr">
@@ -12788,22 +12788,22 @@
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E412" s="7" t="inlineStr">
@@ -12816,22 +12816,22 @@
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E413" s="7" t="inlineStr">
@@ -12854,7 +12854,7 @@
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12882,7 +12882,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12905,12 +12905,12 @@
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12933,12 +12933,12 @@
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12966,7 +12966,7 @@
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12994,7 +12994,7 @@
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13022,7 +13022,7 @@
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13078,7 +13078,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13106,7 +13106,7 @@
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13124,22 +13124,22 @@
     <row r="424">
       <c r="A424" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E424" s="7" t="inlineStr">
@@ -13152,22 +13152,22 @@
     <row r="425">
       <c r="A425" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E425" s="7" t="inlineStr">
@@ -13180,22 +13180,22 @@
     <row r="426">
       <c r="A426" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E426" s="7" t="inlineStr">
@@ -13208,22 +13208,22 @@
     <row r="427">
       <c r="A427" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E427" s="7" t="inlineStr">
@@ -13236,22 +13236,22 @@
     <row r="428">
       <c r="A428" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E428" s="7" t="inlineStr">
@@ -13264,22 +13264,22 @@
     <row r="429">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E429" s="7" t="inlineStr">
@@ -13292,22 +13292,22 @@
     <row r="430">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E430" s="7" t="inlineStr">
@@ -13320,22 +13320,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13348,22 +13348,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13376,17 +13376,17 @@
     <row r="433">
       <c r="A433" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B433" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13404,22 +13404,22 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E434" s="7" t="inlineStr">
@@ -13432,22 +13432,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13460,22 +13460,22 @@
     <row r="436">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E436" s="7" t="inlineStr">
@@ -13488,22 +13488,22 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E437" s="7" t="inlineStr">
@@ -13516,22 +13516,22 @@
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E438" s="7" t="inlineStr">
@@ -13554,20 +13554,188 @@
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
+          <t>BrickHeadz Aragorn</t>
+        </is>
+      </c>
+      <c r="D439" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E439" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F439" s="2" t="n"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B440" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C440" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Arwen Undómiel</t>
+        </is>
+      </c>
+      <c r="D440" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E440" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F440" s="2" t="n"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B441" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C441" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D441" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E441" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F441" s="2" t="n"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B442" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C442" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D442" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E442" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F442" s="2" t="n"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B443" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C443" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D443" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E443" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F443" s="2" t="n"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B444" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C444" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D444" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E444" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F444" s="2" t="n"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B445" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C445" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D439" s="2" t="inlineStr">
-        <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E439" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F439" s="2" t="n"/>
+      <c r="D445" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E445" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F445" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13606,7 +13774,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4">
@@ -13636,7 +13804,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Adiciona Caixa 41 com organizadores
- 2 itens de organização
- Total: 446 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F445"/>
+  <dimension ref="A1:F447"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10752,22 +10752,22 @@
     <row r="340">
       <c r="A340" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 41</t>
         </is>
       </c>
       <c r="B340" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C340" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Organizadores de acrílico</t>
         </is>
       </c>
       <c r="D340" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E340" s="7" t="inlineStr">
@@ -10775,27 +10775,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F340" s="2" t="n"/>
+      <c r="F340" s="2" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 41</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C341" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Outros organizadores (diversos)</t>
         </is>
       </c>
       <c r="D341" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E341" s="7" t="inlineStr">
@@ -10803,7 +10803,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F341" s="2" t="n"/>
+      <c r="F341" s="2" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" s="2" t="inlineStr">
@@ -10813,12 +10813,12 @@
       </c>
       <c r="B342" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C342" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D342" s="2" t="inlineStr">
@@ -10841,12 +10841,12 @@
       </c>
       <c r="B343" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C343" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr">
@@ -10869,12 +10869,12 @@
       </c>
       <c r="B344" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C344" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D344" s="2" t="inlineStr">
@@ -10902,7 +10902,7 @@
       </c>
       <c r="C345" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D345" s="2" t="inlineStr">
@@ -10925,12 +10925,12 @@
       </c>
       <c r="B346" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C346" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D346" s="2" t="inlineStr">
@@ -10953,12 +10953,12 @@
       </c>
       <c r="B347" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C347" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D347" s="2" t="inlineStr">
@@ -10976,22 +10976,22 @@
     <row r="348">
       <c r="A348" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B348" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C348" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D348" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E348" s="7" t="inlineStr">
@@ -11004,22 +11004,22 @@
     <row r="349">
       <c r="A349" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B349" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C349" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D349" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E349" s="7" t="inlineStr">
@@ -11042,7 +11042,7 @@
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
@@ -11098,7 +11098,7 @@
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
@@ -11116,22 +11116,22 @@
     <row r="353">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E353" s="7" t="inlineStr">
@@ -11144,22 +11144,22 @@
     <row r="354">
       <c r="A354" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B354" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E354" s="7" t="inlineStr">
@@ -11177,12 +11177,12 @@
       </c>
       <c r="B355" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11195,11 +11195,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F355" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F355" s="2" t="n"/>
     </row>
     <row r="356">
       <c r="A356" s="2" t="inlineStr">
@@ -11209,12 +11205,12 @@
       </c>
       <c r="B356" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11227,11 +11223,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F356" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F356" s="2" t="n"/>
     </row>
     <row r="357">
       <c r="A357" s="2" t="inlineStr">
@@ -11246,7 +11238,7 @@
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11273,12 +11265,12 @@
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
@@ -11291,7 +11283,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F358" s="2" t="n"/>
+      <c r="F358" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
@@ -11306,7 +11302,7 @@
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
@@ -11333,12 +11329,12 @@
       </c>
       <c r="B360" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
@@ -11361,12 +11357,12 @@
       </c>
       <c r="B361" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
@@ -11379,7 +11375,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F361" s="2" t="n"/>
+      <c r="F361" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="2" t="inlineStr">
@@ -11389,12 +11389,12 @@
       </c>
       <c r="B362" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
@@ -11417,12 +11417,12 @@
       </c>
       <c r="B363" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
@@ -11450,7 +11450,7 @@
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
@@ -11478,7 +11478,7 @@
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11506,7 +11506,7 @@
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11534,7 +11534,7 @@
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
@@ -11562,7 +11562,7 @@
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
@@ -11580,22 +11580,22 @@
     <row r="369">
       <c r="A369" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E369" s="7" t="inlineStr">
@@ -11608,22 +11608,22 @@
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E370" s="7" t="inlineStr">
@@ -11641,12 +11641,12 @@
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11669,12 +11669,12 @@
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
@@ -11697,12 +11697,12 @@
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
@@ -11720,22 +11720,22 @@
     <row r="374">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E374" s="7" t="inlineStr">
@@ -11748,22 +11748,22 @@
     <row r="375">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E375" s="7" t="inlineStr">
@@ -11786,7 +11786,7 @@
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11814,7 +11814,7 @@
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11837,12 +11837,12 @@
       </c>
       <c r="B378" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
@@ -11865,12 +11865,12 @@
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
@@ -11893,12 +11893,12 @@
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
@@ -11921,12 +11921,12 @@
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
@@ -11977,12 +11977,12 @@
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -12005,12 +12005,12 @@
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12033,12 +12033,12 @@
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12061,12 +12061,12 @@
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12094,7 +12094,7 @@
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12112,22 +12112,22 @@
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E388" s="7" t="inlineStr">
@@ -12140,22 +12140,22 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E389" s="7" t="inlineStr">
@@ -12168,17 +12168,17 @@
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
@@ -12191,22 +12191,22 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F390" s="2" t="inlineStr"/>
+      <c r="F390" s="2" t="n"/>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
@@ -12219,7 +12219,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F391" s="2" t="inlineStr"/>
+      <c r="F391" s="2" t="n"/>
     </row>
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
@@ -12229,12 +12229,12 @@
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12247,7 +12247,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F392" s="2" t="inlineStr"/>
+      <c r="F392" s="2" t="n"/>
     </row>
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
@@ -12262,7 +12262,7 @@
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12275,7 +12275,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F393" s="2" t="inlineStr"/>
+      <c r="F393" s="2" t="n"/>
     </row>
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
@@ -12285,12 +12285,12 @@
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12303,7 +12303,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F394" s="2" t="inlineStr"/>
+      <c r="F394" s="2" t="n"/>
     </row>
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
@@ -12313,12 +12313,12 @@
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12331,7 +12331,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F395" s="2" t="inlineStr"/>
+      <c r="F395" s="2" t="n"/>
     </row>
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
@@ -12341,12 +12341,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12359,59 +12359,55 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F396" s="2" t="inlineStr"/>
+      <c r="F396" s="2" t="n"/>
     </row>
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E397" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F397" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E397" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F397" s="2" t="n"/>
     </row>
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E398" s="7" t="inlineStr">
@@ -12424,30 +12420,34 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E399" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F399" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E399" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F399" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
@@ -12457,12 +12457,12 @@
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12485,12 +12485,12 @@
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12513,12 +12513,12 @@
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12541,12 +12541,12 @@
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12574,7 +12574,7 @@
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12597,12 +12597,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12630,7 +12630,7 @@
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12658,7 +12658,7 @@
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12681,12 +12681,12 @@
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12709,12 +12709,12 @@
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12732,17 +12732,17 @@
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12760,17 +12760,17 @@
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12821,12 +12821,12 @@
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12844,22 +12844,22 @@
     <row r="414">
       <c r="A414" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E414" s="7" t="inlineStr">
@@ -12872,22 +12872,22 @@
     <row r="415">
       <c r="A415" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E415" s="7" t="inlineStr">
@@ -12905,12 +12905,12 @@
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12933,12 +12933,12 @@
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12961,12 +12961,12 @@
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12989,12 +12989,12 @@
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13022,7 +13022,7 @@
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13078,7 +13078,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13106,7 +13106,7 @@
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13134,7 +13134,7 @@
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13162,7 +13162,7 @@
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13190,7 +13190,7 @@
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13218,7 +13218,7 @@
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13274,7 +13274,7 @@
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13292,22 +13292,22 @@
     <row r="430">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E430" s="7" t="inlineStr">
@@ -13320,22 +13320,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13358,7 +13358,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13386,7 +13386,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13404,22 +13404,22 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E434" s="7" t="inlineStr">
@@ -13432,22 +13432,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13470,7 +13470,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
@@ -13526,7 +13526,7 @@
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
@@ -13544,22 +13544,22 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E439" s="7" t="inlineStr">
@@ -13572,22 +13572,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13666,7 +13666,7 @@
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Funko Pop Slash</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Funko Pop Axl Rose</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
@@ -13722,20 +13722,76 @@
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D445" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E445" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F445" s="2" t="n"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B446" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C446" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D446" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E446" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F446" s="2" t="n"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B447" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C447" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D445" s="2" t="inlineStr">
-        <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E445" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F445" s="2" t="n"/>
+      <c r="D447" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E447" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F447" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13774,7 +13830,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4">
@@ -13804,7 +13860,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Adiciona Caixa 42 com roupas íntimas
- 8 itens de lingerie, biquínis e meias
- Prioridade Alta
- Total: 454 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F447"/>
+  <dimension ref="A1:F455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10775,7 +10775,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F340" s="2" t="inlineStr"/>
+      <c r="F340" s="2" t="n"/>
     </row>
     <row r="341">
       <c r="A341" s="2" t="inlineStr">
@@ -10803,251 +10803,251 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F341" s="2" t="inlineStr"/>
+      <c r="F341" s="2" t="n"/>
     </row>
     <row r="342">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C342" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Lingeries elaboradas</t>
         </is>
       </c>
       <c r="D342" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E342" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F342" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E342" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F342" s="2" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C343" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Lingeries simples</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E343" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F343" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E343" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F343" s="2" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C344" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Calcinhas para período menstrual</t>
         </is>
       </c>
       <c r="D344" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E344" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F344" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E344" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F344" s="2" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C345" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Cinta-liga</t>
         </is>
       </c>
       <c r="D345" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E345" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F345" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E345" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F345" s="2" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C346" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Meia-calça</t>
         </is>
       </c>
       <c r="D346" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E346" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F346" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E346" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F346" s="2" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C347" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Biquínis</t>
         </is>
       </c>
       <c r="D347" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E347" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F347" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E347" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F347" s="2" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B348" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C348" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Maiôs</t>
         </is>
       </c>
       <c r="D348" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E348" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F348" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E348" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F348" s="2" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B349" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Roupa íntima</t>
         </is>
       </c>
       <c r="C349" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Meias</t>
         </is>
       </c>
       <c r="D349" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E349" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F349" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E349" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F349" s="2" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B350" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E350" s="7" t="inlineStr">
@@ -11060,22 +11060,22 @@
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E351" s="7" t="inlineStr">
@@ -11088,22 +11088,22 @@
     <row r="352">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E352" s="7" t="inlineStr">
@@ -11116,22 +11116,22 @@
     <row r="353">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E353" s="7" t="inlineStr">
@@ -11144,22 +11144,22 @@
     <row r="354">
       <c r="A354" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B354" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E354" s="7" t="inlineStr">
@@ -11172,17 +11172,17 @@
     <row r="355">
       <c r="A355" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B355" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11200,17 +11200,17 @@
     <row r="356">
       <c r="A356" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B356" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11228,17 +11228,17 @@
     <row r="357">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11251,31 +11251,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F357" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F357" s="2" t="n"/>
     </row>
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E358" s="7" t="inlineStr">
@@ -11283,31 +11279,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F358" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F358" s="2" t="n"/>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B359" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E359" s="7" t="inlineStr">
@@ -11315,31 +11307,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F359" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F359" s="2" t="n"/>
     </row>
     <row r="360">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E360" s="7" t="inlineStr">
@@ -11352,22 +11340,22 @@
     <row r="361">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E361" s="7" t="inlineStr">
@@ -11375,31 +11363,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F361" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F361" s="2" t="n"/>
     </row>
     <row r="362">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E362" s="7" t="inlineStr">
@@ -11422,7 +11406,7 @@
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
@@ -11445,12 +11429,12 @@
       </c>
       <c r="B364" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
@@ -11473,12 +11457,12 @@
       </c>
       <c r="B365" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11491,7 +11475,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F365" s="2" t="n"/>
+      <c r="F365" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="2" t="inlineStr">
@@ -11501,12 +11489,12 @@
       </c>
       <c r="B366" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11519,7 +11507,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F366" s="2" t="n"/>
+      <c r="F366" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="2" t="inlineStr">
@@ -11529,12 +11521,12 @@
       </c>
       <c r="B367" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
@@ -11547,7 +11539,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F367" s="2" t="n"/>
+      <c r="F367" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="2" t="inlineStr">
@@ -11562,7 +11558,7 @@
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
@@ -11585,12 +11581,12 @@
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
@@ -11603,7 +11599,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F369" s="2" t="n"/>
+      <c r="F369" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
@@ -11613,12 +11613,12 @@
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11636,22 +11636,22 @@
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E371" s="7" t="inlineStr">
@@ -11664,22 +11664,22 @@
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E372" s="7" t="inlineStr">
@@ -11692,22 +11692,22 @@
     <row r="373">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E373" s="7" t="inlineStr">
@@ -11720,22 +11720,22 @@
     <row r="374">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E374" s="7" t="inlineStr">
@@ -11748,22 +11748,22 @@
     <row r="375">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E375" s="7" t="inlineStr">
@@ -11776,22 +11776,22 @@
     <row r="376">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E376" s="7" t="inlineStr">
@@ -11804,22 +11804,22 @@
     <row r="377">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E377" s="7" t="inlineStr">
@@ -11832,22 +11832,22 @@
     <row r="378">
       <c r="A378" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B378" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E378" s="7" t="inlineStr">
@@ -11860,22 +11860,22 @@
     <row r="379">
       <c r="A379" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E379" s="7" t="inlineStr">
@@ -11888,22 +11888,22 @@
     <row r="380">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E380" s="7" t="inlineStr">
@@ -11916,22 +11916,22 @@
     <row r="381">
       <c r="A381" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E381" s="7" t="inlineStr">
@@ -11944,22 +11944,22 @@
     <row r="382">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E382" s="7" t="inlineStr">
@@ -11972,22 +11972,22 @@
     <row r="383">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E383" s="7" t="inlineStr">
@@ -12010,7 +12010,7 @@
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12033,12 +12033,12 @@
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12061,12 +12061,12 @@
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12094,7 +12094,7 @@
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12117,12 +12117,12 @@
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
@@ -12145,12 +12145,12 @@
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
@@ -12168,22 +12168,22 @@
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E390" s="7" t="inlineStr">
@@ -12196,22 +12196,22 @@
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E391" s="7" t="inlineStr">
@@ -12224,22 +12224,22 @@
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E392" s="7" t="inlineStr">
@@ -12252,22 +12252,22 @@
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E393" s="7" t="inlineStr">
@@ -12280,22 +12280,22 @@
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E394" s="7" t="inlineStr">
@@ -12308,22 +12308,22 @@
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E395" s="7" t="inlineStr">
@@ -12336,22 +12336,22 @@
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E396" s="7" t="inlineStr">
@@ -12364,22 +12364,22 @@
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E397" s="7" t="inlineStr">
@@ -12392,17 +12392,17 @@
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12420,54 +12420,50 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E399" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F399" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E399" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F399" s="2" t="n"/>
     </row>
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E400" s="7" t="inlineStr">
@@ -12480,22 +12476,22 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E401" s="7" t="inlineStr">
@@ -12508,22 +12504,22 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E402" s="7" t="inlineStr">
@@ -12536,22 +12532,22 @@
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E403" s="7" t="inlineStr">
@@ -12564,22 +12560,22 @@
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E404" s="7" t="inlineStr">
@@ -12592,22 +12588,22 @@
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E405" s="7" t="inlineStr">
@@ -12620,22 +12616,22 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E406" s="7" t="inlineStr">
@@ -12648,30 +12644,34 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E407" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F407" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E407" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F407" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
@@ -12686,7 +12686,7 @@
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12709,12 +12709,12 @@
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12742,7 +12742,7 @@
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12770,7 +12770,7 @@
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12788,17 +12788,17 @@
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12816,17 +12816,17 @@
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12844,17 +12844,17 @@
     <row r="414">
       <c r="A414" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12872,7 +12872,7 @@
     <row r="415">
       <c r="A415" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B415" s="2" t="inlineStr">
@@ -12882,7 +12882,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12900,22 +12900,22 @@
     <row r="416">
       <c r="A416" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E416" s="7" t="inlineStr">
@@ -12928,22 +12928,22 @@
     <row r="417">
       <c r="A417" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E417" s="7" t="inlineStr">
@@ -12956,22 +12956,22 @@
     <row r="418">
       <c r="A418" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E418" s="7" t="inlineStr">
@@ -12984,22 +12984,22 @@
     <row r="419">
       <c r="A419" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E419" s="7" t="inlineStr">
@@ -13012,22 +13012,22 @@
     <row r="420">
       <c r="A420" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E420" s="7" t="inlineStr">
@@ -13040,22 +13040,22 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E421" s="7" t="inlineStr">
@@ -13068,22 +13068,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13096,22 +13096,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13134,7 +13134,7 @@
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13162,7 +13162,7 @@
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13185,12 +13185,12 @@
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13213,12 +13213,12 @@
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13274,7 +13274,7 @@
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13348,22 +13348,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13376,22 +13376,22 @@
     <row r="433">
       <c r="A433" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B433" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E433" s="7" t="inlineStr">
@@ -13404,22 +13404,22 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E434" s="7" t="inlineStr">
@@ -13432,22 +13432,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13460,22 +13460,22 @@
     <row r="436">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E436" s="7" t="inlineStr">
@@ -13488,22 +13488,22 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E437" s="7" t="inlineStr">
@@ -13516,22 +13516,22 @@
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E438" s="7" t="inlineStr">
@@ -13544,22 +13544,22 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E439" s="7" t="inlineStr">
@@ -13572,22 +13572,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13600,17 +13600,17 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
@@ -13628,17 +13628,17 @@
     <row r="442">
       <c r="A442" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B442" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13656,17 +13656,17 @@
     <row r="443">
       <c r="A443" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13684,22 +13684,22 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E444" s="7" t="inlineStr">
@@ -13712,22 +13712,22 @@
     <row r="445">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E445" s="7" t="inlineStr">
@@ -13740,22 +13740,22 @@
     <row r="446">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E446" s="7" t="inlineStr">
@@ -13768,30 +13768,254 @@
     <row r="447">
       <c r="A447" s="2" t="inlineStr">
         <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B447" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C447" s="2" t="inlineStr">
+        <is>
+          <t>Ralo click</t>
+        </is>
+      </c>
+      <c r="D447" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E447" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F447" s="2" t="n"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B448" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C448" s="2" t="inlineStr">
+        <is>
+          <t>Escova de limpeza elétrica</t>
+        </is>
+      </c>
+      <c r="D448" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E448" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F448" s="2" t="n"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="2" t="inlineStr">
+        <is>
           <t>Caixa 29501</t>
         </is>
       </c>
-      <c r="B447" s="2" t="inlineStr">
+      <c r="B449" s="2" t="inlineStr">
         <is>
           <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
-      <c r="C447" s="2" t="inlineStr">
+      <c r="C449" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Aragorn</t>
+        </is>
+      </c>
+      <c r="D449" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E449" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F449" s="2" t="n"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B450" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C450" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Arwen Undómiel</t>
+        </is>
+      </c>
+      <c r="D450" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E450" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F450" s="2" t="n"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B451" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C451" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D451" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E451" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F451" s="2" t="n"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B452" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C452" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D452" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E452" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F452" s="2" t="n"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B453" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C453" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D453" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E453" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F453" s="2" t="n"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B454" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C454" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D454" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E454" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F454" s="2" t="n"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B455" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C455" s="2" t="inlineStr">
         <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D447" s="2" t="inlineStr">
+      <c r="D455" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E447" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F447" s="2" t="n"/>
+      <c r="E455" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F455" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13830,7 +14054,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4">
@@ -13850,7 +14074,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixa 43 com cabides
- Prioridade Baixa
- Total: 455 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F455"/>
+  <dimension ref="A1:F456"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10831,7 +10831,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F342" s="2" t="inlineStr"/>
+      <c r="F342" s="2" t="n"/>
     </row>
     <row r="343">
       <c r="A343" s="2" t="inlineStr">
@@ -10859,7 +10859,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F343" s="2" t="inlineStr"/>
+      <c r="F343" s="2" t="n"/>
     </row>
     <row r="344">
       <c r="A344" s="2" t="inlineStr">
@@ -10887,7 +10887,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F344" s="2" t="inlineStr"/>
+      <c r="F344" s="2" t="n"/>
     </row>
     <row r="345">
       <c r="A345" s="2" t="inlineStr">
@@ -10915,7 +10915,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F345" s="2" t="inlineStr"/>
+      <c r="F345" s="2" t="n"/>
     </row>
     <row r="346">
       <c r="A346" s="2" t="inlineStr">
@@ -10943,7 +10943,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F346" s="2" t="inlineStr"/>
+      <c r="F346" s="2" t="n"/>
     </row>
     <row r="347">
       <c r="A347" s="2" t="inlineStr">
@@ -10971,7 +10971,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F347" s="2" t="inlineStr"/>
+      <c r="F347" s="2" t="n"/>
     </row>
     <row r="348">
       <c r="A348" s="2" t="inlineStr">
@@ -10999,7 +10999,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F348" s="2" t="inlineStr"/>
+      <c r="F348" s="2" t="n"/>
     </row>
     <row r="349">
       <c r="A349" s="2" t="inlineStr">
@@ -11027,35 +11027,35 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F349" s="2" t="inlineStr"/>
+      <c r="F349" s="2" t="n"/>
     </row>
     <row r="350">
       <c r="A350" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 43</t>
         </is>
       </c>
       <c r="B350" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Cabides</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E350" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F350" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E350" s="6" t="inlineStr">
+        <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="F350" s="2" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
@@ -11093,12 +11093,12 @@
       </c>
       <c r="B352" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
@@ -11149,12 +11149,12 @@
       </c>
       <c r="B354" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
@@ -11177,12 +11177,12 @@
       </c>
       <c r="B355" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11210,7 +11210,7 @@
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11233,12 +11233,12 @@
       </c>
       <c r="B357" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11256,22 +11256,22 @@
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E358" s="7" t="inlineStr">
@@ -11294,7 +11294,7 @@
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
@@ -11322,7 +11322,7 @@
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
@@ -11350,7 +11350,7 @@
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
@@ -11378,7 +11378,7 @@
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
@@ -11396,22 +11396,22 @@
     <row r="363">
       <c r="A363" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B363" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E363" s="7" t="inlineStr">
@@ -11434,7 +11434,7 @@
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
@@ -11457,12 +11457,12 @@
       </c>
       <c r="B365" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11475,11 +11475,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F365" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F365" s="2" t="n"/>
     </row>
     <row r="366">
       <c r="A366" s="2" t="inlineStr">
@@ -11494,7 +11490,7 @@
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11526,7 +11522,7 @@
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
@@ -11553,12 +11549,12 @@
       </c>
       <c r="B368" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
@@ -11571,7 +11567,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F368" s="2" t="n"/>
+      <c r="F368" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="2" t="inlineStr">
@@ -11581,12 +11581,12 @@
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
@@ -11599,11 +11599,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F369" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F369" s="2" t="n"/>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
@@ -11613,12 +11609,12 @@
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11631,7 +11627,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F370" s="2" t="n"/>
+      <c r="F370" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
@@ -11646,7 +11646,7 @@
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11669,12 +11669,12 @@
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
@@ -11702,7 +11702,7 @@
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
@@ -11730,7 +11730,7 @@
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
@@ -11758,7 +11758,7 @@
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
@@ -11786,7 +11786,7 @@
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11814,7 +11814,7 @@
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11842,7 +11842,7 @@
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
@@ -11860,22 +11860,22 @@
     <row r="379">
       <c r="A379" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E379" s="7" t="inlineStr">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
@@ -11921,12 +11921,12 @@
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
@@ -11949,12 +11949,12 @@
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
@@ -11977,12 +11977,12 @@
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -12000,22 +12000,22 @@
     <row r="384">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E384" s="7" t="inlineStr">
@@ -12038,7 +12038,7 @@
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12094,7 +12094,7 @@
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12117,12 +12117,12 @@
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
@@ -12150,7 +12150,7 @@
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
@@ -12173,12 +12173,12 @@
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
@@ -12206,7 +12206,7 @@
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
@@ -12234,7 +12234,7 @@
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12257,12 +12257,12 @@
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12290,7 +12290,7 @@
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12313,12 +12313,12 @@
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12346,7 +12346,7 @@
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12374,7 +12374,7 @@
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12392,22 +12392,22 @@
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E398" s="7" t="inlineStr">
@@ -12430,7 +12430,7 @@
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12448,17 +12448,17 @@
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12486,7 +12486,7 @@
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12509,12 +12509,12 @@
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12537,12 +12537,12 @@
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12565,12 +12565,12 @@
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12593,12 +12593,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12621,12 +12621,12 @@
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12644,62 +12644,62 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E407" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F407" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E407" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F407" s="2" t="n"/>
     </row>
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E408" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F408" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E408" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F408" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
@@ -12709,12 +12709,12 @@
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12742,7 +12742,7 @@
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12765,12 +12765,12 @@
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12821,12 +12821,12 @@
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12849,12 +12849,12 @@
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12877,12 +12877,12 @@
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12905,12 +12905,12 @@
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12933,12 +12933,12 @@
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12961,12 +12961,12 @@
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12989,12 +12989,12 @@
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13012,17 +13012,17 @@
     <row r="420">
       <c r="A420" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13078,7 +13078,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13101,12 +13101,12 @@
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13124,22 +13124,22 @@
     <row r="424">
       <c r="A424" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E424" s="7" t="inlineStr">
@@ -13162,7 +13162,7 @@
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13185,12 +13185,12 @@
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13218,7 +13218,7 @@
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13241,12 +13241,12 @@
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13274,7 +13274,7 @@
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13358,7 +13358,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13386,7 +13386,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13414,7 +13414,7 @@
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13442,7 +13442,7 @@
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13470,7 +13470,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
@@ -13526,7 +13526,7 @@
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
@@ -13554,7 +13554,7 @@
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
@@ -13572,22 +13572,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13666,7 +13666,7 @@
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13684,22 +13684,22 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E444" s="7" t="inlineStr">
@@ -13722,7 +13722,7 @@
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
@@ -13750,7 +13750,7 @@
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
@@ -13778,7 +13778,7 @@
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
@@ -13806,7 +13806,7 @@
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
@@ -13824,22 +13824,22 @@
     <row r="449">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E449" s="7" t="inlineStr">
@@ -13862,7 +13862,7 @@
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
@@ -13890,7 +13890,7 @@
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
@@ -13918,7 +13918,7 @@
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Funko Pop Slash</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Funko Pop Axl Rose</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
@@ -13974,7 +13974,7 @@
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Hot Wheels – Naves Star Wars</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
@@ -14002,20 +14002,48 @@
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D455" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E455" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F455" s="2" t="n"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B456" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C456" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D455" s="2" t="inlineStr">
+      <c r="D456" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E455" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F455" s="2" t="n"/>
+      <c r="E456" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F456" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14054,7 +14082,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4">
@@ -14094,7 +14122,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Adiciona bijuterias na Caixa 42
- Total: 456 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F456"/>
+  <dimension ref="A1:F457"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11032,17 +11032,17 @@
     <row r="350">
       <c r="A350" s="2" t="inlineStr">
         <is>
-          <t>Caixa 43</t>
+          <t>Caixa 42</t>
         </is>
       </c>
       <c r="B350" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>Cabides</t>
+          <t>Bijuterias</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr">
@@ -11050,9 +11050,9 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E350" s="6" t="inlineStr">
-        <is>
-          <t>Baixa</t>
+      <c r="E350" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F350" s="2" t="inlineStr"/>
@@ -11060,27 +11060,27 @@
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 43</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Cabides</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E351" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E351" s="6" t="inlineStr">
+        <is>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="F351" s="2" t="n"/>
@@ -11098,7 +11098,7 @@
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
@@ -11121,12 +11121,12 @@
       </c>
       <c r="B353" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
@@ -11154,7 +11154,7 @@
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
@@ -11177,12 +11177,12 @@
       </c>
       <c r="B355" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
@@ -11205,12 +11205,12 @@
       </c>
       <c r="B356" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
@@ -11238,7 +11238,7 @@
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
@@ -11261,12 +11261,12 @@
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
@@ -11284,22 +11284,22 @@
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B359" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E359" s="7" t="inlineStr">
@@ -11322,7 +11322,7 @@
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
@@ -11350,7 +11350,7 @@
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
@@ -11378,7 +11378,7 @@
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
@@ -11424,22 +11424,22 @@
     <row r="364">
       <c r="A364" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B364" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E364" s="7" t="inlineStr">
@@ -11462,7 +11462,7 @@
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
@@ -11485,12 +11485,12 @@
       </c>
       <c r="B366" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
@@ -11503,11 +11503,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F366" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F366" s="2" t="n"/>
     </row>
     <row r="367">
       <c r="A367" s="2" t="inlineStr">
@@ -11522,7 +11518,7 @@
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
@@ -11554,7 +11550,7 @@
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
@@ -11581,12 +11577,12 @@
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
@@ -11599,7 +11595,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F369" s="2" t="n"/>
+      <c r="F369" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
@@ -11609,12 +11609,12 @@
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11627,11 +11627,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F370" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F370" s="2" t="n"/>
     </row>
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
@@ -11641,12 +11637,12 @@
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11659,7 +11655,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F371" s="2" t="n"/>
+      <c r="F371" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
@@ -11674,7 +11674,7 @@
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
@@ -11697,12 +11697,12 @@
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
@@ -11730,7 +11730,7 @@
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
@@ -11758,7 +11758,7 @@
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
@@ -11786,7 +11786,7 @@
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11814,7 +11814,7 @@
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11842,7 +11842,7 @@
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
@@ -11870,7 +11870,7 @@
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
@@ -11888,22 +11888,22 @@
     <row r="380">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E380" s="7" t="inlineStr">
@@ -11926,7 +11926,7 @@
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
@@ -11949,12 +11949,12 @@
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
@@ -11977,12 +11977,12 @@
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -12005,12 +12005,12 @@
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12028,22 +12028,22 @@
     <row r="385">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E385" s="7" t="inlineStr">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12094,7 +12094,7 @@
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12122,7 +12122,7 @@
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
@@ -12145,12 +12145,12 @@
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
@@ -12178,7 +12178,7 @@
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
@@ -12201,12 +12201,12 @@
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
@@ -12234,7 +12234,7 @@
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12262,7 +12262,7 @@
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12285,12 +12285,12 @@
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12318,7 +12318,7 @@
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12341,12 +12341,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12374,7 +12374,7 @@
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12402,7 +12402,7 @@
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12420,22 +12420,22 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E399" s="7" t="inlineStr">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12476,17 +12476,17 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12514,7 +12514,7 @@
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12537,12 +12537,12 @@
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12565,12 +12565,12 @@
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12593,12 +12593,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12621,12 +12621,12 @@
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12649,12 +12649,12 @@
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12672,62 +12672,62 @@
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E408" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F408" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E408" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F408" s="2" t="n"/>
     </row>
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E409" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F409" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E409" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F409" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
@@ -12737,12 +12737,12 @@
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12770,7 +12770,7 @@
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12793,12 +12793,12 @@
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12849,12 +12849,12 @@
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12877,12 +12877,12 @@
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12905,12 +12905,12 @@
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12933,12 +12933,12 @@
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12961,12 +12961,12 @@
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12989,12 +12989,12 @@
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13017,12 +13017,12 @@
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13040,17 +13040,17 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13078,7 +13078,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13106,7 +13106,7 @@
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13129,12 +13129,12 @@
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13152,22 +13152,22 @@
     <row r="425">
       <c r="A425" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E425" s="7" t="inlineStr">
@@ -13190,7 +13190,7 @@
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13213,12 +13213,12 @@
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13269,12 +13269,12 @@
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13358,7 +13358,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13386,7 +13386,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13414,7 +13414,7 @@
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13442,7 +13442,7 @@
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13470,7 +13470,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
@@ -13526,7 +13526,7 @@
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
@@ -13554,7 +13554,7 @@
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
@@ -13582,7 +13582,7 @@
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
@@ -13600,22 +13600,22 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E441" s="7" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13666,7 +13666,7 @@
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
@@ -13712,22 +13712,22 @@
     <row r="445">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E445" s="7" t="inlineStr">
@@ -13750,7 +13750,7 @@
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
@@ -13778,7 +13778,7 @@
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
@@ -13806,7 +13806,7 @@
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
@@ -13852,22 +13852,22 @@
     <row r="450">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E450" s="7" t="inlineStr">
@@ -13890,7 +13890,7 @@
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
@@ -13918,7 +13918,7 @@
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Funko Pop Slash</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
@@ -13974,7 +13974,7 @@
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Funko Pop Axl Rose</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
@@ -14002,7 +14002,7 @@
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Hot Wheels – Naves Star Wars</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
@@ -14030,20 +14030,48 @@
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D456" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E456" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F456" s="2" t="n"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B457" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C457" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D456" s="2" t="inlineStr">
+      <c r="D457" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E456" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F456" s="2" t="n"/>
+      <c r="E457" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F457" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14082,7 +14110,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4">
@@ -14102,7 +14130,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixas 44 e 45 com calçados
Caixa 44 (8 itens):
- Sandálias elegantes, botas, Melissa

Caixa 45 (10 itens):
- Tênis esportivos (CrossFit, corrida, basquete)
- Bota de trilha Columbia
- Tênis Mulher-Maravilha

Total: 474 itens (123 de Alta prioridade)
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F457"/>
+  <dimension ref="A1:F475"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11055,7 +11055,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F350" s="2" t="inlineStr"/>
+      <c r="F350" s="2" t="n"/>
     </row>
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
@@ -11088,533 +11088,521 @@
     <row r="352">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Sandália preta elegante</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E352" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F352" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E352" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F352" s="2" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Sapato de salto nude</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E353" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F353" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E353" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F353" s="2" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B354" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Sandália usada no casamento do Nick da Amanda</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E354" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F354" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E354" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F354" s="2" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B355" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Sandália preta de salto altíssimo</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E355" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F355" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E355" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F355" s="2" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B356" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Bota de cano curto</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E356" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F356" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E356" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F356" s="2" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Bota de cano longo</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E357" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F357" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E357" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F357" s="2" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Sandália preta da Melissa</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E358" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F358" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E358" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F358" s="2" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 44</t>
         </is>
       </c>
       <c r="B359" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Sandália marrom da Melissa</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E359" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F359" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E359" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F359" s="2" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Lifter para LPO</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E360" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F360" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E360" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F360" s="2" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Bota de trilha da Columbia</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E361" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F361" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E361" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F361" s="2" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Tênis Metcon 6 (CrossFit)</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E362" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F362" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E362" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F362" s="2" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B363" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Tênis de basquete feminino</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E363" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F363" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E363" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F363" s="2" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B364" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Tênis Nano 12 Mulher-Maravilha</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E364" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F364" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E364" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F364" s="2" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B365" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Tênis Metcon rosa com branco (modelo recente)</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E365" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F365" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E365" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F365" s="2" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Tênis Adidas Dome</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E366" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F366" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E366" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F366" s="2" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Tênis Corremax da Olympikus</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E367" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F367" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E367" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F367" s="2" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B368" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Chinelo branco da Olympikus</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E368" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F368" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E368" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F368" s="2" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 45</t>
         </is>
       </c>
       <c r="B369" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Sapatilha de neoprene</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E369" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F369" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E369" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F369" s="2" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
@@ -11632,17 +11620,17 @@
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
@@ -11655,26 +11643,22 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F371" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F371" s="2" t="n"/>
     </row>
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
@@ -11692,17 +11676,17 @@
     <row r="373">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
@@ -11720,17 +11704,17 @@
     <row r="374">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
@@ -11748,17 +11732,17 @@
     <row r="375">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
@@ -11776,17 +11760,17 @@
     <row r="376">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
@@ -11804,17 +11788,17 @@
     <row r="377">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
@@ -11832,22 +11816,22 @@
     <row r="378">
       <c r="A378" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B378" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E378" s="7" t="inlineStr">
@@ -11860,22 +11844,22 @@
     <row r="379">
       <c r="A379" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E379" s="7" t="inlineStr">
@@ -11888,22 +11872,22 @@
     <row r="380">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E380" s="7" t="inlineStr">
@@ -11916,22 +11900,22 @@
     <row r="381">
       <c r="A381" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E381" s="7" t="inlineStr">
@@ -11944,22 +11928,22 @@
     <row r="382">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E382" s="7" t="inlineStr">
@@ -11972,22 +11956,22 @@
     <row r="383">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E383" s="7" t="inlineStr">
@@ -12000,22 +11984,22 @@
     <row r="384">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E384" s="7" t="inlineStr">
@@ -12028,22 +12012,22 @@
     <row r="385">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E385" s="7" t="inlineStr">
@@ -12051,27 +12035,31 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F385" s="2" t="n"/>
+      <c r="F385" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E386" s="7" t="inlineStr">
@@ -12079,27 +12067,31 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F386" s="2" t="n"/>
+      <c r="F386" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="387">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E387" s="7" t="inlineStr">
@@ -12107,27 +12099,31 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F387" s="2" t="n"/>
+      <c r="F387" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E388" s="7" t="inlineStr">
@@ -12140,22 +12136,22 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E389" s="7" t="inlineStr">
@@ -12163,27 +12159,31 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F389" s="2" t="n"/>
+      <c r="F389" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E390" s="7" t="inlineStr">
@@ -12196,22 +12196,22 @@
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E391" s="7" t="inlineStr">
@@ -12224,22 +12224,22 @@
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E392" s="7" t="inlineStr">
@@ -12252,22 +12252,22 @@
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E393" s="7" t="inlineStr">
@@ -12280,22 +12280,22 @@
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E394" s="7" t="inlineStr">
@@ -12308,22 +12308,22 @@
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E395" s="7" t="inlineStr">
@@ -12336,22 +12336,22 @@
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E396" s="7" t="inlineStr">
@@ -12364,22 +12364,22 @@
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E397" s="7" t="inlineStr">
@@ -12392,22 +12392,22 @@
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E398" s="7" t="inlineStr">
@@ -12420,22 +12420,22 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E399" s="7" t="inlineStr">
@@ -12448,22 +12448,22 @@
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E400" s="7" t="inlineStr">
@@ -12476,22 +12476,22 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E401" s="7" t="inlineStr">
@@ -12504,22 +12504,22 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E402" s="7" t="inlineStr">
@@ -12532,22 +12532,22 @@
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E403" s="7" t="inlineStr">
@@ -12560,22 +12560,22 @@
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E404" s="7" t="inlineStr">
@@ -12588,22 +12588,22 @@
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E405" s="7" t="inlineStr">
@@ -12616,22 +12616,22 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E406" s="7" t="inlineStr">
@@ -12644,22 +12644,22 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E407" s="7" t="inlineStr">
@@ -12672,22 +12672,22 @@
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E408" s="7" t="inlineStr">
@@ -12700,49 +12700,45 @@
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E409" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F409" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E409" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F409" s="2" t="n"/>
     </row>
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12760,17 +12756,17 @@
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12788,17 +12784,17 @@
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12816,17 +12812,17 @@
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12844,17 +12840,17 @@
     <row r="414">
       <c r="A414" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12872,17 +12868,17 @@
     <row r="415">
       <c r="A415" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12900,17 +12896,17 @@
     <row r="416">
       <c r="A416" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12928,17 +12924,17 @@
     <row r="417">
       <c r="A417" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12956,22 +12952,22 @@
     <row r="418">
       <c r="A418" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E418" s="7" t="inlineStr">
@@ -12984,22 +12980,22 @@
     <row r="419">
       <c r="A419" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E419" s="7" t="inlineStr">
@@ -13012,22 +13008,22 @@
     <row r="420">
       <c r="A420" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E420" s="7" t="inlineStr">
@@ -13040,22 +13036,22 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E421" s="7" t="inlineStr">
@@ -13068,22 +13064,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13096,22 +13092,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13124,22 +13120,22 @@
     <row r="424">
       <c r="A424" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E424" s="7" t="inlineStr">
@@ -13152,22 +13148,22 @@
     <row r="425">
       <c r="A425" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E425" s="7" t="inlineStr">
@@ -13180,22 +13176,22 @@
     <row r="426">
       <c r="A426" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E426" s="7" t="inlineStr">
@@ -13208,50 +13204,54 @@
     <row r="427">
       <c r="A427" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
-        </is>
-      </c>
-      <c r="E427" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F427" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E427" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F427" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="428">
       <c r="A428" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E428" s="7" t="inlineStr">
@@ -13264,22 +13264,22 @@
     <row r="429">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E429" s="7" t="inlineStr">
@@ -13292,22 +13292,22 @@
     <row r="430">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E430" s="7" t="inlineStr">
@@ -13320,22 +13320,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13348,22 +13348,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13376,7 +13376,7 @@
     <row r="433">
       <c r="A433" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B433" s="2" t="inlineStr">
@@ -13386,12 +13386,12 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E433" s="7" t="inlineStr">
@@ -13404,22 +13404,22 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E434" s="7" t="inlineStr">
@@ -13432,22 +13432,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13460,22 +13460,22 @@
     <row r="436">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E436" s="7" t="inlineStr">
@@ -13488,22 +13488,22 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E437" s="7" t="inlineStr">
@@ -13516,22 +13516,22 @@
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E438" s="7" t="inlineStr">
@@ -13544,22 +13544,22 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E439" s="7" t="inlineStr">
@@ -13572,22 +13572,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13600,22 +13600,22 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E441" s="7" t="inlineStr">
@@ -13628,7 +13628,7 @@
     <row r="442">
       <c r="A442" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B442" s="2" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13656,17 +13656,17 @@
     <row r="443">
       <c r="A443" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13684,22 +13684,22 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E444" s="7" t="inlineStr">
@@ -13712,22 +13712,22 @@
     <row r="445">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E445" s="7" t="inlineStr">
@@ -13740,22 +13740,22 @@
     <row r="446">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E446" s="7" t="inlineStr">
@@ -13768,22 +13768,22 @@
     <row r="447">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E447" s="7" t="inlineStr">
@@ -13796,22 +13796,22 @@
     <row r="448">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E448" s="7" t="inlineStr">
@@ -13824,22 +13824,22 @@
     <row r="449">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E449" s="7" t="inlineStr">
@@ -13852,22 +13852,22 @@
     <row r="450">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E450" s="7" t="inlineStr">
@@ -13880,7 +13880,7 @@
     <row r="451">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -13890,12 +13890,12 @@
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E451" s="7" t="inlineStr">
@@ -13908,7 +13908,7 @@
     <row r="452">
       <c r="A452" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B452" s="2" t="inlineStr">
@@ -13918,12 +13918,12 @@
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E452" s="7" t="inlineStr">
@@ -13936,7 +13936,7 @@
     <row r="453">
       <c r="A453" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B453" s="2" t="inlineStr">
@@ -13946,12 +13946,12 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E453" s="7" t="inlineStr">
@@ -13964,7 +13964,7 @@
     <row r="454">
       <c r="A454" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B454" s="2" t="inlineStr">
@@ -13974,12 +13974,12 @@
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E454" s="7" t="inlineStr">
@@ -13992,7 +13992,7 @@
     <row r="455">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -14002,12 +14002,12 @@
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E455" s="7" t="inlineStr">
@@ -14020,7 +14020,7 @@
     <row r="456">
       <c r="A456" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B456" s="2" t="inlineStr">
@@ -14030,12 +14030,12 @@
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E456" s="7" t="inlineStr">
@@ -14048,30 +14048,534 @@
     <row r="457">
       <c r="A457" s="2" t="inlineStr">
         <is>
+          <t>Caixa 1948</t>
+        </is>
+      </c>
+      <c r="B457" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C457" s="2" t="inlineStr">
+        <is>
+          <t>Boneco Harry Potter japonês 1</t>
+        </is>
+      </c>
+      <c r="D457" s="2" t="inlineStr">
+        <is>
+          <t>Quarto do Bento</t>
+        </is>
+      </c>
+      <c r="E457" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F457" s="2" t="n"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 1948</t>
+        </is>
+      </c>
+      <c r="B458" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C458" s="2" t="inlineStr">
+        <is>
+          <t>Boneco Harry Potter japonês 2</t>
+        </is>
+      </c>
+      <c r="D458" s="2" t="inlineStr">
+        <is>
+          <t>Quarto do Bento</t>
+        </is>
+      </c>
+      <c r="E458" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F458" s="2" t="n"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 1948</t>
+        </is>
+      </c>
+      <c r="B459" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C459" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
+        </is>
+      </c>
+      <c r="D459" s="2" t="inlineStr">
+        <is>
+          <t>Quarto do Bento</t>
+        </is>
+      </c>
+      <c r="E459" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F459" s="2" t="n"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 3501</t>
+        </is>
+      </c>
+      <c r="B460" s="2" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C460" s="2" t="inlineStr">
+        <is>
+          <t>Bolsas de cabos</t>
+        </is>
+      </c>
+      <c r="D460" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E460" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F460" s="2" t="n"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 3501</t>
+        </is>
+      </c>
+      <c r="B461" s="2" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C461" s="2" t="inlineStr">
+        <is>
+          <t>Cabos soltos</t>
+        </is>
+      </c>
+      <c r="D461" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E461" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F461" s="2" t="n"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 3501</t>
+        </is>
+      </c>
+      <c r="B462" s="2" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C462" s="2" t="inlineStr">
+        <is>
+          <t>Power banks</t>
+        </is>
+      </c>
+      <c r="D462" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E462" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F462" s="2" t="n"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 3501</t>
+        </is>
+      </c>
+      <c r="B463" s="2" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C463" s="2" t="inlineStr">
+        <is>
+          <t>Mesas digitalizadoras</t>
+        </is>
+      </c>
+      <c r="D463" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E463" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F463" s="2" t="n"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B464" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C464" s="2" t="inlineStr">
+        <is>
+          <t>Furadeira</t>
+        </is>
+      </c>
+      <c r="D464" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E464" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F464" s="2" t="n"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B465" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C465" s="2" t="inlineStr">
+        <is>
+          <t>Parafusadeira</t>
+        </is>
+      </c>
+      <c r="D465" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E465" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F465" s="2" t="n"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B466" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C466" s="2" t="inlineStr">
+        <is>
+          <t>Acessórios de aspirador</t>
+        </is>
+      </c>
+      <c r="D466" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E466" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F466" s="2" t="n"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B467" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C467" s="2" t="inlineStr">
+        <is>
+          <t>Ralo click</t>
+        </is>
+      </c>
+      <c r="D467" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E467" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F467" s="2" t="n"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B468" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C468" s="2" t="inlineStr">
+        <is>
+          <t>Escova de limpeza elétrica</t>
+        </is>
+      </c>
+      <c r="D468" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E468" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F468" s="2" t="n"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="2" t="inlineStr">
+        <is>
           <t>Caixa 29501</t>
         </is>
       </c>
-      <c r="B457" s="2" t="inlineStr">
+      <c r="B469" s="2" t="inlineStr">
         <is>
           <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
-      <c r="C457" s="2" t="inlineStr">
+      <c r="C469" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Aragorn</t>
+        </is>
+      </c>
+      <c r="D469" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E469" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F469" s="2" t="n"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B470" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C470" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Arwen Undómiel</t>
+        </is>
+      </c>
+      <c r="D470" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E470" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F470" s="2" t="n"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B471" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C471" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D471" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E471" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F471" s="2" t="n"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B472" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C472" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D472" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E472" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F472" s="2" t="n"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B473" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C473" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D473" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E473" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F473" s="2" t="n"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B474" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C474" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D474" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E474" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F474" s="2" t="n"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B475" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C475" s="2" t="inlineStr">
         <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D457" s="2" t="inlineStr">
+      <c r="D475" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E457" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F457" s="2" t="n"/>
+      <c r="E475" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F475" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14110,7 +14614,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>456</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4">
@@ -14130,7 +14634,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixa 46 com tênis e sandálias especiais
- All Star surrado
- Nano 13 do Chile
- Jordan presente do Rodrigo 💝
- Air Jordan de salto
- Adidas da Maratona do Rio
- Vans roxo e mais

Total: 484 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F475"/>
+  <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11111,7 +11111,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F352" s="2" t="inlineStr"/>
+      <c r="F352" s="2" t="n"/>
     </row>
     <row r="353">
       <c r="A353" s="2" t="inlineStr">
@@ -11139,7 +11139,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F353" s="2" t="inlineStr"/>
+      <c r="F353" s="2" t="n"/>
     </row>
     <row r="354">
       <c r="A354" s="2" t="inlineStr">
@@ -11167,7 +11167,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F354" s="2" t="inlineStr"/>
+      <c r="F354" s="2" t="n"/>
     </row>
     <row r="355">
       <c r="A355" s="2" t="inlineStr">
@@ -11195,7 +11195,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F355" s="2" t="inlineStr"/>
+      <c r="F355" s="2" t="n"/>
     </row>
     <row r="356">
       <c r="A356" s="2" t="inlineStr">
@@ -11223,7 +11223,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F356" s="2" t="inlineStr"/>
+      <c r="F356" s="2" t="n"/>
     </row>
     <row r="357">
       <c r="A357" s="2" t="inlineStr">
@@ -11251,7 +11251,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F357" s="2" t="inlineStr"/>
+      <c r="F357" s="2" t="n"/>
     </row>
     <row r="358">
       <c r="A358" s="2" t="inlineStr">
@@ -11279,7 +11279,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F358" s="2" t="inlineStr"/>
+      <c r="F358" s="2" t="n"/>
     </row>
     <row r="359">
       <c r="A359" s="2" t="inlineStr">
@@ -11307,7 +11307,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F359" s="2" t="inlineStr"/>
+      <c r="F359" s="2" t="n"/>
     </row>
     <row r="360">
       <c r="A360" s="2" t="inlineStr">
@@ -11335,7 +11335,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F360" s="2" t="inlineStr"/>
+      <c r="F360" s="2" t="n"/>
     </row>
     <row r="361">
       <c r="A361" s="2" t="inlineStr">
@@ -11363,7 +11363,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F361" s="2" t="inlineStr"/>
+      <c r="F361" s="2" t="n"/>
     </row>
     <row r="362">
       <c r="A362" s="2" t="inlineStr">
@@ -11391,7 +11391,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F362" s="2" t="inlineStr"/>
+      <c r="F362" s="2" t="n"/>
     </row>
     <row r="363">
       <c r="A363" s="2" t="inlineStr">
@@ -11419,7 +11419,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F363" s="2" t="inlineStr"/>
+      <c r="F363" s="2" t="n"/>
     </row>
     <row r="364">
       <c r="A364" s="2" t="inlineStr">
@@ -11447,7 +11447,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F364" s="2" t="inlineStr"/>
+      <c r="F364" s="2" t="n"/>
     </row>
     <row r="365">
       <c r="A365" s="2" t="inlineStr">
@@ -11475,7 +11475,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F365" s="2" t="inlineStr"/>
+      <c r="F365" s="2" t="n"/>
     </row>
     <row r="366">
       <c r="A366" s="2" t="inlineStr">
@@ -11503,7 +11503,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F366" s="2" t="inlineStr"/>
+      <c r="F366" s="2" t="n"/>
     </row>
     <row r="367">
       <c r="A367" s="2" t="inlineStr">
@@ -11531,7 +11531,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F367" s="2" t="inlineStr"/>
+      <c r="F367" s="2" t="n"/>
     </row>
     <row r="368">
       <c r="A368" s="2" t="inlineStr">
@@ -11559,7 +11559,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F368" s="2" t="inlineStr"/>
+      <c r="F368" s="2" t="n"/>
     </row>
     <row r="369">
       <c r="A369" s="2" t="inlineStr">
@@ -11587,307 +11587,307 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F369" s="2" t="inlineStr"/>
+      <c r="F369" s="2" t="n"/>
     </row>
     <row r="370">
       <c r="A370" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B370" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Tênis All Star branco surrado</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E370" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F370" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E370" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F370" s="2" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B371" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Tênis Nano 13 roxo (comprado no Chile)</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E371" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F371" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E371" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F371" s="2" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B372" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Tênis Jordan creme (presente do Rodrigo)</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E372" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F372" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E372" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F372" s="2" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Tênis Jordan vermelho Rashimura</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E373" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F373" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E373" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F373" s="2" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Tênis Corre 4 rosa</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E374" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F374" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E374" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F374" s="2" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Sandália rasteirinha roxa</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E375" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F375" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E375" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F375" s="2" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Havaianas branca</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E376" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F376" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E376" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F376" s="2" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Tênis Adidas Pro da Maratona do Rio</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E377" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F377" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E377" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F377" s="2" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B378" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Air Jordan de salto</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E378" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F378" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E378" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F378" s="2" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 46</t>
         </is>
       </c>
       <c r="B379" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Tênis Vans roxo</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E379" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F379" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E379" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F379" s="2" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E380" s="7" t="inlineStr">
@@ -11900,22 +11900,22 @@
     <row r="381">
       <c r="A381" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E381" s="7" t="inlineStr">
@@ -11928,22 +11928,22 @@
     <row r="382">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E382" s="7" t="inlineStr">
@@ -11956,17 +11956,17 @@
     <row r="383">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
@@ -11984,17 +11984,17 @@
     <row r="384">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
@@ -12012,17 +12012,17 @@
     <row r="385">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
@@ -12035,26 +12035,22 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F385" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F385" s="2" t="n"/>
     </row>
     <row r="386">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12067,26 +12063,22 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F386" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F386" s="2" t="n"/>
     </row>
     <row r="387">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12099,31 +12091,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F387" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F387" s="2" t="n"/>
     </row>
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E388" s="7" t="inlineStr">
@@ -12136,22 +12124,22 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E389" s="7" t="inlineStr">
@@ -12159,31 +12147,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F389" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F389" s="2" t="n"/>
     </row>
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E390" s="7" t="inlineStr">
@@ -12196,22 +12180,22 @@
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E391" s="7" t="inlineStr">
@@ -12224,22 +12208,22 @@
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E392" s="7" t="inlineStr">
@@ -12257,12 +12241,12 @@
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12285,12 +12269,12 @@
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12313,12 +12297,12 @@
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12331,7 +12315,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F395" s="2" t="n"/>
+      <c r="F395" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
@@ -12341,12 +12329,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12359,7 +12347,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F396" s="2" t="n"/>
+      <c r="F396" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
@@ -12369,12 +12361,12 @@
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12387,7 +12379,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F397" s="2" t="n"/>
+      <c r="F397" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
@@ -12402,7 +12398,7 @@
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12420,22 +12416,22 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E399" s="7" t="inlineStr">
@@ -12443,27 +12439,31 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F399" s="2" t="n"/>
+      <c r="F399" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E400" s="7" t="inlineStr">
@@ -12476,22 +12476,22 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E401" s="7" t="inlineStr">
@@ -12504,22 +12504,22 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E402" s="7" t="inlineStr">
@@ -12532,22 +12532,22 @@
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E403" s="7" t="inlineStr">
@@ -12560,22 +12560,22 @@
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E404" s="7" t="inlineStr">
@@ -12588,22 +12588,22 @@
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E405" s="7" t="inlineStr">
@@ -12616,22 +12616,22 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E406" s="7" t="inlineStr">
@@ -12644,22 +12644,22 @@
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E407" s="7" t="inlineStr">
@@ -12672,22 +12672,22 @@
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E408" s="7" t="inlineStr">
@@ -12700,22 +12700,22 @@
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E409" s="7" t="inlineStr">
@@ -12728,22 +12728,22 @@
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E410" s="7" t="inlineStr">
@@ -12756,22 +12756,22 @@
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E411" s="7" t="inlineStr">
@@ -12784,22 +12784,22 @@
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E412" s="7" t="inlineStr">
@@ -12812,22 +12812,22 @@
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E413" s="7" t="inlineStr">
@@ -12845,12 +12845,12 @@
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12878,7 +12878,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12906,7 +12906,7 @@
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12934,7 +12934,7 @@
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12952,22 +12952,22 @@
     <row r="418">
       <c r="A418" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E418" s="7" t="inlineStr">
@@ -12980,22 +12980,22 @@
     <row r="419">
       <c r="A419" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E419" s="7" t="inlineStr">
@@ -13008,22 +13008,22 @@
     <row r="420">
       <c r="A420" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E420" s="7" t="inlineStr">
@@ -13036,22 +13036,22 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E421" s="7" t="inlineStr">
@@ -13064,22 +13064,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13092,22 +13092,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13120,22 +13120,22 @@
     <row r="424">
       <c r="A424" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E424" s="7" t="inlineStr">
@@ -13148,22 +13148,22 @@
     <row r="425">
       <c r="A425" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E425" s="7" t="inlineStr">
@@ -13176,22 +13176,22 @@
     <row r="426">
       <c r="A426" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E426" s="7" t="inlineStr">
@@ -13204,54 +13204,50 @@
     <row r="427">
       <c r="A427" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E427" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F427" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E427" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F427" s="2" t="n"/>
     </row>
     <row r="428">
       <c r="A428" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E428" s="7" t="inlineStr">
@@ -13264,22 +13260,22 @@
     <row r="429">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E429" s="7" t="inlineStr">
@@ -13292,22 +13288,22 @@
     <row r="430">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E430" s="7" t="inlineStr">
@@ -13320,22 +13316,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13348,22 +13344,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13376,22 +13372,22 @@
     <row r="433">
       <c r="A433" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B433" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E433" s="7" t="inlineStr">
@@ -13404,22 +13400,22 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E434" s="7" t="inlineStr">
@@ -13432,22 +13428,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13460,22 +13456,22 @@
     <row r="436">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E436" s="7" t="inlineStr">
@@ -13488,30 +13484,34 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E437" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F437" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E437" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F437" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
@@ -13521,12 +13521,12 @@
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
@@ -13549,12 +13549,12 @@
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
@@ -13572,17 +13572,17 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
@@ -13600,17 +13600,17 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
@@ -13628,17 +13628,17 @@
     <row r="442">
       <c r="A442" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B442" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13656,17 +13656,17 @@
     <row r="443">
       <c r="A443" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13684,22 +13684,22 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E444" s="7" t="inlineStr">
@@ -13712,22 +13712,22 @@
     <row r="445">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E445" s="7" t="inlineStr">
@@ -13740,22 +13740,22 @@
     <row r="446">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E446" s="7" t="inlineStr">
@@ -13768,22 +13768,22 @@
     <row r="447">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E447" s="7" t="inlineStr">
@@ -13796,22 +13796,22 @@
     <row r="448">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E448" s="7" t="inlineStr">
@@ -13824,22 +13824,22 @@
     <row r="449">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E449" s="7" t="inlineStr">
@@ -13852,22 +13852,22 @@
     <row r="450">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E450" s="7" t="inlineStr">
@@ -13880,22 +13880,22 @@
     <row r="451">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E451" s="7" t="inlineStr">
@@ -13908,22 +13908,22 @@
     <row r="452">
       <c r="A452" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B452" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E452" s="7" t="inlineStr">
@@ -13936,22 +13936,22 @@
     <row r="453">
       <c r="A453" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B453" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E453" s="7" t="inlineStr">
@@ -13974,7 +13974,7 @@
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
@@ -14002,7 +14002,7 @@
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
@@ -14025,12 +14025,12 @@
       </c>
       <c r="B456" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr">
@@ -14053,12 +14053,12 @@
       </c>
       <c r="B457" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C457" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D457" s="2" t="inlineStr">
@@ -14086,7 +14086,7 @@
       </c>
       <c r="C458" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D458" s="2" t="inlineStr">
@@ -14114,7 +14114,7 @@
       </c>
       <c r="C459" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D459" s="2" t="inlineStr">
@@ -14132,22 +14132,22 @@
     <row r="460">
       <c r="A460" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B460" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C460" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D460" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E460" s="7" t="inlineStr">
@@ -14160,22 +14160,22 @@
     <row r="461">
       <c r="A461" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B461" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C461" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D461" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E461" s="7" t="inlineStr">
@@ -14188,22 +14188,22 @@
     <row r="462">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C462" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D462" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E462" s="7" t="inlineStr">
@@ -14216,22 +14216,22 @@
     <row r="463">
       <c r="A463" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B463" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C463" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D463" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E463" s="7" t="inlineStr">
@@ -14244,22 +14244,22 @@
     <row r="464">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C464" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D464" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E464" s="7" t="inlineStr">
@@ -14272,22 +14272,22 @@
     <row r="465">
       <c r="A465" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B465" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C465" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D465" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E465" s="7" t="inlineStr">
@@ -14300,22 +14300,22 @@
     <row r="466">
       <c r="A466" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B466" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C466" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D466" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E466" s="7" t="inlineStr">
@@ -14328,22 +14328,22 @@
     <row r="467">
       <c r="A467" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B467" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C467" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D467" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E467" s="7" t="inlineStr">
@@ -14356,22 +14356,22 @@
     <row r="468">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C468" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D468" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E468" s="7" t="inlineStr">
@@ -14384,7 +14384,7 @@
     <row r="469">
       <c r="A469" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B469" s="2" t="inlineStr">
@@ -14394,12 +14394,12 @@
       </c>
       <c r="C469" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D469" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E469" s="7" t="inlineStr">
@@ -14412,17 +14412,17 @@
     <row r="470">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C470" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D470" s="2" t="inlineStr">
@@ -14440,17 +14440,17 @@
     <row r="471">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr">
@@ -14468,17 +14468,17 @@
     <row r="472">
       <c r="A472" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B472" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C472" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D472" s="2" t="inlineStr">
@@ -14496,17 +14496,17 @@
     <row r="473">
       <c r="A473" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B473" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C473" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D473" s="2" t="inlineStr">
@@ -14524,22 +14524,22 @@
     <row r="474">
       <c r="A474" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B474" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C474" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D474" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E474" s="7" t="inlineStr">
@@ -14552,30 +14552,310 @@
     <row r="475">
       <c r="A475" s="2" t="inlineStr">
         <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B475" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C475" s="2" t="inlineStr">
+        <is>
+          <t>Parafusadeira</t>
+        </is>
+      </c>
+      <c r="D475" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E475" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F475" s="2" t="n"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B476" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C476" s="2" t="inlineStr">
+        <is>
+          <t>Acessórios de aspirador</t>
+        </is>
+      </c>
+      <c r="D476" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E476" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F476" s="2" t="n"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B477" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C477" s="2" t="inlineStr">
+        <is>
+          <t>Ralo click</t>
+        </is>
+      </c>
+      <c r="D477" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E477" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F477" s="2" t="n"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 9501</t>
+        </is>
+      </c>
+      <c r="B478" s="2" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C478" s="2" t="inlineStr">
+        <is>
+          <t>Escova de limpeza elétrica</t>
+        </is>
+      </c>
+      <c r="D478" s="2" t="inlineStr">
+        <is>
+          <t>Lavanderia</t>
+        </is>
+      </c>
+      <c r="E478" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F478" s="2" t="n"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="2" t="inlineStr">
+        <is>
           <t>Caixa 29501</t>
         </is>
       </c>
-      <c r="B475" s="2" t="inlineStr">
+      <c r="B479" s="2" t="inlineStr">
         <is>
           <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
-      <c r="C475" s="2" t="inlineStr">
+      <c r="C479" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Aragorn</t>
+        </is>
+      </c>
+      <c r="D479" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E479" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F479" s="2" t="n"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B480" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C480" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Arwen Undómiel</t>
+        </is>
+      </c>
+      <c r="D480" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E480" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F480" s="2" t="n"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B481" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C481" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D481" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E481" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F481" s="2" t="n"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B482" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C482" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D482" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E482" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F482" s="2" t="n"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B483" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C483" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D483" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E483" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F483" s="2" t="n"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B484" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C484" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D484" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E484" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F484" s="2" t="n"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B485" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C485" s="2" t="inlineStr">
         <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D475" s="2" t="inlineStr">
+      <c r="D485" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E475" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F475" s="2" t="n"/>
+      <c r="E485" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F485" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14614,7 +14894,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>474</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4">
@@ -14634,7 +14914,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixa 47 com tênis de corrida e CrossFit
- Nano 11 Froning
- Adidas ZX presente do Rodrigo 💝
- Nike de placa para corrida
- Chinelo Olympikus Pro Max
- Fivelas Nike Air

Total: 490 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F485"/>
+  <dimension ref="A1:F491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11615,7 +11615,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F370" s="2" t="inlineStr"/>
+      <c r="F370" s="2" t="n"/>
     </row>
     <row r="371">
       <c r="A371" s="2" t="inlineStr">
@@ -11643,7 +11643,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F371" s="2" t="inlineStr"/>
+      <c r="F371" s="2" t="n"/>
     </row>
     <row r="372">
       <c r="A372" s="2" t="inlineStr">
@@ -11671,7 +11671,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F372" s="2" t="inlineStr"/>
+      <c r="F372" s="2" t="n"/>
     </row>
     <row r="373">
       <c r="A373" s="2" t="inlineStr">
@@ -11699,7 +11699,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F373" s="2" t="inlineStr"/>
+      <c r="F373" s="2" t="n"/>
     </row>
     <row r="374">
       <c r="A374" s="2" t="inlineStr">
@@ -11727,7 +11727,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F374" s="2" t="inlineStr"/>
+      <c r="F374" s="2" t="n"/>
     </row>
     <row r="375">
       <c r="A375" s="2" t="inlineStr">
@@ -11755,7 +11755,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F375" s="2" t="inlineStr"/>
+      <c r="F375" s="2" t="n"/>
     </row>
     <row r="376">
       <c r="A376" s="2" t="inlineStr">
@@ -11783,7 +11783,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F376" s="2" t="inlineStr"/>
+      <c r="F376" s="2" t="n"/>
     </row>
     <row r="377">
       <c r="A377" s="2" t="inlineStr">
@@ -11811,7 +11811,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F377" s="2" t="inlineStr"/>
+      <c r="F377" s="2" t="n"/>
     </row>
     <row r="378">
       <c r="A378" s="2" t="inlineStr">
@@ -11839,7 +11839,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F378" s="2" t="inlineStr"/>
+      <c r="F378" s="2" t="n"/>
     </row>
     <row r="379">
       <c r="A379" s="2" t="inlineStr">
@@ -11867,175 +11867,175 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F379" s="2" t="inlineStr"/>
+      <c r="F379" s="2" t="n"/>
     </row>
     <row r="380">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Chinelo Olympikus Eleva Pro Max</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E380" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F380" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E380" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F380" s="2" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B381" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Tênis Nano 11 (Froning)</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E381" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F381" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E381" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F381" s="2" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Tênis Adidas branco ZX (presente do Rodrigo)</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E382" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F382" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E382" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F382" s="2" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Tênis Nike Air branco com roxo</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E383" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F383" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E383" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F383" s="2" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Calçados</t>
         </is>
       </c>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Tênis Nike de placa para corrida (modelo não identificado)</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E384" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F384" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E384" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F384" s="2" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 47</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Fivelas do Nike Air tipo botinha (marrom com roxo)</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E385" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F385" s="2" t="n"/>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E385" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F385" s="2" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" s="2" t="inlineStr">
@@ -12045,12 +12045,12 @@
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12073,12 +12073,12 @@
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
@@ -12096,22 +12096,22 @@
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E388" s="7" t="inlineStr">
@@ -12124,22 +12124,22 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E389" s="7" t="inlineStr">
@@ -12152,22 +12152,22 @@
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E390" s="7" t="inlineStr">
@@ -12180,22 +12180,22 @@
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E391" s="7" t="inlineStr">
@@ -12208,22 +12208,22 @@
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E392" s="7" t="inlineStr">
@@ -12236,17 +12236,17 @@
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12264,22 +12264,22 @@
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E394" s="7" t="inlineStr">
@@ -12292,22 +12292,22 @@
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E395" s="7" t="inlineStr">
@@ -12315,31 +12315,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F395" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F395" s="2" t="n"/>
     </row>
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E396" s="7" t="inlineStr">
@@ -12347,31 +12343,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F396" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F396" s="2" t="n"/>
     </row>
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E397" s="7" t="inlineStr">
@@ -12379,31 +12371,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F397" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F397" s="2" t="n"/>
     </row>
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E398" s="7" t="inlineStr">
@@ -12421,12 +12409,12 @@
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12439,11 +12427,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F399" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F399" s="2" t="n"/>
     </row>
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
@@ -12458,7 +12442,7 @@
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
@@ -12481,12 +12465,12 @@
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
@@ -12499,7 +12483,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F401" s="2" t="n"/>
+      <c r="F401" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
@@ -12509,12 +12497,12 @@
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
@@ -12527,7 +12515,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F402" s="2" t="n"/>
+      <c r="F402" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
@@ -12537,12 +12529,12 @@
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12555,7 +12547,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F403" s="2" t="n"/>
+      <c r="F403" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
@@ -12570,7 +12566,7 @@
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12593,12 +12589,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12611,7 +12607,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F405" s="2" t="n"/>
+      <c r="F405" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
@@ -12621,12 +12621,12 @@
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12649,12 +12649,12 @@
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12682,7 +12682,7 @@
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12700,22 +12700,22 @@
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E409" s="7" t="inlineStr">
@@ -12728,22 +12728,22 @@
     <row r="410">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E410" s="7" t="inlineStr">
@@ -12756,22 +12756,22 @@
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E411" s="7" t="inlineStr">
@@ -12784,22 +12784,22 @@
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E412" s="7" t="inlineStr">
@@ -12812,22 +12812,22 @@
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E413" s="7" t="inlineStr">
@@ -12840,22 +12840,22 @@
     <row r="414">
       <c r="A414" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E414" s="7" t="inlineStr">
@@ -12868,22 +12868,22 @@
     <row r="415">
       <c r="A415" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E415" s="7" t="inlineStr">
@@ -12896,22 +12896,22 @@
     <row r="416">
       <c r="A416" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E416" s="7" t="inlineStr">
@@ -12924,22 +12924,22 @@
     <row r="417">
       <c r="A417" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E417" s="7" t="inlineStr">
@@ -12952,22 +12952,22 @@
     <row r="418">
       <c r="A418" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E418" s="7" t="inlineStr">
@@ -12980,22 +12980,22 @@
     <row r="419">
       <c r="A419" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E419" s="7" t="inlineStr">
@@ -13018,7 +13018,7 @@
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13046,7 +13046,7 @@
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
@@ -13074,7 +13074,7 @@
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
@@ -13097,12 +13097,12 @@
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
@@ -13125,12 +13125,12 @@
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13153,12 +13153,12 @@
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13186,7 +13186,7 @@
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13232,22 +13232,22 @@
     <row r="428">
       <c r="A428" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E428" s="7" t="inlineStr">
@@ -13260,22 +13260,22 @@
     <row r="429">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E429" s="7" t="inlineStr">
@@ -13288,22 +13288,22 @@
     <row r="430">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E430" s="7" t="inlineStr">
@@ -13316,22 +13316,22 @@
     <row r="431">
       <c r="A431" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E431" s="7" t="inlineStr">
@@ -13344,22 +13344,22 @@
     <row r="432">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E432" s="7" t="inlineStr">
@@ -13372,22 +13372,22 @@
     <row r="433">
       <c r="A433" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B433" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E433" s="7" t="inlineStr">
@@ -13400,17 +13400,17 @@
     <row r="434">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13428,17 +13428,17 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13461,12 +13461,12 @@
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13484,54 +13484,50 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E437" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F437" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E437" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F437" s="2" t="n"/>
     </row>
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E438" s="7" t="inlineStr">
@@ -13544,22 +13540,22 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E439" s="7" t="inlineStr">
@@ -13572,22 +13568,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13600,22 +13596,22 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E441" s="7" t="inlineStr">
@@ -13628,22 +13624,22 @@
     <row r="442">
       <c r="A442" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B442" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E442" s="7" t="inlineStr">
@@ -13656,30 +13652,34 @@
     <row r="443">
       <c r="A443" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E443" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F443" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E443" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F443" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
@@ -13717,12 +13717,12 @@
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
@@ -13745,12 +13745,12 @@
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
@@ -13773,12 +13773,12 @@
       </c>
       <c r="B447" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
@@ -13801,12 +13801,12 @@
       </c>
       <c r="B448" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
@@ -13829,12 +13829,12 @@
       </c>
       <c r="B449" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
@@ -13852,17 +13852,17 @@
     <row r="450">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
@@ -13880,17 +13880,17 @@
     <row r="451">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
@@ -13908,17 +13908,17 @@
     <row r="452">
       <c r="A452" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B452" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
@@ -13936,7 +13936,7 @@
     <row r="453">
       <c r="A453" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B453" s="2" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
@@ -13964,22 +13964,22 @@
     <row r="454">
       <c r="A454" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B454" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E454" s="7" t="inlineStr">
@@ -13992,22 +13992,22 @@
     <row r="455">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E455" s="7" t="inlineStr">
@@ -14020,22 +14020,22 @@
     <row r="456">
       <c r="A456" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B456" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E456" s="7" t="inlineStr">
@@ -14048,22 +14048,22 @@
     <row r="457">
       <c r="A457" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B457" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C457" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D457" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E457" s="7" t="inlineStr">
@@ -14076,22 +14076,22 @@
     <row r="458">
       <c r="A458" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B458" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C458" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D458" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E458" s="7" t="inlineStr">
@@ -14104,22 +14104,22 @@
     <row r="459">
       <c r="A459" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B459" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C459" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D459" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E459" s="7" t="inlineStr">
@@ -14142,7 +14142,7 @@
       </c>
       <c r="C460" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D460" s="2" t="inlineStr">
@@ -14170,7 +14170,7 @@
       </c>
       <c r="C461" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D461" s="2" t="inlineStr">
@@ -14193,12 +14193,12 @@
       </c>
       <c r="B462" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C462" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D462" s="2" t="inlineStr">
@@ -14221,12 +14221,12 @@
       </c>
       <c r="B463" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C463" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D463" s="2" t="inlineStr">
@@ -14254,7 +14254,7 @@
       </c>
       <c r="C464" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D464" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
       </c>
       <c r="C465" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D465" s="2" t="inlineStr">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="C466" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D466" s="2" t="inlineStr">
@@ -14338,7 +14338,7 @@
       </c>
       <c r="C467" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D467" s="2" t="inlineStr">
@@ -14366,7 +14366,7 @@
       </c>
       <c r="C468" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D468" s="2" t="inlineStr">
@@ -14394,7 +14394,7 @@
       </c>
       <c r="C469" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D469" s="2" t="inlineStr">
@@ -14412,22 +14412,22 @@
     <row r="470">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C470" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D470" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E470" s="7" t="inlineStr">
@@ -14440,22 +14440,22 @@
     <row r="471">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E471" s="7" t="inlineStr">
@@ -14468,22 +14468,22 @@
     <row r="472">
       <c r="A472" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B472" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C472" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D472" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E472" s="7" t="inlineStr">
@@ -14496,22 +14496,22 @@
     <row r="473">
       <c r="A473" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B473" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C473" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D473" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E473" s="7" t="inlineStr">
@@ -14524,22 +14524,22 @@
     <row r="474">
       <c r="A474" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B474" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C474" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D474" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E474" s="7" t="inlineStr">
@@ -14552,22 +14552,22 @@
     <row r="475">
       <c r="A475" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B475" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C475" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D475" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E475" s="7" t="inlineStr">
@@ -14580,22 +14580,22 @@
     <row r="476">
       <c r="A476" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B476" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C476" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D476" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E476" s="7" t="inlineStr">
@@ -14608,22 +14608,22 @@
     <row r="477">
       <c r="A477" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B477" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C477" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D477" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E477" s="7" t="inlineStr">
@@ -14636,22 +14636,22 @@
     <row r="478">
       <c r="A478" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B478" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C478" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D478" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E478" s="7" t="inlineStr">
@@ -14664,17 +14664,17 @@
     <row r="479">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C479" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D479" s="2" t="inlineStr">
@@ -14692,22 +14692,22 @@
     <row r="480">
       <c r="A480" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B480" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C480" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D480" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E480" s="7" t="inlineStr">
@@ -14720,22 +14720,22 @@
     <row r="481">
       <c r="A481" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B481" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C481" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D481" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E481" s="7" t="inlineStr">
@@ -14748,22 +14748,22 @@
     <row r="482">
       <c r="A482" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B482" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C482" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D482" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E482" s="7" t="inlineStr">
@@ -14776,22 +14776,22 @@
     <row r="483">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C483" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D483" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E483" s="7" t="inlineStr">
@@ -14804,22 +14804,22 @@
     <row r="484">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C484" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D484" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E484" s="7" t="inlineStr">
@@ -14842,20 +14842,188 @@
       </c>
       <c r="C485" s="2" t="inlineStr">
         <is>
+          <t>BrickHeadz Aragorn</t>
+        </is>
+      </c>
+      <c r="D485" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E485" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F485" s="2" t="n"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B486" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C486" s="2" t="inlineStr">
+        <is>
+          <t>BrickHeadz Arwen Undómiel</t>
+        </is>
+      </c>
+      <c r="D486" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E486" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F486" s="2" t="n"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B487" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C487" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D487" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E487" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F487" s="2" t="n"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B488" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C488" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D488" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E488" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F488" s="2" t="n"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B489" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C489" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D489" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E489" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F489" s="2" t="n"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B490" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C490" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D490" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E490" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F490" s="2" t="n"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B491" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C491" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D485" s="2" t="inlineStr">
+      <c r="D491" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E485" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F485" s="2" t="n"/>
+      <c r="E491" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F491" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14894,7 +15062,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4">
@@ -14914,7 +15082,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixa 50 com medicamentos e primeiros socorros
- Dilatador nasal
- Porta-cápsula
- Pomada anti-inflamatória
- Curativos

Prioridade Alta (emergências)
Total: 495 itens
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F492"/>
+  <dimension ref="A1:F496"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12063,119 +12063,119 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F386" s="2" t="inlineStr"/>
+      <c r="F386" s="2" t="n"/>
     </row>
     <row r="387">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Medicamentos</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Dilatador nasal</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E387" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F387" s="2" t="n"/>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E387" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F387" s="2" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Porta-cápsula</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E388" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F388" s="2" t="n"/>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E388" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F388" s="2" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Medicamentos</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Pomada anti-inflamatória</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E389" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F389" s="2" t="n"/>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E389" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F389" s="2" t="inlineStr"/>
     </row>
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Primeiros socorros</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Curativos</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E390" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F390" s="2" t="n"/>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E390" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F390" s="2" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
@@ -12185,12 +12185,12 @@
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
@@ -12213,12 +12213,12 @@
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
@@ -12246,7 +12246,7 @@
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
@@ -12269,12 +12269,12 @@
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
@@ -12292,22 +12292,22 @@
     <row r="395">
       <c r="A395" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E395" s="7" t="inlineStr">
@@ -12320,22 +12320,22 @@
     <row r="396">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E396" s="7" t="inlineStr">
@@ -12348,22 +12348,22 @@
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E397" s="7" t="inlineStr">
@@ -12376,22 +12376,22 @@
     <row r="398">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E398" s="7" t="inlineStr">
@@ -12414,7 +12414,7 @@
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
@@ -12432,22 +12432,22 @@
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E400" s="7" t="inlineStr">
@@ -12460,22 +12460,22 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E401" s="7" t="inlineStr">
@@ -12488,22 +12488,22 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E402" s="7" t="inlineStr">
@@ -12511,31 +12511,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F402" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F402" s="2" t="n"/>
     </row>
     <row r="403">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E403" s="7" t="inlineStr">
@@ -12543,11 +12539,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F403" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F403" s="2" t="n"/>
     </row>
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
@@ -12557,12 +12549,12 @@
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
@@ -12575,11 +12567,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F404" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F404" s="2" t="n"/>
     </row>
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
@@ -12589,12 +12577,12 @@
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
@@ -12622,7 +12610,7 @@
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
@@ -12649,12 +12637,12 @@
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
@@ -12667,7 +12655,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F407" s="2" t="n"/>
+      <c r="F407" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
@@ -12677,12 +12669,12 @@
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12695,7 +12687,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F408" s="2" t="n"/>
+      <c r="F408" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
@@ -12710,7 +12706,7 @@
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12733,12 +12729,12 @@
       </c>
       <c r="B410" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12751,7 +12747,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F410" s="2" t="n"/>
+      <c r="F410" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="411">
       <c r="A411" s="2" t="inlineStr">
@@ -12761,12 +12761,12 @@
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12789,12 +12789,12 @@
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12822,7 +12822,7 @@
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12850,7 +12850,7 @@
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12878,7 +12878,7 @@
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12896,22 +12896,22 @@
     <row r="416">
       <c r="A416" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E416" s="7" t="inlineStr">
@@ -12924,22 +12924,22 @@
     <row r="417">
       <c r="A417" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B417" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E417" s="7" t="inlineStr">
@@ -12952,22 +12952,22 @@
     <row r="418">
       <c r="A418" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B418" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E418" s="7" t="inlineStr">
@@ -12980,22 +12980,22 @@
     <row r="419">
       <c r="A419" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B419" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E419" s="7" t="inlineStr">
@@ -13013,12 +13013,12 @@
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
@@ -13036,22 +13036,22 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E421" s="7" t="inlineStr">
@@ -13064,22 +13064,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13092,22 +13092,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13120,22 +13120,22 @@
     <row r="424">
       <c r="A424" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E424" s="7" t="inlineStr">
@@ -13153,12 +13153,12 @@
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
@@ -13181,12 +13181,12 @@
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
@@ -13242,7 +13242,7 @@
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
@@ -13265,12 +13265,12 @@
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13293,12 +13293,12 @@
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13321,12 +13321,12 @@
       </c>
       <c r="B431" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13354,7 +13354,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13382,7 +13382,7 @@
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13405,12 +13405,12 @@
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13428,22 +13428,22 @@
     <row r="435">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E435" s="7" t="inlineStr">
@@ -13456,22 +13456,22 @@
     <row r="436">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E436" s="7" t="inlineStr">
@@ -13484,22 +13484,22 @@
     <row r="437">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E437" s="7" t="inlineStr">
@@ -13512,22 +13512,22 @@
     <row r="438">
       <c r="A438" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E438" s="7" t="inlineStr">
@@ -13540,17 +13540,17 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
@@ -13568,17 +13568,17 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
@@ -13601,12 +13601,12 @@
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
@@ -13629,12 +13629,12 @@
       </c>
       <c r="B442" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
@@ -13657,12 +13657,12 @@
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13680,54 +13680,50 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E444" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F444" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E444" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F444" s="2" t="n"/>
     </row>
     <row r="445">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E445" s="7" t="inlineStr">
@@ -13740,22 +13736,22 @@
     <row r="446">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E446" s="7" t="inlineStr">
@@ -13768,22 +13764,22 @@
     <row r="447">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E447" s="7" t="inlineStr">
@@ -13796,30 +13792,34 @@
     <row r="448">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E448" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F448" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E448" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F448" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="449">
       <c r="A449" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
@@ -13857,12 +13857,12 @@
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
@@ -13885,12 +13885,12 @@
       </c>
       <c r="B451" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
@@ -13913,12 +13913,12 @@
       </c>
       <c r="B452" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
@@ -13969,12 +13969,12 @@
       </c>
       <c r="B454" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
@@ -13997,12 +13997,12 @@
       </c>
       <c r="B455" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
@@ -14025,12 +14025,12 @@
       </c>
       <c r="B456" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr">
@@ -14048,17 +14048,17 @@
     <row r="457">
       <c r="A457" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B457" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C457" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D457" s="2" t="inlineStr">
@@ -14076,17 +14076,17 @@
     <row r="458">
       <c r="A458" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B458" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C458" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D458" s="2" t="inlineStr">
@@ -14104,17 +14104,17 @@
     <row r="459">
       <c r="A459" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B459" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C459" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D459" s="2" t="inlineStr">
@@ -14132,17 +14132,17 @@
     <row r="460">
       <c r="A460" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B460" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C460" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D460" s="2" t="inlineStr">
@@ -14160,22 +14160,22 @@
     <row r="461">
       <c r="A461" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B461" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C461" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D461" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E461" s="7" t="inlineStr">
@@ -14188,22 +14188,22 @@
     <row r="462">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C462" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D462" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E462" s="7" t="inlineStr">
@@ -14216,22 +14216,22 @@
     <row r="463">
       <c r="A463" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B463" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C463" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D463" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E463" s="7" t="inlineStr">
@@ -14244,22 +14244,22 @@
     <row r="464">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C464" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D464" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E464" s="7" t="inlineStr">
@@ -14282,7 +14282,7 @@
       </c>
       <c r="C465" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D465" s="2" t="inlineStr">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="C466" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D466" s="2" t="inlineStr">
@@ -14333,12 +14333,12 @@
       </c>
       <c r="B467" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C467" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D467" s="2" t="inlineStr">
@@ -14361,12 +14361,12 @@
       </c>
       <c r="B468" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C468" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D468" s="2" t="inlineStr">
@@ -14394,7 +14394,7 @@
       </c>
       <c r="C469" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D469" s="2" t="inlineStr">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="C470" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D470" s="2" t="inlineStr">
@@ -14450,7 +14450,7 @@
       </c>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr">
@@ -14478,7 +14478,7 @@
       </c>
       <c r="C472" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D472" s="2" t="inlineStr">
@@ -14506,7 +14506,7 @@
       </c>
       <c r="C473" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D473" s="2" t="inlineStr">
@@ -14534,7 +14534,7 @@
       </c>
       <c r="C474" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D474" s="2" t="inlineStr">
@@ -14562,7 +14562,7 @@
       </c>
       <c r="C475" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D475" s="2" t="inlineStr">
@@ -14590,7 +14590,7 @@
       </c>
       <c r="C476" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D476" s="2" t="inlineStr">
@@ -14608,22 +14608,22 @@
     <row r="477">
       <c r="A477" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B477" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C477" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D477" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E477" s="7" t="inlineStr">
@@ -14636,22 +14636,22 @@
     <row r="478">
       <c r="A478" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B478" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C478" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D478" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E478" s="7" t="inlineStr">
@@ -14664,22 +14664,22 @@
     <row r="479">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C479" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D479" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E479" s="7" t="inlineStr">
@@ -14692,22 +14692,22 @@
     <row r="480">
       <c r="A480" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B480" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C480" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D480" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E480" s="7" t="inlineStr">
@@ -14720,22 +14720,22 @@
     <row r="481">
       <c r="A481" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B481" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C481" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D481" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E481" s="7" t="inlineStr">
@@ -14748,22 +14748,22 @@
     <row r="482">
       <c r="A482" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B482" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C482" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D482" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E482" s="7" t="inlineStr">
@@ -14776,22 +14776,22 @@
     <row r="483">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C483" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D483" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E483" s="7" t="inlineStr">
@@ -14804,22 +14804,22 @@
     <row r="484">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C484" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D484" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E484" s="7" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="C485" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D485" s="2" t="inlineStr">
@@ -14860,22 +14860,22 @@
     <row r="486">
       <c r="A486" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B486" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C486" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D486" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E486" s="7" t="inlineStr">
@@ -14888,22 +14888,22 @@
     <row r="487">
       <c r="A487" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B487" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C487" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D487" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E487" s="7" t="inlineStr">
@@ -14916,22 +14916,22 @@
     <row r="488">
       <c r="A488" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B488" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C488" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D488" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E488" s="7" t="inlineStr">
@@ -14944,22 +14944,22 @@
     <row r="489">
       <c r="A489" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B489" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C489" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D489" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E489" s="7" t="inlineStr">
@@ -14982,7 +14982,7 @@
       </c>
       <c r="C490" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D490" s="2" t="inlineStr">
@@ -15010,7 +15010,7 @@
       </c>
       <c r="C491" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D491" s="2" t="inlineStr">
@@ -15038,20 +15038,132 @@
       </c>
       <c r="C492" s="2" t="inlineStr">
         <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D492" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E492" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F492" s="2" t="n"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B493" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C493" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D493" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E493" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F493" s="2" t="n"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B494" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C494" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D494" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E494" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F494" s="2" t="n"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B495" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C495" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D495" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E495" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F495" s="2" t="n"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B496" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C496" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D492" s="2" t="inlineStr">
+      <c r="D496" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E492" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F492" s="2" t="n"/>
+      <c r="E496" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F496" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15090,7 +15202,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4">
@@ -15110,7 +15222,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Adiciona Caixa 48 com aromas e aromaterapia
- Incensos
- Aromatizador de ambiente
- Vela perfumada
- Óleo essencial

Total: 499 itens (quase 500! 🎉)
</commit_message>
<xml_diff>
--- a/catalogo_mudanca.xlsx
+++ b/catalogo_mudanca.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F496"/>
+  <dimension ref="A1:F500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12040,17 +12040,17 @@
     <row r="386">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>Caixa 49</t>
+          <t>Caixa 48</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
         <is>
-          <t>Itens pessoais adultos</t>
+          <t>Aromas</t>
         </is>
       </c>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos íntimos (uso pessoal)</t>
+          <t>Incensos</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr">
@@ -12058,37 +12058,37 @@
           <t>Suíte</t>
         </is>
       </c>
-      <c r="E386" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F386" s="2" t="n"/>
+      <c r="E386" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F386" s="2" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>Caixa 50</t>
+          <t>Caixa 48</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
         <is>
-          <t>Medicamentos</t>
+          <t>Aromas</t>
         </is>
       </c>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>Dilatador nasal</t>
+          <t>Aromatizador de ambiente</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E387" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E387" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F387" s="2" t="inlineStr"/>
@@ -12096,27 +12096,27 @@
     <row r="388">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>Caixa 50</t>
+          <t>Caixa 48</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Aromas</t>
         </is>
       </c>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>Porta-cápsula</t>
+          <t>Vela perfumada</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E388" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E388" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F388" s="2" t="inlineStr"/>
@@ -12124,27 +12124,27 @@
     <row r="389">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>Caixa 50</t>
+          <t>Caixa 48</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
         <is>
-          <t>Medicamentos</t>
+          <t>Aromaterapia</t>
         </is>
       </c>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>Pomada anti-inflamatória</t>
+          <t>Óleo essencial</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
-        </is>
-      </c>
-      <c r="E389" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E389" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
         </is>
       </c>
       <c r="F389" s="2" t="inlineStr"/>
@@ -12152,22 +12152,22 @@
     <row r="390">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>Caixa 50</t>
+          <t>Caixa 49</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
         <is>
-          <t>Primeiros socorros</t>
+          <t>Itens pessoais adultos</t>
         </is>
       </c>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>Curativos</t>
+          <t>Brinquedos íntimos (uso pessoal)</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E390" s="3" t="inlineStr">
@@ -12175,32 +12175,32 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="F390" s="2" t="inlineStr"/>
+      <c r="F390" s="2" t="n"/>
     </row>
     <row r="391">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Medicamentos</t>
         </is>
       </c>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>Refil de produtos de limpeza</t>
+          <t>Dilatador nasal</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E391" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E391" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F391" s="2" t="n"/>
@@ -12208,27 +12208,27 @@
     <row r="392">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>Refil de veneno</t>
+          <t>Porta-cápsula</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E392" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E392" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F392" s="2" t="n"/>
@@ -12236,27 +12236,27 @@
     <row r="393">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Medicamentos</t>
         </is>
       </c>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>Ferro de passar</t>
+          <t>Pomada anti-inflamatória</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E393" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E393" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F393" s="2" t="n"/>
@@ -12264,27 +12264,27 @@
     <row r="394">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>Caixa 74</t>
+          <t>Caixa 50</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Primeiros socorros</t>
         </is>
       </c>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>Acessórios do ferro de passar</t>
+          <t>Curativos</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
-        </is>
-      </c>
-      <c r="E394" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
+          <t>Banheiro</t>
+        </is>
+      </c>
+      <c r="E394" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
         </is>
       </c>
       <c r="F394" s="2" t="n"/>
@@ -12297,12 +12297,12 @@
       </c>
       <c r="B395" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>Sacos de lavagem</t>
+          <t>Refil de produtos de limpeza</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr">
@@ -12325,12 +12325,12 @@
       </c>
       <c r="B396" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>Máquina de lavar portátil</t>
+          <t>Refil de veneno</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr">
@@ -12358,7 +12358,7 @@
       </c>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>Acessórios da máquina de lavar portátil</t>
+          <t>Ferro de passar</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr">
@@ -12381,12 +12381,12 @@
       </c>
       <c r="B398" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>Lixa de tapete de pedra de diatomita</t>
+          <t>Acessórios do ferro de passar</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr">
@@ -12404,22 +12404,22 @@
     <row r="399">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>Produtos de higiene do Rodrigo</t>
+          <t>Sacos de lavagem</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E399" s="7" t="inlineStr">
@@ -12432,22 +12432,22 @@
     <row r="400">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>Protetor solar</t>
+          <t>Máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E400" s="7" t="inlineStr">
@@ -12460,22 +12460,22 @@
     <row r="401">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>Shampoo Johnson &amp; Johnson</t>
+          <t>Acessórios da máquina de lavar portátil</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E401" s="7" t="inlineStr">
@@ -12488,22 +12488,22 @@
     <row r="402">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>Caixa 79</t>
+          <t>Caixa 74</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
         <is>
-          <t>Higiene Pessoal</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>Barbeadores</t>
+          <t>Lixa de tapete de pedra de diatomita</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E402" s="7" t="inlineStr">
@@ -12526,7 +12526,7 @@
       </c>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>Cortadores de unha</t>
+          <t>Produtos de higiene do Rodrigo</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr">
@@ -12544,22 +12544,22 @@
     <row r="404">
       <c r="A404" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B404" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>Panos de chão</t>
+          <t>Protetor solar</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E404" s="7" t="inlineStr">
@@ -12572,22 +12572,22 @@
     <row r="405">
       <c r="A405" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B405" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>Perfex</t>
+          <t>Shampoo Johnson &amp; Johnson</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E405" s="7" t="inlineStr">
@@ -12600,22 +12600,22 @@
     <row r="406">
       <c r="A406" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B406" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>Coleiras</t>
+          <t>Barbeadores</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E406" s="7" t="inlineStr">
@@ -12623,31 +12623,27 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F406" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F406" s="2" t="n"/>
     </row>
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>Caixa 128</t>
+          <t>Caixa 79</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>Tapete do corgi</t>
+          <t>Cortadores de unha</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="E407" s="7" t="inlineStr">
@@ -12655,11 +12651,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F407" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F407" s="2" t="n"/>
     </row>
     <row r="408">
       <c r="A408" s="2" t="inlineStr">
@@ -12669,12 +12661,12 @@
       </c>
       <c r="B408" s="2" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>Meias do corgi</t>
+          <t>Panos de chão</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr">
@@ -12687,11 +12679,7 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F408" s="2" t="inlineStr">
-        <is>
-          <t>Corgi</t>
-        </is>
-      </c>
+      <c r="F408" s="2" t="n"/>
     </row>
     <row r="409">
       <c r="A409" s="2" t="inlineStr">
@@ -12701,12 +12689,12 @@
       </c>
       <c r="B409" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato</t>
+          <t>Perfex</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr">
@@ -12734,7 +12722,7 @@
       </c>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>Sacos cata-caca do corgi</t>
+          <t>Coleiras</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr">
@@ -12761,12 +12749,12 @@
       </c>
       <c r="B411" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>Detergente de lavar louça</t>
+          <t>Tapete do corgi</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr">
@@ -12779,7 +12767,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F411" s="2" t="n"/>
+      <c r="F411" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="412">
       <c r="A412" s="2" t="inlineStr">
@@ -12789,12 +12781,12 @@
       </c>
       <c r="B412" s="2" t="inlineStr">
         <is>
-          <t>Produtos de Limpeza</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>Alvejante</t>
+          <t>Meias do corgi</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr">
@@ -12807,7 +12799,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F412" s="2" t="n"/>
+      <c r="F412" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="413">
       <c r="A413" s="2" t="inlineStr">
@@ -12822,7 +12818,7 @@
       </c>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>Garrafas de água genéricas</t>
+          <t>Panos de prato</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr">
@@ -12845,12 +12841,12 @@
       </c>
       <c r="B414" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Pet</t>
         </is>
       </c>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>Copos plásticos</t>
+          <t>Sacos cata-caca do corgi</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr">
@@ -12863,7 +12859,11 @@
           <t>Média</t>
         </is>
       </c>
-      <c r="F414" s="2" t="n"/>
+      <c r="F414" s="2" t="inlineStr">
+        <is>
+          <t>Corgi</t>
+        </is>
+      </c>
     </row>
     <row r="415">
       <c r="A415" s="2" t="inlineStr">
@@ -12873,12 +12873,12 @@
       </c>
       <c r="B415" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>Duas caramanholas Camelbak</t>
+          <t>Detergente de lavar louça</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr">
@@ -12901,12 +12901,12 @@
       </c>
       <c r="B416" s="2" t="inlineStr">
         <is>
-          <t>Cozinha</t>
+          <t>Produtos de Limpeza</t>
         </is>
       </c>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>Garrafa d'água do Shopping Total</t>
+          <t>Alvejante</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr">
@@ -12934,7 +12934,7 @@
       </c>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>Formas de silicone</t>
+          <t>Garrafas de água genéricas</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr">
@@ -12962,7 +12962,7 @@
       </c>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>Panos de prato chiques</t>
+          <t>Copos plásticos</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr">
@@ -12990,7 +12990,7 @@
       </c>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>Mandolins</t>
+          <t>Duas caramanholas Camelbak</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr">
@@ -13008,22 +13008,22 @@
     <row r="420">
       <c r="A420" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B420" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>Quebra-cabeças</t>
+          <t>Garrafa d'água do Shopping Total</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E420" s="7" t="inlineStr">
@@ -13036,22 +13036,22 @@
     <row r="421">
       <c r="A421" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B421" s="2" t="inlineStr">
         <is>
-          <t>Entretenimento</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>Cola para quebra-cabeças</t>
+          <t>Formas de silicone</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E421" s="7" t="inlineStr">
@@ -13064,22 +13064,22 @@
     <row r="422">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>Base com rodas da máquina de lavar</t>
+          <t>Panos de prato chiques</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E422" s="7" t="inlineStr">
@@ -13092,22 +13092,22 @@
     <row r="423">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>Caixa 129</t>
+          <t>Caixa 128</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
         <is>
-          <t>Organização</t>
+          <t>Cozinha</t>
         </is>
       </c>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>Etiquetadora Brother</t>
+          <t>Mandolins</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E423" s="7" t="inlineStr">
@@ -13125,12 +13125,12 @@
       </c>
       <c r="B424" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira a bateria</t>
+          <t>Quebra-cabeças</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr">
@@ -13148,22 +13148,22 @@
     <row r="425">
       <c r="A425" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B425" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Entretenimento</t>
         </is>
       </c>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>Cabos de energia</t>
+          <t>Cola para quebra-cabeças</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E425" s="7" t="inlineStr">
@@ -13176,22 +13176,22 @@
     <row r="426">
       <c r="A426" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B426" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>Película iPhone 15 Pro Max</t>
+          <t>Base com rodas da máquina de lavar</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E426" s="7" t="inlineStr">
@@ -13204,22 +13204,22 @@
     <row r="427">
       <c r="A427" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B427" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Organização</t>
         </is>
       </c>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>Cabo HDMI</t>
+          <t>Etiquetadora Brother</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E427" s="7" t="inlineStr">
@@ -13232,22 +13232,22 @@
     <row r="428">
       <c r="A428" s="2" t="inlineStr">
         <is>
-          <t>Caixa 152</t>
+          <t>Caixa 129</t>
         </is>
       </c>
       <c r="B428" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>Carregadores de pilha</t>
+          <t>Parafusadeira a bateria</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Geral</t>
         </is>
       </c>
       <c r="E428" s="7" t="inlineStr">
@@ -13265,12 +13265,12 @@
       </c>
       <c r="B429" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>Caixa do iPhone da Amanda</t>
+          <t>Cabos de energia</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr">
@@ -13293,12 +13293,12 @@
       </c>
       <c r="B430" s="2" t="inlineStr">
         <is>
-          <t>Embalagens</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>Caixa Polar Loop</t>
+          <t>Película iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr">
@@ -13326,7 +13326,7 @@
       </c>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>Adaptadores de tomada</t>
+          <t>Cabo HDMI</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr">
@@ -13354,7 +13354,7 @@
       </c>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>Controle universal sem fio</t>
+          <t>Carregadores de pilha</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr">
@@ -13377,12 +13377,12 @@
       </c>
       <c r="B433" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>Carregador sem fio</t>
+          <t>Caixa do iPhone da Amanda</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr">
@@ -13405,12 +13405,12 @@
       </c>
       <c r="B434" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Embalagens</t>
         </is>
       </c>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>Thumb grip Steam Deck</t>
+          <t>Caixa Polar Loop</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr">
@@ -13433,12 +13433,12 @@
       </c>
       <c r="B435" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>Base de microfone (Rodrigo)</t>
+          <t>Adaptadores de tomada</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr">
@@ -13466,7 +13466,7 @@
       </c>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>Mouse Logitech MX Anywhere</t>
+          <t>Controle universal sem fio</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr">
@@ -13494,7 +13494,7 @@
       </c>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2025</t>
+          <t>Carregador sem fio</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr">
@@ -13517,12 +13517,12 @@
       </c>
       <c r="B438" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>Baterias CR2032</t>
+          <t>Thumb grip Steam Deck</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr">
@@ -13540,22 +13540,22 @@
     <row r="439">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de banho</t>
+          <t>Base de microfone (Rodrigo)</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E439" s="7" t="inlineStr">
@@ -13568,22 +13568,22 @@
     <row r="440">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>Caixa 301</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
         <is>
-          <t>Roupa de Cama e Banho</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>Toalhas de rosto</t>
+          <t>Mouse Logitech MX Anywhere</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E440" s="7" t="inlineStr">
@@ -13596,22 +13596,22 @@
     <row r="441">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá</t>
+          <t>Baterias CR2025</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E441" s="7" t="inlineStr">
@@ -13624,22 +13624,22 @@
     <row r="442">
       <c r="A442" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 152</t>
         </is>
       </c>
       <c r="B442" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>Cobertor Miolo Wine</t>
+          <t>Baterias CR2032</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr">
         <is>
-          <t>Suíte</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E442" s="7" t="inlineStr">
@@ -13652,17 +13652,17 @@
     <row r="443">
       <c r="A443" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B443" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>Dois jogos americanos</t>
+          <t>Toalhas de banho</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr">
@@ -13680,17 +13680,17 @@
     <row r="444">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>Caixa 302</t>
+          <t>Caixa 301</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
         <is>
-          <t>Têxtil</t>
+          <t>Roupa de Cama e Banho</t>
         </is>
       </c>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>Manta para sofá vermelha</t>
+          <t>Toalhas de rosto</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr">
@@ -13713,12 +13713,12 @@
       </c>
       <c r="B445" s="2" t="inlineStr">
         <is>
-          <t>Banheiro</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>Tapetes de banheiro</t>
+          <t>Manta para sofá</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr">
@@ -13741,12 +13741,12 @@
       </c>
       <c r="B446" s="2" t="inlineStr">
         <is>
-          <t>Mesa posta</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>Toalha de mesa</t>
+          <t>Cobertor Miolo Wine</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr">
@@ -13769,12 +13769,12 @@
       </c>
       <c r="B447" s="2" t="inlineStr">
         <is>
-          <t>Cama</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>Jogo de cama</t>
+          <t>Dois jogos americanos</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr">
@@ -13792,54 +13792,50 @@
     <row r="448">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>Caixa 399</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
         <is>
-          <t>Diversos</t>
+          <t>Têxtil</t>
         </is>
       </c>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>Itens da primeira noite</t>
+          <t>Manta para sofá vermelha</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr">
         <is>
-          <t>Geral</t>
-        </is>
-      </c>
-      <c r="E448" s="3" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="F448" s="2" t="inlineStr">
-        <is>
-          <t>Primeira noite</t>
-        </is>
-      </c>
+          <t>Suíte</t>
+        </is>
+      </c>
+      <c r="E448" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F448" s="2" t="n"/>
     </row>
     <row r="449">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Banheiro</t>
         </is>
       </c>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>Caixa de placa-mãe</t>
+          <t>Tapetes de banheiro</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E449" s="7" t="inlineStr">
@@ -13852,22 +13848,22 @@
     <row r="450">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Mesa posta</t>
         </is>
       </c>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>Jogos físicos</t>
+          <t>Toalha de mesa</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E450" s="7" t="inlineStr">
@@ -13880,22 +13876,22 @@
     <row r="451">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 302</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Cama</t>
         </is>
       </c>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>Blu-ray Star Wars</t>
+          <t>Jogo de cama</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Suíte</t>
         </is>
       </c>
       <c r="E451" s="7" t="inlineStr">
@@ -13908,30 +13904,34 @@
     <row r="452">
       <c r="A452" s="2" t="inlineStr">
         <is>
-          <t>Caixa 749</t>
+          <t>Caixa 399</t>
         </is>
       </c>
       <c r="B452" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Diversos</t>
         </is>
       </c>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>Caixa de GPU</t>
+          <t>Itens da primeira noite</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
-        </is>
-      </c>
-      <c r="E452" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F452" s="2" t="n"/>
+          <t>Geral</t>
+        </is>
+      </c>
+      <c r="E452" s="3" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="F452" s="2" t="inlineStr">
+        <is>
+          <t>Primeira noite</t>
+        </is>
+      </c>
     </row>
     <row r="453">
       <c r="A453" s="2" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>Caixa de CPU</t>
+          <t>Caixa de placa-mãe</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr">
@@ -13969,12 +13969,12 @@
       </c>
       <c r="B454" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>Acessórios e caixas de cubo mágico</t>
+          <t>Jogos físicos</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr">
@@ -13997,12 +13997,12 @@
       </c>
       <c r="B455" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>RX 480 (na caixa da RTX 4070)</t>
+          <t>Blu-ray Star Wars</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr">
@@ -14025,12 +14025,12 @@
       </c>
       <c r="B456" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>Bag de lente / objetiva</t>
+          <t>Caixa de GPU</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr">
@@ -14058,7 +14058,7 @@
       </c>
       <c r="C457" s="2" t="inlineStr">
         <is>
-          <t>Teclado Ducky TKL (case Pro X TKL)</t>
+          <t>Caixa de CPU</t>
         </is>
       </c>
       <c r="D457" s="2" t="inlineStr">
@@ -14081,12 +14081,12 @@
       </c>
       <c r="B458" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C458" s="2" t="inlineStr">
         <is>
-          <t>Hard case Ugreen</t>
+          <t>Acessórios e caixas de cubo mágico</t>
         </is>
       </c>
       <c r="D458" s="2" t="inlineStr">
@@ -14109,12 +14109,12 @@
       </c>
       <c r="B459" s="2" t="inlineStr">
         <is>
-          <t>Jogos e Mídia</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C459" s="2" t="inlineStr">
         <is>
-          <t>Caixa do Switch 2</t>
+          <t>RX 480 (na caixa da RTX 4070)</t>
         </is>
       </c>
       <c r="D459" s="2" t="inlineStr">
@@ -14137,12 +14137,12 @@
       </c>
       <c r="B460" s="2" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C460" s="2" t="inlineStr">
         <is>
-          <t>Teclado Corsair Strafe RGB ABNT</t>
+          <t>Bag de lente / objetiva</t>
         </is>
       </c>
       <c r="D460" s="2" t="inlineStr">
@@ -14160,17 +14160,17 @@
     <row r="461">
       <c r="A461" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B461" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C461" s="2" t="inlineStr">
         <is>
-          <t>Filtros de linha</t>
+          <t>Teclado Ducky TKL (case Pro X TKL)</t>
         </is>
       </c>
       <c r="D461" s="2" t="inlineStr">
@@ -14188,17 +14188,17 @@
     <row r="462">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C462" s="2" t="inlineStr">
         <is>
-          <t>Power cubes</t>
+          <t>Hard case Ugreen</t>
         </is>
       </c>
       <c r="D462" s="2" t="inlineStr">
@@ -14216,17 +14216,17 @@
     <row r="463">
       <c r="A463" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B463" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Jogos e Mídia</t>
         </is>
       </c>
       <c r="C463" s="2" t="inlineStr">
         <is>
-          <t>Fonte da soundbar</t>
+          <t>Caixa do Switch 2</t>
         </is>
       </c>
       <c r="D463" s="2" t="inlineStr">
@@ -14244,17 +14244,17 @@
     <row r="464">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1702</t>
+          <t>Caixa 749</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
         <is>
-          <t>Acessórios</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C464" s="2" t="inlineStr">
         <is>
-          <t>Suporte da soundbar</t>
+          <t>Teclado Corsair Strafe RGB ABNT</t>
         </is>
       </c>
       <c r="D464" s="2" t="inlineStr">
@@ -14272,22 +14272,22 @@
     <row r="465">
       <c r="A465" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B465" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C465" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Encanto</t>
+          <t>Filtros de linha</t>
         </is>
       </c>
       <c r="D465" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E465" s="7" t="inlineStr">
@@ -14300,22 +14300,22 @@
     <row r="466">
       <c r="A466" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B466" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C466" s="2" t="inlineStr">
         <is>
-          <t>Câmeras de LEGO</t>
+          <t>Power cubes</t>
         </is>
       </c>
       <c r="D466" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E466" s="7" t="inlineStr">
@@ -14328,22 +14328,22 @@
     <row r="467">
       <c r="A467" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B467" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C467" s="2" t="inlineStr">
         <is>
-          <t>Guarda-chuva de frevo</t>
+          <t>Fonte da soundbar</t>
         </is>
       </c>
       <c r="D467" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E467" s="7" t="inlineStr">
@@ -14356,22 +14356,22 @@
     <row r="468">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>Caixa 1948</t>
+          <t>Caixa 1702</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
         <is>
-          <t>Recordações</t>
+          <t>Acessórios</t>
         </is>
       </c>
       <c r="C468" s="2" t="inlineStr">
         <is>
-          <t>Medalhas</t>
+          <t>Suporte da soundbar</t>
         </is>
       </c>
       <c r="D468" s="2" t="inlineStr">
         <is>
-          <t>Quarto do Bento</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E468" s="7" t="inlineStr">
@@ -14394,7 +14394,7 @@
       </c>
       <c r="C469" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco Kong</t>
+          <t>BrickHeadz Encanto</t>
         </is>
       </c>
       <c r="D469" s="2" t="inlineStr">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="C470" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco primo do Tupac</t>
+          <t>Câmeras de LEGO</t>
         </is>
       </c>
       <c r="D470" s="2" t="inlineStr">
@@ -14445,12 +14445,12 @@
       </c>
       <c r="B471" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>LEGO macaco de boné no carrinho</t>
+          <t>Guarda-chuva de frevo</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr">
@@ -14473,12 +14473,12 @@
       </c>
       <c r="B472" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Recordações</t>
         </is>
       </c>
       <c r="C472" s="2" t="inlineStr">
         <is>
-          <t>LEGO topeira estranha</t>
+          <t>Medalhas</t>
         </is>
       </c>
       <c r="D472" s="2" t="inlineStr">
@@ -14506,7 +14506,7 @@
       </c>
       <c r="C473" s="2" t="inlineStr">
         <is>
-          <t>Kirby Carmen Miranda</t>
+          <t>LEGO macaco Kong</t>
         </is>
       </c>
       <c r="D473" s="2" t="inlineStr">
@@ -14534,7 +14534,7 @@
       </c>
       <c r="C474" s="2" t="inlineStr">
         <is>
-          <t>Funko Satoru Gojo</t>
+          <t>LEGO macaco primo do Tupac</t>
         </is>
       </c>
       <c r="D474" s="2" t="inlineStr">
@@ -14562,7 +14562,7 @@
       </c>
       <c r="C475" s="2" t="inlineStr">
         <is>
-          <t>Bonecos de Jujutsu Kaisen</t>
+          <t>LEGO macaco de boné no carrinho</t>
         </is>
       </c>
       <c r="D475" s="2" t="inlineStr">
@@ -14590,7 +14590,7 @@
       </c>
       <c r="C476" s="2" t="inlineStr">
         <is>
-          <t>Mario Kart vestido de rata</t>
+          <t>LEGO topeira estranha</t>
         </is>
       </c>
       <c r="D476" s="2" t="inlineStr">
@@ -14618,7 +14618,7 @@
       </c>
       <c r="C477" s="2" t="inlineStr">
         <is>
-          <t>Bonecos do Bob Esponja</t>
+          <t>Kirby Carmen Miranda</t>
         </is>
       </c>
       <c r="D477" s="2" t="inlineStr">
@@ -14646,7 +14646,7 @@
       </c>
       <c r="C478" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 1</t>
+          <t>Funko Satoru Gojo</t>
         </is>
       </c>
       <c r="D478" s="2" t="inlineStr">
@@ -14674,7 +14674,7 @@
       </c>
       <c r="C479" s="2" t="inlineStr">
         <is>
-          <t>Boneco Harry Potter japonês 2</t>
+          <t>Bonecos de Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="D479" s="2" t="inlineStr">
@@ -14702,7 +14702,7 @@
       </c>
       <c r="C480" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Batman (Feira da Fruta)</t>
+          <t>Mario Kart vestido de rata</t>
         </is>
       </c>
       <c r="D480" s="2" t="inlineStr">
@@ -14720,22 +14720,22 @@
     <row r="481">
       <c r="A481" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B481" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C481" s="2" t="inlineStr">
         <is>
-          <t>Bolsas de cabos</t>
+          <t>Bonecos do Bob Esponja</t>
         </is>
       </c>
       <c r="D481" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E481" s="7" t="inlineStr">
@@ -14748,22 +14748,22 @@
     <row r="482">
       <c r="A482" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B482" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C482" s="2" t="inlineStr">
         <is>
-          <t>Cabos soltos</t>
+          <t>Boneco Harry Potter japonês 1</t>
         </is>
       </c>
       <c r="D482" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E482" s="7" t="inlineStr">
@@ -14776,22 +14776,22 @@
     <row r="483">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C483" s="2" t="inlineStr">
         <is>
-          <t>Power banks</t>
+          <t>Boneco Harry Potter japonês 2</t>
         </is>
       </c>
       <c r="D483" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E483" s="7" t="inlineStr">
@@ -14804,22 +14804,22 @@
     <row r="484">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>Caixa 3501</t>
+          <t>Caixa 1948</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Brinquedos e Colecionáveis</t>
         </is>
       </c>
       <c r="C484" s="2" t="inlineStr">
         <is>
-          <t>Mesas digitalizadoras</t>
+          <t>BrickHeadz Batman (Feira da Fruta)</t>
         </is>
       </c>
       <c r="D484" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Quarto do Bento</t>
         </is>
       </c>
       <c r="E484" s="7" t="inlineStr">
@@ -14832,22 +14832,22 @@
     <row r="485">
       <c r="A485" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B485" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C485" s="2" t="inlineStr">
         <is>
-          <t>Furadeira</t>
+          <t>Bolsas de cabos</t>
         </is>
       </c>
       <c r="D485" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E485" s="7" t="inlineStr">
@@ -14860,22 +14860,22 @@
     <row r="486">
       <c r="A486" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B486" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C486" s="2" t="inlineStr">
         <is>
-          <t>Parafusadeira</t>
+          <t>Cabos soltos</t>
         </is>
       </c>
       <c r="D486" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E486" s="7" t="inlineStr">
@@ -14888,22 +14888,22 @@
     <row r="487">
       <c r="A487" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B487" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C487" s="2" t="inlineStr">
         <is>
-          <t>Acessórios de aspirador</t>
+          <t>Power banks</t>
         </is>
       </c>
       <c r="D487" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E487" s="7" t="inlineStr">
@@ -14916,22 +14916,22 @@
     <row r="488">
       <c r="A488" s="2" t="inlineStr">
         <is>
-          <t>Caixa 9501</t>
+          <t>Caixa 3501</t>
         </is>
       </c>
       <c r="B488" s="2" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C488" s="2" t="inlineStr">
         <is>
-          <t>Ralo click</t>
+          <t>Mesas digitalizadoras</t>
         </is>
       </c>
       <c r="D488" s="2" t="inlineStr">
         <is>
-          <t>Lavanderia</t>
+          <t>Escritório</t>
         </is>
       </c>
       <c r="E488" s="7" t="inlineStr">
@@ -14954,7 +14954,7 @@
       </c>
       <c r="C489" s="2" t="inlineStr">
         <is>
-          <t>Escova de limpeza elétrica</t>
+          <t>Furadeira</t>
         </is>
       </c>
       <c r="D489" s="2" t="inlineStr">
@@ -14972,22 +14972,22 @@
     <row r="490">
       <c r="A490" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B490" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C490" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Aragorn</t>
+          <t>Parafusadeira</t>
         </is>
       </c>
       <c r="D490" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E490" s="7" t="inlineStr">
@@ -15000,22 +15000,22 @@
     <row r="491">
       <c r="A491" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B491" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C491" s="2" t="inlineStr">
         <is>
-          <t>BrickHeadz Arwen Undómiel</t>
+          <t>Acessórios de aspirador</t>
         </is>
       </c>
       <c r="D491" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E491" s="7" t="inlineStr">
@@ -15028,22 +15028,22 @@
     <row r="492">
       <c r="A492" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B492" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C492" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Slash</t>
+          <t>Ralo click</t>
         </is>
       </c>
       <c r="D492" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E492" s="7" t="inlineStr">
@@ -15056,22 +15056,22 @@
     <row r="493">
       <c r="A493" s="2" t="inlineStr">
         <is>
-          <t>Caixa 29501</t>
+          <t>Caixa 9501</t>
         </is>
       </c>
       <c r="B493" s="2" t="inlineStr">
         <is>
-          <t>Brinquedos e Colecionáveis</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C493" s="2" t="inlineStr">
         <is>
-          <t>Funko Pop Axl Rose</t>
+          <t>Escova de limpeza elétrica</t>
         </is>
       </c>
       <c r="D493" s="2" t="inlineStr">
         <is>
-          <t>Escritório</t>
+          <t>Lavanderia</t>
         </is>
       </c>
       <c r="E493" s="7" t="inlineStr">
@@ -15094,7 +15094,7 @@
       </c>
       <c r="C494" s="2" t="inlineStr">
         <is>
-          <t>Hot Wheels – Naves Star Wars</t>
+          <t>BrickHeadz Aragorn</t>
         </is>
       </c>
       <c r="D494" s="2" t="inlineStr">
@@ -15122,7 +15122,7 @@
       </c>
       <c r="C495" s="2" t="inlineStr">
         <is>
-          <t>GooJitZu do Sonic</t>
+          <t>BrickHeadz Arwen Undómiel</t>
         </is>
       </c>
       <c r="D495" s="2" t="inlineStr">
@@ -15150,20 +15150,132 @@
       </c>
       <c r="C496" s="2" t="inlineStr">
         <is>
+          <t>Funko Pop Slash</t>
+        </is>
+      </c>
+      <c r="D496" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E496" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F496" s="2" t="n"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B497" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C497" s="2" t="inlineStr">
+        <is>
+          <t>Funko Pop Axl Rose</t>
+        </is>
+      </c>
+      <c r="D497" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E497" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F497" s="2" t="n"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B498" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C498" s="2" t="inlineStr">
+        <is>
+          <t>Hot Wheels – Naves Star Wars</t>
+        </is>
+      </c>
+      <c r="D498" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E498" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F498" s="2" t="n"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B499" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C499" s="2" t="inlineStr">
+        <is>
+          <t>GooJitZu do Sonic</t>
+        </is>
+      </c>
+      <c r="D499" s="2" t="inlineStr">
+        <is>
+          <t>Escritório</t>
+        </is>
+      </c>
+      <c r="E499" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F499" s="2" t="n"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="2" t="inlineStr">
+        <is>
+          <t>Caixa 29501</t>
+        </is>
+      </c>
+      <c r="B500" s="2" t="inlineStr">
+        <is>
+          <t>Brinquedos e Colecionáveis</t>
+        </is>
+      </c>
+      <c r="C500" s="2" t="inlineStr">
+        <is>
           <t>Cubos mágicos</t>
         </is>
       </c>
-      <c r="D496" s="2" t="inlineStr">
+      <c r="D500" s="2" t="inlineStr">
         <is>
           <t>Escritório</t>
         </is>
       </c>
-      <c r="E496" s="7" t="inlineStr">
-        <is>
-          <t>Média</t>
-        </is>
-      </c>
-      <c r="F496" s="2" t="n"/>
+      <c r="E500" s="7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="F500" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15202,7 +15314,7 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4">
@@ -15232,7 +15344,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8">

</xml_diff>